<commit_message>
StatementXLS: currency list import was implemented. Test set was updated
</commit_message>
<xml_diff>
--- a/tests/test_data/kit.xlsx
+++ b/tests/test_data/kit.xlsx
@@ -737,7 +737,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="110">
+  <cellXfs count="106">
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -854,10 +854,6 @@
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="167" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1030,10 +1026,6 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="167" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1044,10 +1036,6 @@
     </xf>
     <xf numFmtId="171" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="5" fillId="3" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="11" fillId="3" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -1127,10 +1115,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1351,9 +1335,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>204120</xdr:colOff>
+      <xdr:colOff>203760</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>21240</xdr:rowOff>
+      <xdr:rowOff>20880</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1367,7 +1351,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="2742840" cy="691560"/>
+          <a:ext cx="2742480" cy="691200"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1389,11 +1373,11 @@
   </sheetPr>
   <dimension ref="A1:AC52"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A31" colorId="64" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D53" activeCellId="0" sqref="D53"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J16" activeCellId="0" sqref="J16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="1" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="1" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="14.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="13.89"/>
@@ -1625,9 +1609,15 @@
       <c r="D13" s="20"/>
       <c r="E13" s="20"/>
       <c r="F13" s="20"/>
-      <c r="G13" s="21"/>
-      <c r="H13" s="21"/>
-      <c r="I13" s="21"/>
+      <c r="G13" s="21" t="n">
+        <v>55.85</v>
+      </c>
+      <c r="H13" s="21" t="n">
+        <v>1</v>
+      </c>
+      <c r="I13" s="21" t="n">
+        <v>120</v>
+      </c>
       <c r="J13" s="22"/>
       <c r="K13" s="22"/>
       <c r="L13" s="22"/>
@@ -1642,9 +1632,15 @@
       <c r="D14" s="20"/>
       <c r="E14" s="20"/>
       <c r="F14" s="20"/>
-      <c r="G14" s="21"/>
-      <c r="H14" s="21"/>
-      <c r="I14" s="21"/>
+      <c r="G14" s="21" t="n">
+        <v>0.12</v>
+      </c>
+      <c r="H14" s="21" t="n">
+        <v>1</v>
+      </c>
+      <c r="I14" s="21" t="n">
+        <v>80</v>
+      </c>
       <c r="J14" s="22"/>
       <c r="K14" s="22"/>
       <c r="L14" s="22"/>
@@ -1659,9 +1655,15 @@
       <c r="D15" s="23"/>
       <c r="E15" s="23"/>
       <c r="F15" s="23"/>
-      <c r="G15" s="21"/>
-      <c r="H15" s="21"/>
-      <c r="I15" s="21"/>
+      <c r="G15" s="21" t="n">
+        <v>0.12</v>
+      </c>
+      <c r="H15" s="21" t="n">
+        <v>1</v>
+      </c>
+      <c r="I15" s="21" t="n">
+        <v>80</v>
+      </c>
       <c r="J15" s="22"/>
       <c r="K15" s="22"/>
       <c r="L15" s="22"/>
@@ -1676,9 +1678,15 @@
       <c r="D16" s="23"/>
       <c r="E16" s="23"/>
       <c r="F16" s="23"/>
-      <c r="G16" s="21"/>
-      <c r="H16" s="21"/>
-      <c r="I16" s="21"/>
+      <c r="G16" s="21" t="n">
+        <v>55.97</v>
+      </c>
+      <c r="H16" s="21" t="n">
+        <v>0</v>
+      </c>
+      <c r="I16" s="21" t="n">
+        <v>0</v>
+      </c>
       <c r="J16" s="22"/>
       <c r="K16" s="22"/>
       <c r="L16" s="22"/>
@@ -1693,9 +1701,15 @@
       <c r="D17" s="20"/>
       <c r="E17" s="20"/>
       <c r="F17" s="20"/>
-      <c r="G17" s="21"/>
-      <c r="H17" s="21"/>
-      <c r="I17" s="21"/>
+      <c r="G17" s="21" t="n">
+        <v>55.97</v>
+      </c>
+      <c r="H17" s="21" t="n">
+        <v>2</v>
+      </c>
+      <c r="I17" s="21" t="n">
+        <v>200</v>
+      </c>
       <c r="J17" s="22"/>
       <c r="K17" s="22"/>
       <c r="L17" s="22"/>
@@ -1710,9 +1724,15 @@
       <c r="D18" s="23"/>
       <c r="E18" s="23"/>
       <c r="F18" s="23"/>
-      <c r="G18" s="21"/>
-      <c r="H18" s="21"/>
-      <c r="I18" s="21"/>
+      <c r="G18" s="21" t="n">
+        <v>55.97</v>
+      </c>
+      <c r="H18" s="21" t="n">
+        <v>2</v>
+      </c>
+      <c r="I18" s="21" t="n">
+        <v>200</v>
+      </c>
       <c r="J18" s="22"/>
       <c r="K18" s="22"/>
       <c r="L18" s="22"/>
@@ -1727,9 +1747,15 @@
       <c r="D19" s="23"/>
       <c r="E19" s="23"/>
       <c r="F19" s="23"/>
-      <c r="G19" s="21"/>
-      <c r="H19" s="21"/>
-      <c r="I19" s="21"/>
+      <c r="G19" s="21" t="n">
+        <v>55.97</v>
+      </c>
+      <c r="H19" s="21" t="n">
+        <v>2</v>
+      </c>
+      <c r="I19" s="21" t="n">
+        <v>200</v>
+      </c>
       <c r="J19" s="22"/>
       <c r="K19" s="22"/>
       <c r="L19" s="22"/>
@@ -1744,9 +1770,15 @@
       <c r="D20" s="23"/>
       <c r="E20" s="23"/>
       <c r="F20" s="23"/>
-      <c r="G20" s="21"/>
-      <c r="H20" s="21"/>
-      <c r="I20" s="21"/>
+      <c r="G20" s="21" t="n">
+        <v>1</v>
+      </c>
+      <c r="H20" s="21" t="n">
+        <v>2</v>
+      </c>
+      <c r="I20" s="21" t="n">
+        <v>200</v>
+      </c>
       <c r="J20" s="22"/>
       <c r="K20" s="22"/>
       <c r="L20" s="22"/>
@@ -1762,7 +1794,9 @@
       <c r="E21" s="23"/>
       <c r="F21" s="23"/>
       <c r="G21" s="21"/>
-      <c r="H21" s="21"/>
+      <c r="H21" s="21" t="n">
+        <v>70</v>
+      </c>
       <c r="I21" s="21"/>
       <c r="J21" s="22"/>
       <c r="K21" s="22"/>
@@ -1783,7 +1817,7 @@
       <c r="K22" s="22"/>
       <c r="L22" s="22"/>
     </row>
-    <row r="23" s="29" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="23" s="1" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="26"/>
       <c r="B23" s="26"/>
       <c r="C23" s="26"/>
@@ -1799,197 +1833,197 @@
       <c r="M23" s="28"/>
     </row>
     <row r="24" s="16" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A24" s="30" t="s">
+      <c r="A24" s="29" t="s">
         <v>25</v>
       </c>
-      <c r="B24" s="30"/>
-      <c r="C24" s="30"/>
-      <c r="D24" s="30"/>
-      <c r="E24" s="30"/>
-      <c r="F24" s="30"/>
-      <c r="G24" s="30"/>
-      <c r="H24" s="30"/>
-      <c r="I24" s="30"/>
-      <c r="J24" s="30"/>
-      <c r="K24" s="30"/>
-      <c r="L24" s="30"/>
-      <c r="M24" s="30"/>
-    </row>
-    <row r="25" s="35" customFormat="true" ht="56.7" hidden="false" customHeight="true" outlineLevel="1" collapsed="false">
-      <c r="A25" s="31" t="s">
+      <c r="B24" s="29"/>
+      <c r="C24" s="29"/>
+      <c r="D24" s="29"/>
+      <c r="E24" s="29"/>
+      <c r="F24" s="29"/>
+      <c r="G24" s="29"/>
+      <c r="H24" s="29"/>
+      <c r="I24" s="29"/>
+      <c r="J24" s="29"/>
+      <c r="K24" s="29"/>
+      <c r="L24" s="29"/>
+      <c r="M24" s="29"/>
+    </row>
+    <row r="25" s="34" customFormat="true" ht="56.7" hidden="false" customHeight="true" outlineLevel="1" collapsed="false">
+      <c r="A25" s="30" t="s">
         <v>26</v>
       </c>
-      <c r="B25" s="31"/>
-      <c r="C25" s="31"/>
-      <c r="D25" s="32" t="s">
+      <c r="B25" s="30"/>
+      <c r="C25" s="30"/>
+      <c r="D25" s="31" t="s">
         <v>27</v>
       </c>
-      <c r="E25" s="32" t="s">
+      <c r="E25" s="31" t="s">
         <v>28</v>
       </c>
-      <c r="F25" s="32" t="s">
+      <c r="F25" s="31" t="s">
         <v>29</v>
       </c>
-      <c r="G25" s="33" t="s">
+      <c r="G25" s="32" t="s">
         <v>30</v>
       </c>
-      <c r="H25" s="33" t="s">
+      <c r="H25" s="32" t="s">
         <v>31</v>
       </c>
-      <c r="I25" s="32" t="s">
+      <c r="I25" s="31" t="s">
         <v>32</v>
       </c>
-      <c r="J25" s="33" t="s">
+      <c r="J25" s="32" t="s">
         <v>33</v>
       </c>
-      <c r="K25" s="33" t="s">
+      <c r="K25" s="32" t="s">
         <v>34</v>
       </c>
-      <c r="L25" s="32" t="s">
+      <c r="L25" s="31" t="s">
         <v>35</v>
       </c>
-      <c r="M25" s="34" t="s">
+      <c r="M25" s="33" t="s">
         <v>36</v>
       </c>
-      <c r="N25" s="32" t="s">
+      <c r="N25" s="31" t="s">
         <v>37</v>
       </c>
-      <c r="O25" s="34" t="s">
+      <c r="O25" s="33" t="s">
         <v>38</v>
       </c>
-      <c r="P25" s="34" t="s">
+      <c r="P25" s="33" t="s">
         <v>39</v>
       </c>
-      <c r="Q25" s="34" t="s">
+      <c r="Q25" s="33" t="s">
         <v>40</v>
       </c>
-      <c r="R25" s="34" t="s">
+      <c r="R25" s="33" t="s">
         <v>41</v>
       </c>
-      <c r="S25" s="32" t="s">
+      <c r="S25" s="31" t="s">
         <v>42</v>
       </c>
-      <c r="T25" s="34" t="s">
+      <c r="T25" s="33" t="s">
         <v>43</v>
       </c>
-      <c r="U25" s="31" t="s">
+      <c r="U25" s="30" t="s">
         <v>44</v>
       </c>
-      <c r="V25" s="31"/>
-      <c r="W25" s="32" t="s">
+      <c r="V25" s="30"/>
+      <c r="W25" s="31" t="s">
         <v>45</v>
       </c>
-      <c r="X25" s="32" t="s">
+      <c r="X25" s="31" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="26" s="35" customFormat="true" ht="15.3" hidden="false" customHeight="true" outlineLevel="1" collapsed="false">
-      <c r="A26" s="36" t="s">
+    <row r="26" s="34" customFormat="true" ht="15.3" hidden="false" customHeight="true" outlineLevel="1" collapsed="false">
+      <c r="A26" s="35" t="s">
         <v>47</v>
       </c>
-      <c r="B26" s="36"/>
-      <c r="C26" s="36"/>
-      <c r="D26" s="37"/>
-      <c r="E26" s="37"/>
-      <c r="F26" s="38"/>
-      <c r="G26" s="38"/>
-      <c r="H26" s="38"/>
-      <c r="I26" s="38"/>
-      <c r="J26" s="38"/>
-      <c r="K26" s="38"/>
-      <c r="L26" s="38"/>
-      <c r="M26" s="39"/>
-      <c r="N26" s="39"/>
-      <c r="O26" s="39"/>
-      <c r="P26" s="40"/>
-      <c r="Q26" s="39"/>
-      <c r="R26" s="41"/>
-      <c r="S26" s="41"/>
-      <c r="T26" s="41"/>
-      <c r="U26" s="42"/>
-      <c r="V26" s="42"/>
-      <c r="W26" s="43"/>
-      <c r="X26" s="44"/>
-      <c r="Y26" s="45"/>
-      <c r="Z26" s="46"/>
-      <c r="AA26" s="45"/>
-      <c r="AB26" s="45"/>
-      <c r="AC26" s="46"/>
-    </row>
-    <row r="27" s="51" customFormat="true" ht="17.1" hidden="false" customHeight="true" outlineLevel="1" collapsed="false">
-      <c r="A27" s="47"/>
-      <c r="B27" s="48"/>
-      <c r="C27" s="48"/>
-      <c r="D27" s="49"/>
-      <c r="E27" s="49"/>
-      <c r="F27" s="49"/>
-      <c r="G27" s="49"/>
-      <c r="H27" s="49"/>
-      <c r="I27" s="49"/>
-      <c r="J27" s="49"/>
-      <c r="K27" s="49"/>
-      <c r="L27" s="49"/>
-      <c r="M27" s="49"/>
-      <c r="N27" s="49"/>
-      <c r="O27" s="49"/>
-      <c r="P27" s="48"/>
-      <c r="Q27" s="49"/>
-      <c r="R27" s="49"/>
-      <c r="S27" s="49"/>
-      <c r="T27" s="49"/>
-      <c r="U27" s="50"/>
-      <c r="V27" s="50"/>
-      <c r="W27" s="49"/>
-      <c r="X27" s="48"/>
+      <c r="B26" s="35"/>
+      <c r="C26" s="35"/>
+      <c r="D26" s="36"/>
+      <c r="E26" s="36"/>
+      <c r="F26" s="37"/>
+      <c r="G26" s="37"/>
+      <c r="H26" s="37"/>
+      <c r="I26" s="37"/>
+      <c r="J26" s="37"/>
+      <c r="K26" s="37"/>
+      <c r="L26" s="37"/>
+      <c r="M26" s="38"/>
+      <c r="N26" s="38"/>
+      <c r="O26" s="38"/>
+      <c r="P26" s="39"/>
+      <c r="Q26" s="38"/>
+      <c r="R26" s="40"/>
+      <c r="S26" s="40"/>
+      <c r="T26" s="40"/>
+      <c r="U26" s="41"/>
+      <c r="V26" s="41"/>
+      <c r="W26" s="42"/>
+      <c r="X26" s="43"/>
+      <c r="Y26" s="44"/>
+      <c r="Z26" s="45"/>
+      <c r="AA26" s="44"/>
+      <c r="AB26" s="44"/>
+      <c r="AC26" s="45"/>
+    </row>
+    <row r="27" s="50" customFormat="true" ht="17.1" hidden="false" customHeight="true" outlineLevel="1" collapsed="false">
+      <c r="A27" s="46"/>
+      <c r="B27" s="47"/>
+      <c r="C27" s="47"/>
+      <c r="D27" s="48"/>
+      <c r="E27" s="48"/>
+      <c r="F27" s="48"/>
+      <c r="G27" s="48"/>
+      <c r="H27" s="48"/>
+      <c r="I27" s="48"/>
+      <c r="J27" s="48"/>
+      <c r="K27" s="48"/>
+      <c r="L27" s="48"/>
+      <c r="M27" s="48"/>
+      <c r="N27" s="48"/>
+      <c r="O27" s="48"/>
+      <c r="P27" s="47"/>
+      <c r="Q27" s="48"/>
+      <c r="R27" s="48"/>
+      <c r="S27" s="48"/>
+      <c r="T27" s="48"/>
+      <c r="U27" s="49"/>
+      <c r="V27" s="49"/>
+      <c r="W27" s="48"/>
+      <c r="X27" s="47"/>
     </row>
     <row r="28" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="30" t="s">
+      <c r="A28" s="29" t="s">
         <v>48</v>
       </c>
-      <c r="B28" s="52"/>
-      <c r="C28" s="52"/>
-      <c r="D28" s="52"/>
-      <c r="E28" s="52"/>
-      <c r="F28" s="52"/>
-      <c r="G28" s="52"/>
-      <c r="H28" s="52"/>
-      <c r="I28" s="52"/>
-      <c r="J28" s="52"/>
-      <c r="K28" s="52"/>
-      <c r="L28" s="52"/>
-      <c r="M28" s="52"/>
-      <c r="N28" s="52"/>
-      <c r="O28" s="52"/>
-      <c r="P28" s="52"/>
-      <c r="Q28" s="52"/>
-      <c r="R28" s="52"/>
-      <c r="S28" s="52"/>
-      <c r="T28" s="52"/>
-      <c r="U28" s="52"/>
-      <c r="V28" s="52"/>
-      <c r="W28" s="52"/>
+      <c r="B28" s="51"/>
+      <c r="C28" s="51"/>
+      <c r="D28" s="51"/>
+      <c r="E28" s="51"/>
+      <c r="F28" s="51"/>
+      <c r="G28" s="51"/>
+      <c r="H28" s="51"/>
+      <c r="I28" s="51"/>
+      <c r="J28" s="51"/>
+      <c r="K28" s="51"/>
+      <c r="L28" s="51"/>
+      <c r="M28" s="51"/>
+      <c r="N28" s="51"/>
+      <c r="O28" s="51"/>
+      <c r="P28" s="51"/>
+      <c r="Q28" s="51"/>
+      <c r="R28" s="51"/>
+      <c r="S28" s="51"/>
+      <c r="T28" s="51"/>
+      <c r="U28" s="51"/>
+      <c r="V28" s="51"/>
+      <c r="W28" s="51"/>
     </row>
     <row r="29" customFormat="false" ht="15.3" hidden="false" customHeight="true" outlineLevel="1" collapsed="false">
-      <c r="A29" s="53" t="s">
+      <c r="A29" s="52" t="s">
         <v>49</v>
       </c>
-      <c r="B29" s="53"/>
-      <c r="C29" s="53"/>
-      <c r="D29" s="53"/>
-      <c r="E29" s="53" t="s">
+      <c r="B29" s="52"/>
+      <c r="C29" s="52"/>
+      <c r="D29" s="52"/>
+      <c r="E29" s="52" t="s">
         <v>50</v>
       </c>
-      <c r="F29" s="53"/>
-      <c r="G29" s="53"/>
-      <c r="H29" s="53"/>
-      <c r="I29" s="53" t="s">
+      <c r="F29" s="52"/>
+      <c r="G29" s="52"/>
+      <c r="H29" s="52"/>
+      <c r="I29" s="52" t="s">
         <v>51</v>
       </c>
-      <c r="J29" s="53"/>
-      <c r="K29" s="53"/>
-      <c r="L29" s="53"/>
-      <c r="M29" s="54"/>
-      <c r="N29" s="55"/>
+      <c r="J29" s="52"/>
+      <c r="K29" s="52"/>
+      <c r="L29" s="52"/>
+      <c r="M29" s="53"/>
+      <c r="N29" s="54"/>
       <c r="O29" s="22"/>
       <c r="P29" s="22"/>
       <c r="Q29" s="22"/>
@@ -1997,32 +2031,32 @@
       <c r="S29" s="22"/>
     </row>
     <row r="30" customFormat="false" ht="29.7" hidden="false" customHeight="true" outlineLevel="1" collapsed="false">
-      <c r="A30" s="56" t="s">
+      <c r="A30" s="55" t="s">
         <v>52</v>
       </c>
-      <c r="B30" s="56"/>
-      <c r="C30" s="56" t="s">
+      <c r="B30" s="55"/>
+      <c r="C30" s="55" t="s">
         <v>53</v>
       </c>
-      <c r="D30" s="56"/>
-      <c r="E30" s="56" t="s">
+      <c r="D30" s="55"/>
+      <c r="E30" s="55" t="s">
         <v>52</v>
       </c>
-      <c r="F30" s="56"/>
-      <c r="G30" s="56" t="s">
+      <c r="F30" s="55"/>
+      <c r="G30" s="55" t="s">
         <v>54</v>
       </c>
-      <c r="H30" s="56"/>
-      <c r="I30" s="56" t="s">
+      <c r="H30" s="55"/>
+      <c r="I30" s="55" t="s">
         <v>52</v>
       </c>
-      <c r="J30" s="56"/>
-      <c r="K30" s="56" t="s">
+      <c r="J30" s="55"/>
+      <c r="K30" s="55" t="s">
         <v>54</v>
       </c>
-      <c r="L30" s="56"/>
-      <c r="M30" s="54"/>
-      <c r="N30" s="55"/>
+      <c r="L30" s="55"/>
+      <c r="M30" s="53"/>
+      <c r="N30" s="54"/>
       <c r="O30" s="22"/>
       <c r="P30" s="22"/>
       <c r="Q30" s="22"/>
@@ -2030,171 +2064,171 @@
       <c r="S30" s="22"/>
     </row>
     <row r="31" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="1" collapsed="false">
-      <c r="A31" s="57" t="s">
+      <c r="A31" s="56" t="s">
         <v>47</v>
       </c>
-      <c r="B31" s="57"/>
-      <c r="C31" s="58"/>
-      <c r="D31" s="58"/>
-      <c r="E31" s="58"/>
-      <c r="F31" s="58"/>
-      <c r="G31" s="58"/>
-      <c r="H31" s="58"/>
-      <c r="I31" s="58"/>
-      <c r="J31" s="58"/>
-      <c r="K31" s="58"/>
-      <c r="L31" s="58"/>
-      <c r="M31" s="54"/>
-      <c r="N31" s="55"/>
+      <c r="B31" s="56"/>
+      <c r="C31" s="57"/>
+      <c r="D31" s="57"/>
+      <c r="E31" s="57"/>
+      <c r="F31" s="57"/>
+      <c r="G31" s="57"/>
+      <c r="H31" s="57"/>
+      <c r="I31" s="57"/>
+      <c r="J31" s="57"/>
+      <c r="K31" s="57"/>
+      <c r="L31" s="57"/>
+      <c r="M31" s="53"/>
+      <c r="N31" s="54"/>
       <c r="O31" s="22"/>
       <c r="P31" s="22"/>
       <c r="Q31" s="22"/>
       <c r="R31" s="22"/>
       <c r="S31" s="22"/>
     </row>
-    <row r="32" s="51" customFormat="true" ht="16.5" hidden="false" customHeight="true" outlineLevel="1" collapsed="false">
-      <c r="A32" s="48"/>
-      <c r="B32" s="48"/>
-      <c r="C32" s="48"/>
-      <c r="D32" s="48"/>
-      <c r="E32" s="48"/>
-      <c r="F32" s="49"/>
-      <c r="G32" s="49"/>
-      <c r="H32" s="49"/>
-      <c r="I32" s="49"/>
-      <c r="J32" s="49"/>
-      <c r="K32" s="49"/>
-      <c r="L32" s="49"/>
+    <row r="32" s="50" customFormat="true" ht="16.5" hidden="false" customHeight="true" outlineLevel="1" collapsed="false">
+      <c r="A32" s="47"/>
+      <c r="B32" s="47"/>
+      <c r="C32" s="47"/>
+      <c r="D32" s="47"/>
+      <c r="E32" s="47"/>
+      <c r="F32" s="48"/>
+      <c r="G32" s="48"/>
+      <c r="H32" s="48"/>
+      <c r="I32" s="48"/>
+      <c r="J32" s="48"/>
+      <c r="K32" s="48"/>
+      <c r="L32" s="48"/>
       <c r="M32" s="28"/>
       <c r="N32" s="28"/>
-      <c r="O32" s="59"/>
+      <c r="O32" s="58"/>
       <c r="P32" s="28"/>
       <c r="Q32" s="28"/>
       <c r="R32" s="28"/>
       <c r="S32" s="28"/>
-      <c r="T32" s="60"/>
-      <c r="U32" s="60"/>
+      <c r="T32" s="59"/>
+      <c r="U32" s="59"/>
       <c r="V32" s="28"/>
-      <c r="W32" s="59"/>
+      <c r="W32" s="58"/>
     </row>
     <row r="33" s="16" customFormat="true" ht="17.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A33" s="30" t="s">
+      <c r="A33" s="29" t="s">
         <v>55</v>
       </c>
-      <c r="B33" s="30"/>
-      <c r="C33" s="30"/>
-      <c r="D33" s="30"/>
-      <c r="E33" s="30"/>
-      <c r="F33" s="30"/>
-      <c r="G33" s="30"/>
-      <c r="H33" s="30"/>
-      <c r="I33" s="30"/>
-      <c r="J33" s="30"/>
-      <c r="K33" s="30"/>
-      <c r="L33" s="30"/>
-      <c r="M33" s="30"/>
-    </row>
-    <row r="34" s="64" customFormat="true" ht="15.3" hidden="false" customHeight="true" outlineLevel="1" collapsed="false">
-      <c r="A34" s="31" t="s">
+      <c r="B33" s="29"/>
+      <c r="C33" s="29"/>
+      <c r="D33" s="29"/>
+      <c r="E33" s="29"/>
+      <c r="F33" s="29"/>
+      <c r="G33" s="29"/>
+      <c r="H33" s="29"/>
+      <c r="I33" s="29"/>
+      <c r="J33" s="29"/>
+      <c r="K33" s="29"/>
+      <c r="L33" s="29"/>
+      <c r="M33" s="29"/>
+    </row>
+    <row r="34" s="63" customFormat="true" ht="15.3" hidden="false" customHeight="true" outlineLevel="1" collapsed="false">
+      <c r="A34" s="30" t="s">
         <v>56</v>
       </c>
-      <c r="B34" s="61" t="s">
+      <c r="B34" s="60" t="s">
         <v>57</v>
       </c>
-      <c r="C34" s="61"/>
-      <c r="D34" s="61"/>
-      <c r="E34" s="61"/>
-      <c r="F34" s="61"/>
-      <c r="G34" s="31" t="s">
+      <c r="C34" s="60"/>
+      <c r="D34" s="60"/>
+      <c r="E34" s="60"/>
+      <c r="F34" s="60"/>
+      <c r="G34" s="30" t="s">
         <v>58</v>
       </c>
-      <c r="H34" s="31" t="s">
+      <c r="H34" s="30" t="s">
         <v>59</v>
       </c>
-      <c r="I34" s="31" t="s">
+      <c r="I34" s="30" t="s">
         <v>60</v>
       </c>
-      <c r="J34" s="31"/>
-      <c r="K34" s="31"/>
-      <c r="L34" s="31"/>
-      <c r="M34" s="62" t="s">
+      <c r="J34" s="30"/>
+      <c r="K34" s="30"/>
+      <c r="L34" s="30"/>
+      <c r="M34" s="61" t="s">
         <v>61</v>
       </c>
-      <c r="N34" s="62"/>
-      <c r="O34" s="62"/>
-      <c r="P34" s="62"/>
-      <c r="Q34" s="63" t="s">
+      <c r="N34" s="61"/>
+      <c r="O34" s="61"/>
+      <c r="P34" s="61"/>
+      <c r="Q34" s="62" t="s">
         <v>62</v>
       </c>
-      <c r="R34" s="63"/>
+      <c r="R34" s="62"/>
     </row>
     <row r="35" s="16" customFormat="true" ht="29.7" hidden="false" customHeight="true" outlineLevel="1" collapsed="false">
-      <c r="A35" s="65" t="n">
+      <c r="A35" s="64" t="n">
         <v>44223</v>
       </c>
-      <c r="B35" s="37" t="s">
+      <c r="B35" s="36" t="s">
         <v>63</v>
       </c>
-      <c r="C35" s="37"/>
-      <c r="D35" s="37"/>
-      <c r="E35" s="37"/>
-      <c r="F35" s="37"/>
-      <c r="G35" s="66" t="n">
+      <c r="C35" s="36"/>
+      <c r="D35" s="36"/>
+      <c r="E35" s="36"/>
+      <c r="F35" s="36"/>
+      <c r="G35" s="65" t="n">
         <v>-808</v>
       </c>
-      <c r="H35" s="67" t="s">
+      <c r="H35" s="66" t="s">
         <v>64</v>
       </c>
-      <c r="I35" s="68" t="s">
+      <c r="I35" s="67" t="s">
         <v>65</v>
       </c>
-      <c r="J35" s="68"/>
-      <c r="K35" s="68"/>
-      <c r="L35" s="68"/>
-      <c r="M35" s="69" t="s">
+      <c r="J35" s="67"/>
+      <c r="K35" s="67"/>
+      <c r="L35" s="67"/>
+      <c r="M35" s="68" t="s">
         <v>66</v>
       </c>
-      <c r="N35" s="69"/>
-      <c r="O35" s="69"/>
-      <c r="P35" s="69"/>
-      <c r="Q35" s="67" t="s">
+      <c r="N35" s="68"/>
+      <c r="O35" s="68"/>
+      <c r="P35" s="68"/>
+      <c r="Q35" s="66" t="s">
         <v>67</v>
       </c>
-      <c r="R35" s="67"/>
-    </row>
-    <row r="36" s="73" customFormat="true" ht="17.1" hidden="false" customHeight="true" outlineLevel="1" collapsed="false">
-      <c r="A36" s="48"/>
-      <c r="B36" s="48"/>
-      <c r="C36" s="48"/>
-      <c r="D36" s="48"/>
-      <c r="E36" s="48"/>
-      <c r="F36" s="48"/>
-      <c r="G36" s="48"/>
-      <c r="H36" s="70"/>
-      <c r="I36" s="71"/>
-      <c r="J36" s="71"/>
-      <c r="K36" s="48"/>
-      <c r="L36" s="48"/>
-      <c r="M36" s="48"/>
-      <c r="N36" s="48"/>
-      <c r="O36" s="72"/>
-      <c r="P36" s="71"/>
-      <c r="Q36" s="71"/>
-      <c r="R36" s="71"/>
+      <c r="R35" s="66"/>
+    </row>
+    <row r="36" s="1" customFormat="true" ht="17.1" hidden="false" customHeight="true" outlineLevel="1" collapsed="false">
+      <c r="A36" s="47"/>
+      <c r="B36" s="47"/>
+      <c r="C36" s="47"/>
+      <c r="D36" s="47"/>
+      <c r="E36" s="47"/>
+      <c r="F36" s="47"/>
+      <c r="G36" s="47"/>
+      <c r="H36" s="69"/>
+      <c r="I36" s="70"/>
+      <c r="J36" s="70"/>
+      <c r="K36" s="47"/>
+      <c r="L36" s="47"/>
+      <c r="M36" s="47"/>
+      <c r="N36" s="47"/>
+      <c r="O36" s="71"/>
+      <c r="P36" s="70"/>
+      <c r="Q36" s="70"/>
+      <c r="R36" s="70"/>
     </row>
     <row r="37" s="16" customFormat="true" ht="17.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A37" s="30" t="s">
+      <c r="A37" s="29" t="s">
         <v>68</v>
       </c>
-      <c r="B37" s="30"/>
-      <c r="C37" s="30"/>
-      <c r="D37" s="30"/>
-      <c r="E37" s="74"/>
-      <c r="F37" s="74"/>
-      <c r="G37" s="74"/>
-      <c r="H37" s="55"/>
-      <c r="I37" s="75"/>
-      <c r="J37" s="76"/>
+      <c r="B37" s="29"/>
+      <c r="C37" s="29"/>
+      <c r="D37" s="29"/>
+      <c r="E37" s="72"/>
+      <c r="F37" s="72"/>
+      <c r="G37" s="72"/>
+      <c r="H37" s="54"/>
+      <c r="I37" s="73"/>
+      <c r="J37" s="74"/>
       <c r="K37" s="27"/>
       <c r="L37" s="27"/>
       <c r="M37" s="27"/>
@@ -2202,319 +2236,319 @@
       <c r="O37" s="27"/>
       <c r="P37" s="27"/>
     </row>
-    <row r="38" s="81" customFormat="true" ht="56.7" hidden="false" customHeight="true" outlineLevel="1" collapsed="false">
-      <c r="A38" s="77" t="s">
+    <row r="38" s="78" customFormat="true" ht="56.7" hidden="false" customHeight="true" outlineLevel="1" collapsed="false">
+      <c r="A38" s="61" t="s">
         <v>69</v>
       </c>
-      <c r="B38" s="77"/>
-      <c r="C38" s="77"/>
-      <c r="D38" s="78" t="s">
+      <c r="B38" s="61"/>
+      <c r="C38" s="61"/>
+      <c r="D38" s="75" t="s">
         <v>70</v>
       </c>
-      <c r="E38" s="78" t="s">
+      <c r="E38" s="75" t="s">
         <v>71</v>
       </c>
-      <c r="F38" s="78" t="s">
+      <c r="F38" s="75" t="s">
         <v>72</v>
       </c>
-      <c r="G38" s="78" t="s">
+      <c r="G38" s="75" t="s">
         <v>73</v>
       </c>
-      <c r="H38" s="79" t="s">
+      <c r="H38" s="76" t="s">
         <v>74</v>
       </c>
-      <c r="I38" s="79" t="s">
+      <c r="I38" s="76" t="s">
         <v>75</v>
       </c>
-      <c r="J38" s="79" t="s">
+      <c r="J38" s="76" t="s">
         <v>76</v>
       </c>
-      <c r="K38" s="77" t="s">
+      <c r="K38" s="61" t="s">
         <v>77</v>
       </c>
-      <c r="L38" s="77"/>
-      <c r="M38" s="77"/>
-      <c r="N38" s="63" t="s">
+      <c r="L38" s="61"/>
+      <c r="M38" s="61"/>
+      <c r="N38" s="62" t="s">
         <v>62</v>
       </c>
-      <c r="O38" s="63"/>
-      <c r="P38" s="80"/>
-      <c r="Q38" s="80" t="s">
+      <c r="O38" s="62"/>
+      <c r="P38" s="77"/>
+      <c r="Q38" s="77" t="s">
         <v>78</v>
       </c>
-      <c r="R38" s="80"/>
-      <c r="S38" s="80"/>
-    </row>
-    <row r="39" s="81" customFormat="true" ht="29.7" hidden="false" customHeight="true" outlineLevel="1" collapsed="false">
-      <c r="A39" s="82" t="s">
+      <c r="R38" s="77"/>
+      <c r="S38" s="77"/>
+    </row>
+    <row r="39" s="78" customFormat="true" ht="29.7" hidden="false" customHeight="true" outlineLevel="1" collapsed="false">
+      <c r="A39" s="79" t="s">
         <v>79</v>
       </c>
-      <c r="B39" s="82"/>
-      <c r="C39" s="82"/>
-      <c r="D39" s="83" t="n">
+      <c r="B39" s="79"/>
+      <c r="C39" s="79"/>
+      <c r="D39" s="80" t="n">
         <v>44210</v>
       </c>
-      <c r="E39" s="84" t="n">
+      <c r="E39" s="81" t="n">
         <v>2600</v>
       </c>
-      <c r="F39" s="85" t="n">
+      <c r="F39" s="82" t="n">
         <v>2.391</v>
       </c>
-      <c r="G39" s="86" t="n">
+      <c r="G39" s="83" t="n">
         <v>6216.6</v>
       </c>
-      <c r="H39" s="87" t="n">
+      <c r="H39" s="84" t="n">
         <v>6216.6</v>
       </c>
-      <c r="I39" s="88" t="s">
+      <c r="I39" s="85" t="s">
         <v>64</v>
       </c>
-      <c r="J39" s="89" t="n">
+      <c r="J39" s="86" t="n">
         <v>44223</v>
       </c>
-      <c r="K39" s="82" t="s">
+      <c r="K39" s="79" t="s">
         <v>80</v>
       </c>
-      <c r="L39" s="82"/>
-      <c r="M39" s="82"/>
-      <c r="N39" s="67" t="s">
+      <c r="L39" s="79"/>
+      <c r="M39" s="79"/>
+      <c r="N39" s="66" t="s">
         <v>67</v>
       </c>
-      <c r="O39" s="67"/>
-      <c r="P39" s="80"/>
-      <c r="Q39" s="80"/>
-      <c r="R39" s="80"/>
-      <c r="S39" s="80"/>
-    </row>
-    <row r="40" s="94" customFormat="true" ht="13.2" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
-      <c r="A40" s="90"/>
-      <c r="B40" s="90"/>
-      <c r="C40" s="90"/>
-      <c r="D40" s="91"/>
-      <c r="E40" s="90"/>
-      <c r="F40" s="91"/>
-      <c r="G40" s="91"/>
-      <c r="H40" s="91"/>
-      <c r="I40" s="92"/>
-      <c r="J40" s="91"/>
-      <c r="K40" s="90"/>
-      <c r="L40" s="90"/>
-      <c r="M40" s="90"/>
-      <c r="N40" s="93"/>
-      <c r="O40" s="93"/>
-      <c r="P40" s="80"/>
-      <c r="Q40" s="80"/>
-      <c r="R40" s="80"/>
+      <c r="O39" s="66"/>
+      <c r="P39" s="77"/>
+      <c r="Q39" s="77"/>
+      <c r="R39" s="77"/>
+      <c r="S39" s="77"/>
+    </row>
+    <row r="40" s="91" customFormat="true" ht="13.2" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
+      <c r="A40" s="87"/>
+      <c r="B40" s="87"/>
+      <c r="C40" s="87"/>
+      <c r="D40" s="88"/>
+      <c r="E40" s="87"/>
+      <c r="F40" s="88"/>
+      <c r="G40" s="88"/>
+      <c r="H40" s="88"/>
+      <c r="I40" s="89"/>
+      <c r="J40" s="88"/>
+      <c r="K40" s="87"/>
+      <c r="L40" s="87"/>
+      <c r="M40" s="87"/>
+      <c r="N40" s="90"/>
+      <c r="O40" s="90"/>
+      <c r="P40" s="77"/>
+      <c r="Q40" s="77"/>
+      <c r="R40" s="77"/>
     </row>
     <row r="41" s="15" customFormat="true" ht="17.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A41" s="30" t="s">
+      <c r="A41" s="29" t="s">
         <v>81</v>
       </c>
-      <c r="B41" s="30"/>
-      <c r="C41" s="30"/>
-      <c r="D41" s="30"/>
-      <c r="E41" s="30"/>
-      <c r="F41" s="30"/>
-      <c r="G41" s="30"/>
-      <c r="H41" s="30"/>
-      <c r="I41" s="30"/>
-      <c r="J41" s="30"/>
-      <c r="K41" s="30"/>
-      <c r="L41" s="30"/>
-      <c r="M41" s="30"/>
+      <c r="B41" s="29"/>
+      <c r="C41" s="29"/>
+      <c r="D41" s="29"/>
+      <c r="E41" s="29"/>
+      <c r="F41" s="29"/>
+      <c r="G41" s="29"/>
+      <c r="H41" s="29"/>
+      <c r="I41" s="29"/>
+      <c r="J41" s="29"/>
+      <c r="K41" s="29"/>
+      <c r="L41" s="29"/>
+      <c r="M41" s="29"/>
       <c r="N41" s="22"/>
       <c r="O41" s="22"/>
-      <c r="P41" s="95"/>
+      <c r="P41" s="92"/>
     </row>
     <row r="42" s="15" customFormat="true" ht="43.2" hidden="false" customHeight="true" outlineLevel="1" collapsed="false">
-      <c r="A42" s="78" t="s">
+      <c r="A42" s="75" t="s">
         <v>82</v>
       </c>
-      <c r="B42" s="78"/>
-      <c r="C42" s="78"/>
-      <c r="D42" s="78" t="s">
+      <c r="B42" s="75"/>
+      <c r="C42" s="75"/>
+      <c r="D42" s="75" t="s">
         <v>83</v>
       </c>
-      <c r="E42" s="78"/>
-      <c r="F42" s="78" t="s">
+      <c r="E42" s="75"/>
+      <c r="F42" s="75" t="s">
         <v>84</v>
       </c>
-      <c r="G42" s="78"/>
-      <c r="H42" s="78" t="s">
+      <c r="G42" s="75"/>
+      <c r="H42" s="75" t="s">
         <v>85</v>
       </c>
-      <c r="I42" s="78"/>
-      <c r="J42" s="78" t="s">
+      <c r="I42" s="75"/>
+      <c r="J42" s="75" t="s">
         <v>86</v>
       </c>
-      <c r="K42" s="78"/>
-      <c r="L42" s="78" t="s">
+      <c r="K42" s="75"/>
+      <c r="L42" s="75" t="s">
         <v>87</v>
       </c>
-      <c r="M42" s="78"/>
-      <c r="N42" s="78" t="s">
+      <c r="M42" s="75"/>
+      <c r="N42" s="75" t="s">
         <v>88</v>
       </c>
-      <c r="O42" s="78"/>
+      <c r="O42" s="75"/>
       <c r="P42" s="22"/>
       <c r="Q42" s="22"/>
-      <c r="R42" s="95"/>
+      <c r="R42" s="92"/>
     </row>
     <row r="43" s="15" customFormat="true" ht="17.1" hidden="false" customHeight="true" outlineLevel="1" collapsed="false">
-      <c r="A43" s="88" t="s">
+      <c r="A43" s="85" t="s">
         <v>89</v>
       </c>
-      <c r="B43" s="88"/>
-      <c r="C43" s="88"/>
-      <c r="D43" s="88"/>
-      <c r="E43" s="88"/>
-      <c r="F43" s="88"/>
-      <c r="G43" s="88"/>
-      <c r="H43" s="96"/>
-      <c r="I43" s="96"/>
-      <c r="J43" s="88"/>
-      <c r="K43" s="88"/>
-      <c r="L43" s="88"/>
-      <c r="M43" s="88"/>
-      <c r="N43" s="88"/>
-      <c r="O43" s="88"/>
+      <c r="B43" s="85"/>
+      <c r="C43" s="85"/>
+      <c r="D43" s="85"/>
+      <c r="E43" s="85"/>
+      <c r="F43" s="85"/>
+      <c r="G43" s="85"/>
+      <c r="H43" s="93"/>
+      <c r="I43" s="93"/>
+      <c r="J43" s="85"/>
+      <c r="K43" s="85"/>
+      <c r="L43" s="85"/>
+      <c r="M43" s="85"/>
+      <c r="N43" s="85"/>
+      <c r="O43" s="85"/>
       <c r="P43" s="22"/>
       <c r="Q43" s="22"/>
-      <c r="R43" s="95"/>
-    </row>
-    <row r="44" s="51" customFormat="true" ht="17.1" hidden="false" customHeight="true" outlineLevel="1" collapsed="false">
-      <c r="A44" s="97"/>
-      <c r="B44" s="97"/>
-      <c r="C44" s="97"/>
-      <c r="D44" s="97"/>
-      <c r="E44" s="97"/>
-      <c r="F44" s="97"/>
-      <c r="G44" s="97"/>
-      <c r="H44" s="97"/>
-      <c r="I44" s="97"/>
-      <c r="J44" s="97"/>
-      <c r="K44" s="97"/>
-      <c r="L44" s="97"/>
-      <c r="M44" s="98"/>
-      <c r="N44" s="97"/>
-      <c r="O44" s="97"/>
+      <c r="R43" s="92"/>
+    </row>
+    <row r="44" s="50" customFormat="true" ht="17.1" hidden="false" customHeight="true" outlineLevel="1" collapsed="false">
+      <c r="A44" s="94"/>
+      <c r="B44" s="94"/>
+      <c r="C44" s="94"/>
+      <c r="D44" s="94"/>
+      <c r="E44" s="94"/>
+      <c r="F44" s="94"/>
+      <c r="G44" s="94"/>
+      <c r="H44" s="94"/>
+      <c r="I44" s="94"/>
+      <c r="J44" s="94"/>
+      <c r="K44" s="94"/>
+      <c r="L44" s="94"/>
+      <c r="M44" s="70"/>
+      <c r="N44" s="94"/>
+      <c r="O44" s="94"/>
     </row>
     <row r="45" s="15" customFormat="true" ht="17.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A45" s="30" t="s">
+      <c r="A45" s="29" t="s">
         <v>90</v>
       </c>
-      <c r="B45" s="30"/>
-      <c r="C45" s="30"/>
-      <c r="D45" s="30"/>
-      <c r="E45" s="30"/>
-      <c r="F45" s="30"/>
-      <c r="G45" s="30"/>
-      <c r="H45" s="30"/>
-      <c r="I45" s="30"/>
-      <c r="J45" s="30"/>
-      <c r="K45" s="30"/>
-      <c r="L45" s="30"/>
-      <c r="M45" s="30"/>
+      <c r="B45" s="29"/>
+      <c r="C45" s="29"/>
+      <c r="D45" s="29"/>
+      <c r="E45" s="29"/>
+      <c r="F45" s="29"/>
+      <c r="G45" s="29"/>
+      <c r="H45" s="29"/>
+      <c r="I45" s="29"/>
+      <c r="J45" s="29"/>
+      <c r="K45" s="29"/>
+      <c r="L45" s="29"/>
+      <c r="M45" s="29"/>
       <c r="N45" s="22"/>
       <c r="O45" s="22"/>
-      <c r="P45" s="95"/>
-    </row>
-    <row r="46" s="101" customFormat="true" ht="56.7" hidden="false" customHeight="true" outlineLevel="1" collapsed="false">
-      <c r="A46" s="34" t="s">
+      <c r="P45" s="92"/>
+    </row>
+    <row r="46" s="97" customFormat="true" ht="56.7" hidden="false" customHeight="true" outlineLevel="1" collapsed="false">
+      <c r="A46" s="33" t="s">
         <v>91</v>
       </c>
-      <c r="B46" s="34"/>
-      <c r="C46" s="34" t="s">
+      <c r="B46" s="33"/>
+      <c r="C46" s="33" t="s">
         <v>92</v>
       </c>
-      <c r="D46" s="34"/>
-      <c r="E46" s="31" t="s">
+      <c r="D46" s="33"/>
+      <c r="E46" s="30" t="s">
         <v>93</v>
       </c>
-      <c r="F46" s="31"/>
-      <c r="G46" s="31" t="s">
+      <c r="F46" s="30"/>
+      <c r="G46" s="30" t="s">
         <v>94</v>
       </c>
-      <c r="H46" s="31"/>
-      <c r="I46" s="31" t="s">
+      <c r="H46" s="30"/>
+      <c r="I46" s="30" t="s">
         <v>95</v>
       </c>
-      <c r="J46" s="31"/>
-      <c r="K46" s="31" t="s">
+      <c r="J46" s="30"/>
+      <c r="K46" s="30" t="s">
         <v>96</v>
       </c>
-      <c r="L46" s="31"/>
-      <c r="M46" s="31" t="s">
+      <c r="L46" s="30"/>
+      <c r="M46" s="30" t="s">
         <v>97</v>
       </c>
-      <c r="N46" s="31"/>
-      <c r="O46" s="31" t="s">
+      <c r="N46" s="30"/>
+      <c r="O46" s="30" t="s">
         <v>98</v>
       </c>
-      <c r="P46" s="31"/>
-      <c r="Q46" s="31" t="s">
+      <c r="P46" s="30"/>
+      <c r="Q46" s="30" t="s">
         <v>99</v>
       </c>
-      <c r="R46" s="31"/>
-      <c r="S46" s="99"/>
-      <c r="T46" s="99"/>
-      <c r="U46" s="99"/>
-      <c r="V46" s="99"/>
-      <c r="W46" s="100"/>
+      <c r="R46" s="30"/>
+      <c r="S46" s="95"/>
+      <c r="T46" s="95"/>
+      <c r="U46" s="95"/>
+      <c r="V46" s="95"/>
+      <c r="W46" s="96"/>
     </row>
     <row r="47" s="15" customFormat="true" ht="17.1" hidden="false" customHeight="true" outlineLevel="1" collapsed="false">
-      <c r="A47" s="102" t="s">
+      <c r="A47" s="98" t="s">
         <v>47</v>
       </c>
-      <c r="B47" s="102"/>
-      <c r="C47" s="102"/>
-      <c r="D47" s="102"/>
-      <c r="E47" s="102"/>
-      <c r="F47" s="102"/>
-      <c r="G47" s="102"/>
-      <c r="H47" s="102"/>
-      <c r="I47" s="102"/>
-      <c r="J47" s="102"/>
-      <c r="K47" s="102"/>
-      <c r="L47" s="102"/>
-      <c r="M47" s="102"/>
-      <c r="N47" s="102"/>
-      <c r="O47" s="103"/>
-      <c r="P47" s="103"/>
-      <c r="Q47" s="103"/>
-      <c r="R47" s="103"/>
+      <c r="B47" s="98"/>
+      <c r="C47" s="98"/>
+      <c r="D47" s="98"/>
+      <c r="E47" s="98"/>
+      <c r="F47" s="98"/>
+      <c r="G47" s="98"/>
+      <c r="H47" s="98"/>
+      <c r="I47" s="98"/>
+      <c r="J47" s="98"/>
+      <c r="K47" s="98"/>
+      <c r="L47" s="98"/>
+      <c r="M47" s="98"/>
+      <c r="N47" s="98"/>
+      <c r="O47" s="99"/>
+      <c r="P47" s="99"/>
+      <c r="Q47" s="99"/>
+      <c r="R47" s="99"/>
       <c r="S47" s="22"/>
       <c r="T47" s="22"/>
       <c r="U47" s="22"/>
       <c r="V47" s="22"/>
-      <c r="W47" s="95"/>
-    </row>
-    <row r="48" s="29" customFormat="true" ht="17.1" hidden="false" customHeight="true" outlineLevel="1" collapsed="false">
-      <c r="A48" s="49"/>
-      <c r="B48" s="49"/>
-      <c r="C48" s="49"/>
-      <c r="D48" s="49"/>
-      <c r="E48" s="49"/>
-      <c r="F48" s="49"/>
-      <c r="G48" s="49"/>
-      <c r="H48" s="49"/>
-      <c r="I48" s="49"/>
-      <c r="J48" s="49"/>
-      <c r="K48" s="49"/>
-      <c r="L48" s="49"/>
-      <c r="M48" s="49"/>
-      <c r="N48" s="98"/>
-      <c r="O48" s="49"/>
-      <c r="P48" s="49"/>
-      <c r="Q48" s="49"/>
-      <c r="R48" s="98"/>
+      <c r="W47" s="92"/>
+    </row>
+    <row r="48" s="1" customFormat="true" ht="17.1" hidden="false" customHeight="true" outlineLevel="1" collapsed="false">
+      <c r="A48" s="48"/>
+      <c r="B48" s="48"/>
+      <c r="C48" s="48"/>
+      <c r="D48" s="48"/>
+      <c r="E48" s="48"/>
+      <c r="F48" s="48"/>
+      <c r="G48" s="48"/>
+      <c r="H48" s="48"/>
+      <c r="I48" s="48"/>
+      <c r="J48" s="48"/>
+      <c r="K48" s="48"/>
+      <c r="L48" s="48"/>
+      <c r="M48" s="48"/>
+      <c r="N48" s="70"/>
+      <c r="O48" s="48"/>
+      <c r="P48" s="48"/>
+      <c r="Q48" s="48"/>
+      <c r="R48" s="70"/>
     </row>
     <row r="49" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="104"/>
-      <c r="B49" s="104"/>
-      <c r="C49" s="104"/>
-      <c r="D49" s="104"/>
-      <c r="E49" s="104"/>
+      <c r="A49" s="100"/>
+      <c r="B49" s="100"/>
+      <c r="C49" s="100"/>
+      <c r="D49" s="100"/>
+      <c r="E49" s="100"/>
       <c r="F49" s="22"/>
       <c r="G49" s="22"/>
       <c r="H49" s="22"/>
@@ -2525,11 +2559,11 @@
       <c r="M49" s="22"/>
     </row>
     <row r="50" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="105"/>
-      <c r="B50" s="104"/>
-      <c r="C50" s="104"/>
-      <c r="D50" s="104"/>
-      <c r="E50" s="104"/>
+      <c r="A50" s="101"/>
+      <c r="B50" s="100"/>
+      <c r="C50" s="100"/>
+      <c r="D50" s="100"/>
+      <c r="E50" s="100"/>
       <c r="F50" s="22"/>
       <c r="G50" s="22"/>
       <c r="H50" s="22"/>
@@ -2540,15 +2574,15 @@
       <c r="M50" s="22"/>
     </row>
     <row r="51" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A51" s="106" t="s">
+      <c r="A51" s="102" t="s">
         <v>100</v>
       </c>
-      <c r="B51" s="106"/>
-      <c r="C51" s="106"/>
-      <c r="D51" s="106"/>
-      <c r="E51" s="106"/>
-      <c r="F51" s="106"/>
-      <c r="G51" s="106"/>
+      <c r="B51" s="102"/>
+      <c r="C51" s="102"/>
+      <c r="D51" s="102"/>
+      <c r="E51" s="102"/>
+      <c r="F51" s="102"/>
+      <c r="G51" s="102"/>
       <c r="H51" s="22"/>
       <c r="I51" s="22"/>
       <c r="J51" s="22"/>
@@ -2557,11 +2591,11 @@
       <c r="M51" s="22"/>
     </row>
     <row r="52" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A52" s="107" t="s">
+      <c r="A52" s="103" t="s">
         <v>101</v>
       </c>
-      <c r="B52" s="107"/>
-      <c r="C52" s="107"/>
+      <c r="B52" s="103"/>
+      <c r="C52" s="103"/>
       <c r="D52" s="14" t="s">
         <v>102</v>
       </c>
@@ -2813,7 +2847,7 @@
       <selection pane="topLeft" activeCell="U27" activeCellId="0" sqref="U27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.89"/>
@@ -2846,136 +2880,136 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="108" t="s">
+      <c r="A1" s="104" t="s">
         <v>103</v>
       </c>
-      <c r="V1" s="109" t="s">
+      <c r="V1" s="105" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="V2" s="109" t="s">
+      <c r="V2" s="105" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="V3" s="109" t="s">
+      <c r="V3" s="105" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="V4" s="109" t="s">
+      <c r="V4" s="105" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="V5" s="109" t="s">
+      <c r="V5" s="105" t="s">
         <v>108</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="V6" s="109" t="s">
+      <c r="V6" s="105" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="V7" s="109" t="s">
+      <c r="V7" s="105" t="s">
         <v>110</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="V8" s="109" t="s">
+      <c r="V8" s="105" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="V9" s="109" t="s">
+      <c r="V9" s="105" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="V10" s="109" t="s">
+      <c r="V10" s="105" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="V11" s="109" t="s">
+      <c r="V11" s="105" t="s">
         <v>114</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="V12" s="109" t="s">
+      <c r="V12" s="105" t="s">
         <v>115</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="V13" s="109" t="s">
+      <c r="V13" s="105" t="s">
         <v>116</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="V14" s="109" t="s">
+      <c r="V14" s="105" t="s">
         <v>117</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="V15" s="109" t="s">
+      <c r="V15" s="105" t="s">
         <v>118</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="V16" s="109" t="s">
+      <c r="V16" s="105" t="s">
         <v>119</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="V17" s="109" t="s">
+      <c r="V17" s="105" t="s">
         <v>120</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="V18" s="109" t="s">
+      <c r="V18" s="105" t="s">
         <v>121</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="109"/>
+      <c r="A20" s="105"/>
     </row>
     <row r="21" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="109"/>
+      <c r="A21" s="105"/>
     </row>
     <row r="22" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="109"/>
+      <c r="A22" s="105"/>
     </row>
     <row r="23" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="109"/>
+      <c r="A23" s="105"/>
     </row>
     <row r="24" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="109"/>
+      <c r="A24" s="105"/>
     </row>
     <row r="25" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="109"/>
+      <c r="A25" s="105"/>
     </row>
     <row r="26" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="109"/>
+      <c r="A26" s="105"/>
     </row>
     <row r="27" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="109"/>
+      <c r="A27" s="105"/>
     </row>
     <row r="28" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="109"/>
+      <c r="A28" s="105"/>
     </row>
     <row r="29" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="109"/>
+      <c r="A29" s="105"/>
     </row>
     <row r="30" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="109"/>
+      <c r="A30" s="105"/>
     </row>
     <row r="31" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="109"/>
+      <c r="A31" s="105"/>
     </row>
     <row r="32" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="109"/>
+      <c r="A32" s="105"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
StatementXLS: assets load from statement was implemented Tests were updated
</commit_message>
<xml_diff>
--- a/tests/test_data/kit.xlsx
+++ b/tests/test_data/kit.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="133">
   <si>
     <t xml:space="preserve">КИТ Финанс (АО)</t>
   </si>
@@ -170,7 +170,40 @@
     <t xml:space="preserve">Валюта номинала</t>
   </si>
   <si>
-    <t xml:space="preserve">xxx</t>
+    <t xml:space="preserve">АО "Аэрофлот" ПАО</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RU0009062285</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1-01-00010-A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">РУБ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">НРД торг. МБ обеспечение</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FinEx Gold ETF USD Shares</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IE00B8XB7377</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CEOGCS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">USD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">АО "Тинькофф Банк" БО-07</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RU000A0JWM31</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4B020702673B</t>
   </si>
   <si>
     <t xml:space="preserve">Оценка активов</t>
@@ -195,6 +228,9 @@
     <t xml:space="preserve">с учетом незавершенных сделок и договоров займа ЦБ</t>
   </si>
   <si>
+    <t xml:space="preserve">xxx</t>
+  </si>
+  <si>
     <t xml:space="preserve">Движение денежных средств по неторговым операциям</t>
   </si>
   <si>
@@ -220,9 +256,6 @@
   </si>
   <si>
     <t xml:space="preserve">Налог с див.доход ФЛ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">РУБ</t>
   </si>
   <si>
     <t xml:space="preserve">выписка банка от 27.01.2021</t>
@@ -737,7 +770,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="106">
+  <cellXfs count="107">
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -920,6 +953,10 @@
     </xf>
     <xf numFmtId="166" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="169" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -1225,24 +1262,6 @@
       <numFmt numFmtId="164" formatCode="#,##0.0##########"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="#,##0.0##########"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="#,##0.0##########"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="#,##0.0##########"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="#,##0.0##########"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="#,##0.0##########"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="#,##0.0##########"/>
-    </dxf>
-    <dxf>
       <font>
         <b val="1"/>
         <i val="0"/>
@@ -1258,6 +1277,73 @@
       <numFmt numFmtId="164" formatCode="#,##0.0##########"/>
     </dxf>
     <dxf>
+      <font>
+        <name val="Calibri"/>
+        <charset val="204"/>
+        <family val="2"/>
+        <color rgb="FF000000"/>
+        <sz val="11"/>
+      </font>
+      <numFmt numFmtId="164" formatCode="#,##0.0##########"/>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="Calibri"/>
+        <charset val="204"/>
+        <family val="2"/>
+        <color rgb="FF000000"/>
+        <sz val="11"/>
+      </font>
+      <numFmt numFmtId="164" formatCode="#,##0.0##########"/>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="Calibri"/>
+        <charset val="204"/>
+        <family val="2"/>
+        <color rgb="FF000000"/>
+        <sz val="11"/>
+      </font>
+      <numFmt numFmtId="164" formatCode="#,##0.0##########"/>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="Calibri"/>
+        <charset val="204"/>
+        <family val="2"/>
+        <color rgb="FF000000"/>
+        <sz val="11"/>
+      </font>
+      <numFmt numFmtId="164" formatCode="#,##0.0##########"/>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="Calibri"/>
+        <charset val="204"/>
+        <family val="2"/>
+        <color rgb="FF000000"/>
+        <sz val="11"/>
+      </font>
+      <numFmt numFmtId="164" formatCode="#,##0.0##########"/>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="Calibri"/>
+        <charset val="204"/>
+        <family val="2"/>
+        <color rgb="FF000000"/>
+        <sz val="11"/>
+      </font>
+      <numFmt numFmtId="164" formatCode="#,##0.0##########"/>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="Calibri"/>
+        <charset val="204"/>
+        <family val="2"/>
+        <color rgb="FF000000"/>
+        <sz val="11"/>
+      </font>
       <numFmt numFmtId="164" formatCode="#,##0.0##########"/>
     </dxf>
   </dxfs>
@@ -1335,9 +1421,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>203760</xdr:colOff>
+      <xdr:colOff>203040</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>20880</xdr:rowOff>
+      <xdr:rowOff>20160</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1351,7 +1437,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="2742480" cy="691200"/>
+          <a:ext cx="2741760" cy="690480"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1371,10 +1457,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="true"/>
   </sheetPr>
-  <dimension ref="A1:AC52"/>
+  <dimension ref="A1:AC54"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J16" activeCellId="0" sqref="J16"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E29" activeCellId="0" sqref="E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="1" outlineLevelCol="0"/>
@@ -1923,666 +2009,816 @@
       </c>
       <c r="B26" s="35"/>
       <c r="C26" s="35"/>
-      <c r="D26" s="36"/>
-      <c r="E26" s="36"/>
-      <c r="F26" s="37"/>
-      <c r="G26" s="37"/>
-      <c r="H26" s="37"/>
-      <c r="I26" s="37"/>
-      <c r="J26" s="37"/>
-      <c r="K26" s="37"/>
-      <c r="L26" s="37"/>
-      <c r="M26" s="38"/>
-      <c r="N26" s="38"/>
-      <c r="O26" s="38"/>
-      <c r="P26" s="39"/>
+      <c r="D26" s="36" t="s">
+        <v>48</v>
+      </c>
+      <c r="E26" s="36" t="s">
+        <v>49</v>
+      </c>
+      <c r="F26" s="37" t="n">
+        <v>20</v>
+      </c>
+      <c r="G26" s="37" t="n">
+        <v>0</v>
+      </c>
+      <c r="H26" s="37" t="n">
+        <v>0</v>
+      </c>
+      <c r="I26" s="37" t="n">
+        <v>20</v>
+      </c>
+      <c r="J26" s="37" t="n">
+        <v>20</v>
+      </c>
+      <c r="K26" s="37" t="n">
+        <v>20</v>
+      </c>
+      <c r="L26" s="37" t="n">
+        <v>20</v>
+      </c>
+      <c r="M26" s="38" t="n">
+        <v>65.9</v>
+      </c>
+      <c r="N26" s="38" t="n">
+        <v>66</v>
+      </c>
+      <c r="O26" s="38" t="n">
+        <v>66</v>
+      </c>
+      <c r="P26" s="39" t="s">
+        <v>50</v>
+      </c>
       <c r="Q26" s="38"/>
-      <c r="R26" s="40"/>
-      <c r="S26" s="40"/>
-      <c r="T26" s="40"/>
-      <c r="U26" s="41"/>
+      <c r="R26" s="40" t="n">
+        <v>1318</v>
+      </c>
+      <c r="S26" s="40" t="n">
+        <v>1320</v>
+      </c>
+      <c r="T26" s="40" t="n">
+        <v>1320</v>
+      </c>
+      <c r="U26" s="41" t="s">
+        <v>51</v>
+      </c>
       <c r="V26" s="41"/>
-      <c r="W26" s="42"/>
-      <c r="X26" s="43"/>
+      <c r="W26" s="42" t="n">
+        <v>1</v>
+      </c>
+      <c r="X26" s="43" t="s">
+        <v>50</v>
+      </c>
       <c r="Y26" s="44"/>
       <c r="Z26" s="45"/>
       <c r="AA26" s="44"/>
       <c r="AB26" s="44"/>
       <c r="AC26" s="45"/>
     </row>
-    <row r="27" s="50" customFormat="true" ht="17.1" hidden="false" customHeight="true" outlineLevel="1" collapsed="false">
-      <c r="A27" s="46"/>
-      <c r="B27" s="47"/>
-      <c r="C27" s="47"/>
-      <c r="D27" s="48"/>
-      <c r="E27" s="48"/>
-      <c r="F27" s="48"/>
-      <c r="G27" s="48"/>
-      <c r="H27" s="48"/>
-      <c r="I27" s="48"/>
-      <c r="J27" s="48"/>
-      <c r="K27" s="48"/>
-      <c r="L27" s="48"/>
-      <c r="M27" s="48"/>
-      <c r="N27" s="48"/>
-      <c r="O27" s="48"/>
-      <c r="P27" s="47"/>
-      <c r="Q27" s="48"/>
-      <c r="R27" s="48"/>
-      <c r="S27" s="48"/>
-      <c r="T27" s="48"/>
-      <c r="U27" s="49"/>
-      <c r="V27" s="49"/>
-      <c r="W27" s="48"/>
-      <c r="X27" s="47"/>
-    </row>
-    <row r="28" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="29" t="s">
-        <v>48</v>
-      </c>
-      <c r="B28" s="51"/>
-      <c r="C28" s="51"/>
-      <c r="D28" s="51"/>
-      <c r="E28" s="51"/>
-      <c r="F28" s="51"/>
-      <c r="G28" s="51"/>
-      <c r="H28" s="51"/>
-      <c r="I28" s="51"/>
-      <c r="J28" s="51"/>
-      <c r="K28" s="51"/>
-      <c r="L28" s="51"/>
-      <c r="M28" s="51"/>
-      <c r="N28" s="51"/>
-      <c r="O28" s="51"/>
-      <c r="P28" s="51"/>
-      <c r="Q28" s="51"/>
-      <c r="R28" s="51"/>
-      <c r="S28" s="51"/>
-      <c r="T28" s="51"/>
-      <c r="U28" s="51"/>
-      <c r="V28" s="51"/>
-      <c r="W28" s="51"/>
-    </row>
-    <row r="29" customFormat="false" ht="15.3" hidden="false" customHeight="true" outlineLevel="1" collapsed="false">
-      <c r="A29" s="52" t="s">
-        <v>49</v>
-      </c>
-      <c r="B29" s="52"/>
-      <c r="C29" s="52"/>
-      <c r="D29" s="52"/>
-      <c r="E29" s="52" t="s">
+    <row r="27" s="34" customFormat="true" ht="15.3" hidden="false" customHeight="true" outlineLevel="1" collapsed="false">
+      <c r="A27" s="35" t="s">
+        <v>52</v>
+      </c>
+      <c r="B27" s="35"/>
+      <c r="C27" s="35"/>
+      <c r="D27" s="36" t="s">
+        <v>53</v>
+      </c>
+      <c r="E27" s="36" t="s">
+        <v>54</v>
+      </c>
+      <c r="F27" s="37" t="n">
+        <v>10</v>
+      </c>
+      <c r="G27" s="37" t="n">
+        <v>0</v>
+      </c>
+      <c r="H27" s="37" t="n">
+        <v>0</v>
+      </c>
+      <c r="I27" s="37" t="n">
+        <v>10</v>
+      </c>
+      <c r="J27" s="37" t="n">
+        <v>10</v>
+      </c>
+      <c r="K27" s="37" t="n">
+        <v>10</v>
+      </c>
+      <c r="L27" s="37" t="n">
+        <v>10</v>
+      </c>
+      <c r="M27" s="38" t="n">
+        <v>891.6</v>
+      </c>
+      <c r="N27" s="38" t="n">
+        <v>900</v>
+      </c>
+      <c r="O27" s="38" t="n">
+        <v>900</v>
+      </c>
+      <c r="P27" s="39" t="s">
         <v>50</v>
       </c>
-      <c r="F29" s="52"/>
-      <c r="G29" s="52"/>
-      <c r="H29" s="52"/>
-      <c r="I29" s="52" t="s">
+      <c r="Q27" s="38"/>
+      <c r="R27" s="40" t="n">
+        <v>8916</v>
+      </c>
+      <c r="S27" s="40" t="n">
+        <v>9000</v>
+      </c>
+      <c r="T27" s="40" t="n">
+        <v>9000</v>
+      </c>
+      <c r="U27" s="41" t="s">
         <v>51</v>
       </c>
-      <c r="J29" s="52"/>
-      <c r="K29" s="52"/>
-      <c r="L29" s="52"/>
-      <c r="M29" s="53"/>
-      <c r="N29" s="54"/>
-      <c r="O29" s="22"/>
-      <c r="P29" s="22"/>
-      <c r="Q29" s="22"/>
-      <c r="R29" s="22"/>
-      <c r="S29" s="22"/>
-    </row>
-    <row r="30" customFormat="false" ht="29.7" hidden="false" customHeight="true" outlineLevel="1" collapsed="false">
-      <c r="A30" s="55" t="s">
-        <v>52</v>
-      </c>
-      <c r="B30" s="55"/>
-      <c r="C30" s="55" t="s">
-        <v>53</v>
-      </c>
-      <c r="D30" s="55"/>
-      <c r="E30" s="55" t="s">
-        <v>52</v>
-      </c>
-      <c r="F30" s="55"/>
-      <c r="G30" s="55" t="s">
-        <v>54</v>
-      </c>
-      <c r="H30" s="55"/>
-      <c r="I30" s="55" t="s">
-        <v>52</v>
-      </c>
-      <c r="J30" s="55"/>
-      <c r="K30" s="55" t="s">
-        <v>54</v>
-      </c>
-      <c r="L30" s="55"/>
-      <c r="M30" s="53"/>
-      <c r="N30" s="54"/>
-      <c r="O30" s="22"/>
-      <c r="P30" s="22"/>
-      <c r="Q30" s="22"/>
-      <c r="R30" s="22"/>
-      <c r="S30" s="22"/>
-    </row>
-    <row r="31" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="1" collapsed="false">
-      <c r="A31" s="56" t="s">
-        <v>47</v>
-      </c>
-      <c r="B31" s="56"/>
-      <c r="C31" s="57"/>
-      <c r="D31" s="57"/>
-      <c r="E31" s="57"/>
-      <c r="F31" s="57"/>
-      <c r="G31" s="57"/>
-      <c r="H31" s="57"/>
-      <c r="I31" s="57"/>
-      <c r="J31" s="57"/>
-      <c r="K31" s="57"/>
-      <c r="L31" s="57"/>
-      <c r="M31" s="53"/>
-      <c r="N31" s="54"/>
+      <c r="V27" s="41"/>
+      <c r="W27" s="42" t="n">
+        <v>1</v>
+      </c>
+      <c r="X27" s="43" t="s">
+        <v>55</v>
+      </c>
+      <c r="Y27" s="44"/>
+      <c r="Z27" s="45"/>
+      <c r="AA27" s="44"/>
+      <c r="AB27" s="44"/>
+      <c r="AC27" s="45"/>
+    </row>
+    <row r="28" s="34" customFormat="true" ht="15.3" hidden="false" customHeight="true" outlineLevel="1" collapsed="false">
+      <c r="A28" s="35" t="s">
+        <v>56</v>
+      </c>
+      <c r="B28" s="35"/>
+      <c r="C28" s="35"/>
+      <c r="D28" s="36" t="s">
+        <v>57</v>
+      </c>
+      <c r="E28" s="36" t="s">
+        <v>58</v>
+      </c>
+      <c r="F28" s="37" t="n">
+        <v>50</v>
+      </c>
+      <c r="G28" s="37" t="n">
+        <v>0</v>
+      </c>
+      <c r="H28" s="37" t="n">
+        <v>0</v>
+      </c>
+      <c r="I28" s="37" t="n">
+        <v>50</v>
+      </c>
+      <c r="J28" s="37" t="n">
+        <v>50</v>
+      </c>
+      <c r="K28" s="37" t="n">
+        <v>50</v>
+      </c>
+      <c r="L28" s="37" t="n">
+        <v>50</v>
+      </c>
+      <c r="M28" s="38" t="n">
+        <v>100.05</v>
+      </c>
+      <c r="N28" s="38" t="n">
+        <v>100.05</v>
+      </c>
+      <c r="O28" s="38" t="n">
+        <v>100.09</v>
+      </c>
+      <c r="P28" s="39" t="s">
+        <v>50</v>
+      </c>
+      <c r="Q28" s="46" t="n">
+        <v>33</v>
+      </c>
+      <c r="R28" s="40" t="n">
+        <v>50025</v>
+      </c>
+      <c r="S28" s="40" t="n">
+        <v>50045</v>
+      </c>
+      <c r="T28" s="40" t="n">
+        <v>60385</v>
+      </c>
+      <c r="U28" s="41" t="s">
+        <v>51</v>
+      </c>
+      <c r="V28" s="41"/>
+      <c r="W28" s="42" t="n">
+        <v>1</v>
+      </c>
+      <c r="X28" s="43" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y28" s="44"/>
+      <c r="Z28" s="45"/>
+      <c r="AA28" s="44"/>
+      <c r="AB28" s="44"/>
+      <c r="AC28" s="45"/>
+    </row>
+    <row r="29" s="51" customFormat="true" ht="17.1" hidden="false" customHeight="true" outlineLevel="1" collapsed="false">
+      <c r="A29" s="47"/>
+      <c r="B29" s="48"/>
+      <c r="C29" s="48"/>
+      <c r="D29" s="49"/>
+      <c r="E29" s="49"/>
+      <c r="F29" s="49"/>
+      <c r="G29" s="49"/>
+      <c r="H29" s="49"/>
+      <c r="I29" s="49"/>
+      <c r="J29" s="49"/>
+      <c r="K29" s="49"/>
+      <c r="L29" s="49"/>
+      <c r="M29" s="49"/>
+      <c r="N29" s="49"/>
+      <c r="O29" s="49"/>
+      <c r="P29" s="48"/>
+      <c r="Q29" s="49"/>
+      <c r="R29" s="49"/>
+      <c r="S29" s="49"/>
+      <c r="T29" s="49"/>
+      <c r="U29" s="50"/>
+      <c r="V29" s="50"/>
+      <c r="W29" s="49"/>
+      <c r="X29" s="48"/>
+    </row>
+    <row r="30" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="B30" s="52"/>
+      <c r="C30" s="52"/>
+      <c r="D30" s="52"/>
+      <c r="E30" s="52"/>
+      <c r="F30" s="52"/>
+      <c r="G30" s="52"/>
+      <c r="H30" s="52"/>
+      <c r="I30" s="52"/>
+      <c r="J30" s="52"/>
+      <c r="K30" s="52"/>
+      <c r="L30" s="52"/>
+      <c r="M30" s="52"/>
+      <c r="N30" s="52"/>
+      <c r="O30" s="52"/>
+      <c r="P30" s="52"/>
+      <c r="Q30" s="52"/>
+      <c r="R30" s="52"/>
+      <c r="S30" s="52"/>
+      <c r="T30" s="52"/>
+      <c r="U30" s="52"/>
+      <c r="V30" s="52"/>
+      <c r="W30" s="52"/>
+    </row>
+    <row r="31" customFormat="false" ht="15.3" hidden="false" customHeight="true" outlineLevel="1" collapsed="false">
+      <c r="A31" s="53" t="s">
+        <v>60</v>
+      </c>
+      <c r="B31" s="53"/>
+      <c r="C31" s="53"/>
+      <c r="D31" s="53"/>
+      <c r="E31" s="53" t="s">
+        <v>61</v>
+      </c>
+      <c r="F31" s="53"/>
+      <c r="G31" s="53"/>
+      <c r="H31" s="53"/>
+      <c r="I31" s="53" t="s">
+        <v>62</v>
+      </c>
+      <c r="J31" s="53"/>
+      <c r="K31" s="53"/>
+      <c r="L31" s="53"/>
+      <c r="M31" s="54"/>
+      <c r="N31" s="55"/>
       <c r="O31" s="22"/>
       <c r="P31" s="22"/>
       <c r="Q31" s="22"/>
       <c r="R31" s="22"/>
       <c r="S31" s="22"/>
     </row>
-    <row r="32" s="50" customFormat="true" ht="16.5" hidden="false" customHeight="true" outlineLevel="1" collapsed="false">
-      <c r="A32" s="47"/>
-      <c r="B32" s="47"/>
-      <c r="C32" s="47"/>
-      <c r="D32" s="47"/>
-      <c r="E32" s="47"/>
-      <c r="F32" s="48"/>
-      <c r="G32" s="48"/>
-      <c r="H32" s="48"/>
-      <c r="I32" s="48"/>
-      <c r="J32" s="48"/>
-      <c r="K32" s="48"/>
-      <c r="L32" s="48"/>
-      <c r="M32" s="28"/>
-      <c r="N32" s="28"/>
-      <c r="O32" s="58"/>
-      <c r="P32" s="28"/>
-      <c r="Q32" s="28"/>
-      <c r="R32" s="28"/>
-      <c r="S32" s="28"/>
-      <c r="T32" s="59"/>
-      <c r="U32" s="59"/>
-      <c r="V32" s="28"/>
-      <c r="W32" s="58"/>
-    </row>
-    <row r="33" s="16" customFormat="true" ht="17.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A33" s="29" t="s">
-        <v>55</v>
-      </c>
-      <c r="B33" s="29"/>
-      <c r="C33" s="29"/>
-      <c r="D33" s="29"/>
-      <c r="E33" s="29"/>
-      <c r="F33" s="29"/>
-      <c r="G33" s="29"/>
-      <c r="H33" s="29"/>
-      <c r="I33" s="29"/>
-      <c r="J33" s="29"/>
-      <c r="K33" s="29"/>
-      <c r="L33" s="29"/>
-      <c r="M33" s="29"/>
-    </row>
-    <row r="34" s="63" customFormat="true" ht="15.3" hidden="false" customHeight="true" outlineLevel="1" collapsed="false">
-      <c r="A34" s="30" t="s">
-        <v>56</v>
-      </c>
-      <c r="B34" s="60" t="s">
-        <v>57</v>
-      </c>
-      <c r="C34" s="60"/>
-      <c r="D34" s="60"/>
-      <c r="E34" s="60"/>
-      <c r="F34" s="60"/>
-      <c r="G34" s="30" t="s">
-        <v>58</v>
-      </c>
-      <c r="H34" s="30" t="s">
-        <v>59</v>
-      </c>
-      <c r="I34" s="30" t="s">
-        <v>60</v>
-      </c>
-      <c r="J34" s="30"/>
-      <c r="K34" s="30"/>
-      <c r="L34" s="30"/>
-      <c r="M34" s="61" t="s">
-        <v>61</v>
-      </c>
-      <c r="N34" s="61"/>
-      <c r="O34" s="61"/>
-      <c r="P34" s="61"/>
-      <c r="Q34" s="62" t="s">
-        <v>62</v>
-      </c>
-      <c r="R34" s="62"/>
-    </row>
-    <row r="35" s="16" customFormat="true" ht="29.7" hidden="false" customHeight="true" outlineLevel="1" collapsed="false">
-      <c r="A35" s="64" t="n">
+    <row r="32" customFormat="false" ht="29.7" hidden="false" customHeight="true" outlineLevel="1" collapsed="false">
+      <c r="A32" s="56" t="s">
+        <v>63</v>
+      </c>
+      <c r="B32" s="56"/>
+      <c r="C32" s="56" t="s">
+        <v>64</v>
+      </c>
+      <c r="D32" s="56"/>
+      <c r="E32" s="56" t="s">
+        <v>63</v>
+      </c>
+      <c r="F32" s="56"/>
+      <c r="G32" s="56" t="s">
+        <v>65</v>
+      </c>
+      <c r="H32" s="56"/>
+      <c r="I32" s="56" t="s">
+        <v>63</v>
+      </c>
+      <c r="J32" s="56"/>
+      <c r="K32" s="56" t="s">
+        <v>65</v>
+      </c>
+      <c r="L32" s="56"/>
+      <c r="M32" s="54"/>
+      <c r="N32" s="55"/>
+      <c r="O32" s="22"/>
+      <c r="P32" s="22"/>
+      <c r="Q32" s="22"/>
+      <c r="R32" s="22"/>
+      <c r="S32" s="22"/>
+    </row>
+    <row r="33" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="1" collapsed="false">
+      <c r="A33" s="57" t="s">
+        <v>66</v>
+      </c>
+      <c r="B33" s="57"/>
+      <c r="C33" s="58"/>
+      <c r="D33" s="58"/>
+      <c r="E33" s="58"/>
+      <c r="F33" s="58"/>
+      <c r="G33" s="58"/>
+      <c r="H33" s="58"/>
+      <c r="I33" s="58"/>
+      <c r="J33" s="58"/>
+      <c r="K33" s="58"/>
+      <c r="L33" s="58"/>
+      <c r="M33" s="54"/>
+      <c r="N33" s="55"/>
+      <c r="O33" s="22"/>
+      <c r="P33" s="22"/>
+      <c r="Q33" s="22"/>
+      <c r="R33" s="22"/>
+      <c r="S33" s="22"/>
+    </row>
+    <row r="34" s="51" customFormat="true" ht="16.5" hidden="false" customHeight="true" outlineLevel="1" collapsed="false">
+      <c r="A34" s="48"/>
+      <c r="B34" s="48"/>
+      <c r="C34" s="48"/>
+      <c r="D34" s="48"/>
+      <c r="E34" s="48"/>
+      <c r="F34" s="49"/>
+      <c r="G34" s="49"/>
+      <c r="H34" s="49"/>
+      <c r="I34" s="49"/>
+      <c r="J34" s="49"/>
+      <c r="K34" s="49"/>
+      <c r="L34" s="49"/>
+      <c r="M34" s="28"/>
+      <c r="N34" s="28"/>
+      <c r="O34" s="59"/>
+      <c r="P34" s="28"/>
+      <c r="Q34" s="28"/>
+      <c r="R34" s="28"/>
+      <c r="S34" s="28"/>
+      <c r="T34" s="60"/>
+      <c r="U34" s="60"/>
+      <c r="V34" s="28"/>
+      <c r="W34" s="59"/>
+    </row>
+    <row r="35" s="16" customFormat="true" ht="17.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A35" s="29" t="s">
+        <v>67</v>
+      </c>
+      <c r="B35" s="29"/>
+      <c r="C35" s="29"/>
+      <c r="D35" s="29"/>
+      <c r="E35" s="29"/>
+      <c r="F35" s="29"/>
+      <c r="G35" s="29"/>
+      <c r="H35" s="29"/>
+      <c r="I35" s="29"/>
+      <c r="J35" s="29"/>
+      <c r="K35" s="29"/>
+      <c r="L35" s="29"/>
+      <c r="M35" s="29"/>
+    </row>
+    <row r="36" s="64" customFormat="true" ht="15.3" hidden="false" customHeight="true" outlineLevel="1" collapsed="false">
+      <c r="A36" s="30" t="s">
+        <v>68</v>
+      </c>
+      <c r="B36" s="61" t="s">
+        <v>69</v>
+      </c>
+      <c r="C36" s="61"/>
+      <c r="D36" s="61"/>
+      <c r="E36" s="61"/>
+      <c r="F36" s="61"/>
+      <c r="G36" s="30" t="s">
+        <v>70</v>
+      </c>
+      <c r="H36" s="30" t="s">
+        <v>71</v>
+      </c>
+      <c r="I36" s="30" t="s">
+        <v>72</v>
+      </c>
+      <c r="J36" s="30"/>
+      <c r="K36" s="30"/>
+      <c r="L36" s="30"/>
+      <c r="M36" s="62" t="s">
+        <v>73</v>
+      </c>
+      <c r="N36" s="62"/>
+      <c r="O36" s="62"/>
+      <c r="P36" s="62"/>
+      <c r="Q36" s="63" t="s">
+        <v>74</v>
+      </c>
+      <c r="R36" s="63"/>
+    </row>
+    <row r="37" s="16" customFormat="true" ht="29.7" hidden="false" customHeight="true" outlineLevel="1" collapsed="false">
+      <c r="A37" s="65" t="n">
         <v>44223</v>
       </c>
-      <c r="B35" s="36" t="s">
-        <v>63</v>
-      </c>
-      <c r="C35" s="36"/>
-      <c r="D35" s="36"/>
-      <c r="E35" s="36"/>
-      <c r="F35" s="36"/>
-      <c r="G35" s="65" t="n">
+      <c r="B37" s="36" t="s">
+        <v>75</v>
+      </c>
+      <c r="C37" s="36"/>
+      <c r="D37" s="36"/>
+      <c r="E37" s="36"/>
+      <c r="F37" s="36"/>
+      <c r="G37" s="66" t="n">
         <v>-808</v>
       </c>
-      <c r="H35" s="66" t="s">
-        <v>64</v>
-      </c>
-      <c r="I35" s="67" t="s">
-        <v>65</v>
-      </c>
-      <c r="J35" s="67"/>
-      <c r="K35" s="67"/>
-      <c r="L35" s="67"/>
-      <c r="M35" s="68" t="s">
+      <c r="H37" s="67" t="s">
+        <v>50</v>
+      </c>
+      <c r="I37" s="68" t="s">
+        <v>76</v>
+      </c>
+      <c r="J37" s="68"/>
+      <c r="K37" s="68"/>
+      <c r="L37" s="68"/>
+      <c r="M37" s="69" t="s">
+        <v>77</v>
+      </c>
+      <c r="N37" s="69"/>
+      <c r="O37" s="69"/>
+      <c r="P37" s="69"/>
+      <c r="Q37" s="67" t="s">
+        <v>78</v>
+      </c>
+      <c r="R37" s="67"/>
+    </row>
+    <row r="38" s="1" customFormat="true" ht="17.1" hidden="false" customHeight="true" outlineLevel="1" collapsed="false">
+      <c r="A38" s="48"/>
+      <c r="B38" s="48"/>
+      <c r="C38" s="48"/>
+      <c r="D38" s="48"/>
+      <c r="E38" s="48"/>
+      <c r="F38" s="48"/>
+      <c r="G38" s="48"/>
+      <c r="H38" s="70"/>
+      <c r="I38" s="71"/>
+      <c r="J38" s="71"/>
+      <c r="K38" s="48"/>
+      <c r="L38" s="48"/>
+      <c r="M38" s="48"/>
+      <c r="N38" s="48"/>
+      <c r="O38" s="72"/>
+      <c r="P38" s="71"/>
+      <c r="Q38" s="71"/>
+      <c r="R38" s="71"/>
+    </row>
+    <row r="39" s="16" customFormat="true" ht="17.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A39" s="29" t="s">
+        <v>79</v>
+      </c>
+      <c r="B39" s="29"/>
+      <c r="C39" s="29"/>
+      <c r="D39" s="29"/>
+      <c r="E39" s="73"/>
+      <c r="F39" s="73"/>
+      <c r="G39" s="73"/>
+      <c r="H39" s="55"/>
+      <c r="I39" s="74"/>
+      <c r="J39" s="75"/>
+      <c r="K39" s="27"/>
+      <c r="L39" s="27"/>
+      <c r="M39" s="27"/>
+      <c r="N39" s="27"/>
+      <c r="O39" s="27"/>
+      <c r="P39" s="27"/>
+    </row>
+    <row r="40" s="79" customFormat="true" ht="56.7" hidden="false" customHeight="true" outlineLevel="1" collapsed="false">
+      <c r="A40" s="62" t="s">
+        <v>80</v>
+      </c>
+      <c r="B40" s="62"/>
+      <c r="C40" s="62"/>
+      <c r="D40" s="76" t="s">
+        <v>81</v>
+      </c>
+      <c r="E40" s="76" t="s">
+        <v>82</v>
+      </c>
+      <c r="F40" s="76" t="s">
+        <v>83</v>
+      </c>
+      <c r="G40" s="76" t="s">
+        <v>84</v>
+      </c>
+      <c r="H40" s="77" t="s">
+        <v>85</v>
+      </c>
+      <c r="I40" s="77" t="s">
+        <v>86</v>
+      </c>
+      <c r="J40" s="77" t="s">
+        <v>87</v>
+      </c>
+      <c r="K40" s="62" t="s">
+        <v>88</v>
+      </c>
+      <c r="L40" s="62"/>
+      <c r="M40" s="62"/>
+      <c r="N40" s="63" t="s">
+        <v>74</v>
+      </c>
+      <c r="O40" s="63"/>
+      <c r="P40" s="78"/>
+      <c r="Q40" s="78" t="s">
+        <v>89</v>
+      </c>
+      <c r="R40" s="78"/>
+      <c r="S40" s="78"/>
+    </row>
+    <row r="41" s="79" customFormat="true" ht="29.7" hidden="false" customHeight="true" outlineLevel="1" collapsed="false">
+      <c r="A41" s="80" t="s">
+        <v>90</v>
+      </c>
+      <c r="B41" s="80"/>
+      <c r="C41" s="80"/>
+      <c r="D41" s="81" t="n">
+        <v>44210</v>
+      </c>
+      <c r="E41" s="82" t="n">
+        <v>2600</v>
+      </c>
+      <c r="F41" s="83" t="n">
+        <v>2.391</v>
+      </c>
+      <c r="G41" s="84" t="n">
+        <v>6216.6</v>
+      </c>
+      <c r="H41" s="85" t="n">
+        <v>6216.6</v>
+      </c>
+      <c r="I41" s="86" t="s">
+        <v>50</v>
+      </c>
+      <c r="J41" s="87" t="n">
+        <v>44223</v>
+      </c>
+      <c r="K41" s="80" t="s">
+        <v>91</v>
+      </c>
+      <c r="L41" s="80"/>
+      <c r="M41" s="80"/>
+      <c r="N41" s="67" t="s">
+        <v>78</v>
+      </c>
+      <c r="O41" s="67"/>
+      <c r="P41" s="78"/>
+      <c r="Q41" s="78"/>
+      <c r="R41" s="78"/>
+      <c r="S41" s="78"/>
+    </row>
+    <row r="42" s="92" customFormat="true" ht="13.2" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
+      <c r="A42" s="88"/>
+      <c r="B42" s="88"/>
+      <c r="C42" s="88"/>
+      <c r="D42" s="89"/>
+      <c r="E42" s="88"/>
+      <c r="F42" s="89"/>
+      <c r="G42" s="89"/>
+      <c r="H42" s="89"/>
+      <c r="I42" s="90"/>
+      <c r="J42" s="89"/>
+      <c r="K42" s="88"/>
+      <c r="L42" s="88"/>
+      <c r="M42" s="88"/>
+      <c r="N42" s="91"/>
+      <c r="O42" s="91"/>
+      <c r="P42" s="78"/>
+      <c r="Q42" s="78"/>
+      <c r="R42" s="78"/>
+    </row>
+    <row r="43" s="15" customFormat="true" ht="17.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A43" s="29" t="s">
+        <v>92</v>
+      </c>
+      <c r="B43" s="29"/>
+      <c r="C43" s="29"/>
+      <c r="D43" s="29"/>
+      <c r="E43" s="29"/>
+      <c r="F43" s="29"/>
+      <c r="G43" s="29"/>
+      <c r="H43" s="29"/>
+      <c r="I43" s="29"/>
+      <c r="J43" s="29"/>
+      <c r="K43" s="29"/>
+      <c r="L43" s="29"/>
+      <c r="M43" s="29"/>
+      <c r="N43" s="22"/>
+      <c r="O43" s="22"/>
+      <c r="P43" s="93"/>
+    </row>
+    <row r="44" s="15" customFormat="true" ht="43.2" hidden="false" customHeight="true" outlineLevel="1" collapsed="false">
+      <c r="A44" s="76" t="s">
+        <v>93</v>
+      </c>
+      <c r="B44" s="76"/>
+      <c r="C44" s="76"/>
+      <c r="D44" s="76" t="s">
+        <v>94</v>
+      </c>
+      <c r="E44" s="76"/>
+      <c r="F44" s="76" t="s">
+        <v>95</v>
+      </c>
+      <c r="G44" s="76"/>
+      <c r="H44" s="76" t="s">
+        <v>96</v>
+      </c>
+      <c r="I44" s="76"/>
+      <c r="J44" s="76" t="s">
+        <v>97</v>
+      </c>
+      <c r="K44" s="76"/>
+      <c r="L44" s="76" t="s">
+        <v>98</v>
+      </c>
+      <c r="M44" s="76"/>
+      <c r="N44" s="76" t="s">
+        <v>99</v>
+      </c>
+      <c r="O44" s="76"/>
+      <c r="P44" s="22"/>
+      <c r="Q44" s="22"/>
+      <c r="R44" s="93"/>
+    </row>
+    <row r="45" s="15" customFormat="true" ht="17.1" hidden="false" customHeight="true" outlineLevel="1" collapsed="false">
+      <c r="A45" s="86" t="s">
+        <v>100</v>
+      </c>
+      <c r="B45" s="86"/>
+      <c r="C45" s="86"/>
+      <c r="D45" s="86"/>
+      <c r="E45" s="86"/>
+      <c r="F45" s="86"/>
+      <c r="G45" s="86"/>
+      <c r="H45" s="94"/>
+      <c r="I45" s="94"/>
+      <c r="J45" s="86"/>
+      <c r="K45" s="86"/>
+      <c r="L45" s="86"/>
+      <c r="M45" s="86"/>
+      <c r="N45" s="86"/>
+      <c r="O45" s="86"/>
+      <c r="P45" s="22"/>
+      <c r="Q45" s="22"/>
+      <c r="R45" s="93"/>
+    </row>
+    <row r="46" s="51" customFormat="true" ht="17.1" hidden="false" customHeight="true" outlineLevel="1" collapsed="false">
+      <c r="A46" s="95"/>
+      <c r="B46" s="95"/>
+      <c r="C46" s="95"/>
+      <c r="D46" s="95"/>
+      <c r="E46" s="95"/>
+      <c r="F46" s="95"/>
+      <c r="G46" s="95"/>
+      <c r="H46" s="95"/>
+      <c r="I46" s="95"/>
+      <c r="J46" s="95"/>
+      <c r="K46" s="95"/>
+      <c r="L46" s="95"/>
+      <c r="M46" s="71"/>
+      <c r="N46" s="95"/>
+      <c r="O46" s="95"/>
+    </row>
+    <row r="47" s="15" customFormat="true" ht="17.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A47" s="29" t="s">
+        <v>101</v>
+      </c>
+      <c r="B47" s="29"/>
+      <c r="C47" s="29"/>
+      <c r="D47" s="29"/>
+      <c r="E47" s="29"/>
+      <c r="F47" s="29"/>
+      <c r="G47" s="29"/>
+      <c r="H47" s="29"/>
+      <c r="I47" s="29"/>
+      <c r="J47" s="29"/>
+      <c r="K47" s="29"/>
+      <c r="L47" s="29"/>
+      <c r="M47" s="29"/>
+      <c r="N47" s="22"/>
+      <c r="O47" s="22"/>
+      <c r="P47" s="93"/>
+    </row>
+    <row r="48" s="98" customFormat="true" ht="56.7" hidden="false" customHeight="true" outlineLevel="1" collapsed="false">
+      <c r="A48" s="33" t="s">
+        <v>102</v>
+      </c>
+      <c r="B48" s="33"/>
+      <c r="C48" s="33" t="s">
+        <v>103</v>
+      </c>
+      <c r="D48" s="33"/>
+      <c r="E48" s="30" t="s">
+        <v>104</v>
+      </c>
+      <c r="F48" s="30"/>
+      <c r="G48" s="30" t="s">
+        <v>105</v>
+      </c>
+      <c r="H48" s="30"/>
+      <c r="I48" s="30" t="s">
+        <v>106</v>
+      </c>
+      <c r="J48" s="30"/>
+      <c r="K48" s="30" t="s">
+        <v>107</v>
+      </c>
+      <c r="L48" s="30"/>
+      <c r="M48" s="30" t="s">
+        <v>108</v>
+      </c>
+      <c r="N48" s="30"/>
+      <c r="O48" s="30" t="s">
+        <v>109</v>
+      </c>
+      <c r="P48" s="30"/>
+      <c r="Q48" s="30" t="s">
+        <v>110</v>
+      </c>
+      <c r="R48" s="30"/>
+      <c r="S48" s="96"/>
+      <c r="T48" s="96"/>
+      <c r="U48" s="96"/>
+      <c r="V48" s="96"/>
+      <c r="W48" s="97"/>
+    </row>
+    <row r="49" s="15" customFormat="true" ht="17.1" hidden="false" customHeight="true" outlineLevel="1" collapsed="false">
+      <c r="A49" s="99" t="s">
         <v>66</v>
       </c>
-      <c r="N35" s="68"/>
-      <c r="O35" s="68"/>
-      <c r="P35" s="68"/>
-      <c r="Q35" s="66" t="s">
-        <v>67</v>
-      </c>
-      <c r="R35" s="66"/>
-    </row>
-    <row r="36" s="1" customFormat="true" ht="17.1" hidden="false" customHeight="true" outlineLevel="1" collapsed="false">
-      <c r="A36" s="47"/>
-      <c r="B36" s="47"/>
-      <c r="C36" s="47"/>
-      <c r="D36" s="47"/>
-      <c r="E36" s="47"/>
-      <c r="F36" s="47"/>
-      <c r="G36" s="47"/>
-      <c r="H36" s="69"/>
-      <c r="I36" s="70"/>
-      <c r="J36" s="70"/>
-      <c r="K36" s="47"/>
-      <c r="L36" s="47"/>
-      <c r="M36" s="47"/>
-      <c r="N36" s="47"/>
-      <c r="O36" s="71"/>
-      <c r="P36" s="70"/>
-      <c r="Q36" s="70"/>
-      <c r="R36" s="70"/>
-    </row>
-    <row r="37" s="16" customFormat="true" ht="17.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A37" s="29" t="s">
-        <v>68</v>
-      </c>
-      <c r="B37" s="29"/>
-      <c r="C37" s="29"/>
-      <c r="D37" s="29"/>
-      <c r="E37" s="72"/>
-      <c r="F37" s="72"/>
-      <c r="G37" s="72"/>
-      <c r="H37" s="54"/>
-      <c r="I37" s="73"/>
-      <c r="J37" s="74"/>
-      <c r="K37" s="27"/>
-      <c r="L37" s="27"/>
-      <c r="M37" s="27"/>
-      <c r="N37" s="27"/>
-      <c r="O37" s="27"/>
-      <c r="P37" s="27"/>
-    </row>
-    <row r="38" s="78" customFormat="true" ht="56.7" hidden="false" customHeight="true" outlineLevel="1" collapsed="false">
-      <c r="A38" s="61" t="s">
-        <v>69</v>
-      </c>
-      <c r="B38" s="61"/>
-      <c r="C38" s="61"/>
-      <c r="D38" s="75" t="s">
-        <v>70</v>
-      </c>
-      <c r="E38" s="75" t="s">
-        <v>71</v>
-      </c>
-      <c r="F38" s="75" t="s">
-        <v>72</v>
-      </c>
-      <c r="G38" s="75" t="s">
-        <v>73</v>
-      </c>
-      <c r="H38" s="76" t="s">
-        <v>74</v>
-      </c>
-      <c r="I38" s="76" t="s">
-        <v>75</v>
-      </c>
-      <c r="J38" s="76" t="s">
-        <v>76</v>
-      </c>
-      <c r="K38" s="61" t="s">
-        <v>77</v>
-      </c>
-      <c r="L38" s="61"/>
-      <c r="M38" s="61"/>
-      <c r="N38" s="62" t="s">
-        <v>62</v>
-      </c>
-      <c r="O38" s="62"/>
-      <c r="P38" s="77"/>
-      <c r="Q38" s="77" t="s">
-        <v>78</v>
-      </c>
-      <c r="R38" s="77"/>
-      <c r="S38" s="77"/>
-    </row>
-    <row r="39" s="78" customFormat="true" ht="29.7" hidden="false" customHeight="true" outlineLevel="1" collapsed="false">
-      <c r="A39" s="79" t="s">
-        <v>79</v>
-      </c>
-      <c r="B39" s="79"/>
-      <c r="C39" s="79"/>
-      <c r="D39" s="80" t="n">
-        <v>44210</v>
-      </c>
-      <c r="E39" s="81" t="n">
-        <v>2600</v>
-      </c>
-      <c r="F39" s="82" t="n">
-        <v>2.391</v>
-      </c>
-      <c r="G39" s="83" t="n">
-        <v>6216.6</v>
-      </c>
-      <c r="H39" s="84" t="n">
-        <v>6216.6</v>
-      </c>
-      <c r="I39" s="85" t="s">
-        <v>64</v>
-      </c>
-      <c r="J39" s="86" t="n">
-        <v>44223</v>
-      </c>
-      <c r="K39" s="79" t="s">
-        <v>80</v>
-      </c>
-      <c r="L39" s="79"/>
-      <c r="M39" s="79"/>
-      <c r="N39" s="66" t="s">
-        <v>67</v>
-      </c>
-      <c r="O39" s="66"/>
-      <c r="P39" s="77"/>
-      <c r="Q39" s="77"/>
-      <c r="R39" s="77"/>
-      <c r="S39" s="77"/>
-    </row>
-    <row r="40" s="91" customFormat="true" ht="13.2" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
-      <c r="A40" s="87"/>
-      <c r="B40" s="87"/>
-      <c r="C40" s="87"/>
-      <c r="D40" s="88"/>
-      <c r="E40" s="87"/>
-      <c r="F40" s="88"/>
-      <c r="G40" s="88"/>
-      <c r="H40" s="88"/>
-      <c r="I40" s="89"/>
-      <c r="J40" s="88"/>
-      <c r="K40" s="87"/>
-      <c r="L40" s="87"/>
-      <c r="M40" s="87"/>
-      <c r="N40" s="90"/>
-      <c r="O40" s="90"/>
-      <c r="P40" s="77"/>
-      <c r="Q40" s="77"/>
-      <c r="R40" s="77"/>
-    </row>
-    <row r="41" s="15" customFormat="true" ht="17.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A41" s="29" t="s">
-        <v>81</v>
-      </c>
-      <c r="B41" s="29"/>
-      <c r="C41" s="29"/>
-      <c r="D41" s="29"/>
-      <c r="E41" s="29"/>
-      <c r="F41" s="29"/>
-      <c r="G41" s="29"/>
-      <c r="H41" s="29"/>
-      <c r="I41" s="29"/>
-      <c r="J41" s="29"/>
-      <c r="K41" s="29"/>
-      <c r="L41" s="29"/>
-      <c r="M41" s="29"/>
-      <c r="N41" s="22"/>
-      <c r="O41" s="22"/>
-      <c r="P41" s="92"/>
-    </row>
-    <row r="42" s="15" customFormat="true" ht="43.2" hidden="false" customHeight="true" outlineLevel="1" collapsed="false">
-      <c r="A42" s="75" t="s">
-        <v>82</v>
-      </c>
-      <c r="B42" s="75"/>
-      <c r="C42" s="75"/>
-      <c r="D42" s="75" t="s">
-        <v>83</v>
-      </c>
-      <c r="E42" s="75"/>
-      <c r="F42" s="75" t="s">
-        <v>84</v>
-      </c>
-      <c r="G42" s="75"/>
-      <c r="H42" s="75" t="s">
-        <v>85</v>
-      </c>
-      <c r="I42" s="75"/>
-      <c r="J42" s="75" t="s">
-        <v>86</v>
-      </c>
-      <c r="K42" s="75"/>
-      <c r="L42" s="75" t="s">
-        <v>87</v>
-      </c>
-      <c r="M42" s="75"/>
-      <c r="N42" s="75" t="s">
-        <v>88</v>
-      </c>
-      <c r="O42" s="75"/>
-      <c r="P42" s="22"/>
-      <c r="Q42" s="22"/>
-      <c r="R42" s="92"/>
-    </row>
-    <row r="43" s="15" customFormat="true" ht="17.1" hidden="false" customHeight="true" outlineLevel="1" collapsed="false">
-      <c r="A43" s="85" t="s">
-        <v>89</v>
-      </c>
-      <c r="B43" s="85"/>
-      <c r="C43" s="85"/>
-      <c r="D43" s="85"/>
-      <c r="E43" s="85"/>
-      <c r="F43" s="85"/>
-      <c r="G43" s="85"/>
-      <c r="H43" s="93"/>
-      <c r="I43" s="93"/>
-      <c r="J43" s="85"/>
-      <c r="K43" s="85"/>
-      <c r="L43" s="85"/>
-      <c r="M43" s="85"/>
-      <c r="N43" s="85"/>
-      <c r="O43" s="85"/>
-      <c r="P43" s="22"/>
-      <c r="Q43" s="22"/>
-      <c r="R43" s="92"/>
-    </row>
-    <row r="44" s="50" customFormat="true" ht="17.1" hidden="false" customHeight="true" outlineLevel="1" collapsed="false">
-      <c r="A44" s="94"/>
-      <c r="B44" s="94"/>
-      <c r="C44" s="94"/>
-      <c r="D44" s="94"/>
-      <c r="E44" s="94"/>
-      <c r="F44" s="94"/>
-      <c r="G44" s="94"/>
-      <c r="H44" s="94"/>
-      <c r="I44" s="94"/>
-      <c r="J44" s="94"/>
-      <c r="K44" s="94"/>
-      <c r="L44" s="94"/>
-      <c r="M44" s="70"/>
-      <c r="N44" s="94"/>
-      <c r="O44" s="94"/>
-    </row>
-    <row r="45" s="15" customFormat="true" ht="17.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A45" s="29" t="s">
-        <v>90</v>
-      </c>
-      <c r="B45" s="29"/>
-      <c r="C45" s="29"/>
-      <c r="D45" s="29"/>
-      <c r="E45" s="29"/>
-      <c r="F45" s="29"/>
-      <c r="G45" s="29"/>
-      <c r="H45" s="29"/>
-      <c r="I45" s="29"/>
-      <c r="J45" s="29"/>
-      <c r="K45" s="29"/>
-      <c r="L45" s="29"/>
-      <c r="M45" s="29"/>
-      <c r="N45" s="22"/>
-      <c r="O45" s="22"/>
-      <c r="P45" s="92"/>
-    </row>
-    <row r="46" s="97" customFormat="true" ht="56.7" hidden="false" customHeight="true" outlineLevel="1" collapsed="false">
-      <c r="A46" s="33" t="s">
-        <v>91</v>
-      </c>
-      <c r="B46" s="33"/>
-      <c r="C46" s="33" t="s">
-        <v>92</v>
-      </c>
-      <c r="D46" s="33"/>
-      <c r="E46" s="30" t="s">
-        <v>93</v>
-      </c>
-      <c r="F46" s="30"/>
-      <c r="G46" s="30" t="s">
-        <v>94</v>
-      </c>
-      <c r="H46" s="30"/>
-      <c r="I46" s="30" t="s">
-        <v>95</v>
-      </c>
-      <c r="J46" s="30"/>
-      <c r="K46" s="30" t="s">
-        <v>96</v>
-      </c>
-      <c r="L46" s="30"/>
-      <c r="M46" s="30" t="s">
-        <v>97</v>
-      </c>
-      <c r="N46" s="30"/>
-      <c r="O46" s="30" t="s">
-        <v>98</v>
-      </c>
-      <c r="P46" s="30"/>
-      <c r="Q46" s="30" t="s">
-        <v>99</v>
-      </c>
-      <c r="R46" s="30"/>
-      <c r="S46" s="95"/>
-      <c r="T46" s="95"/>
-      <c r="U46" s="95"/>
-      <c r="V46" s="95"/>
-      <c r="W46" s="96"/>
-    </row>
-    <row r="47" s="15" customFormat="true" ht="17.1" hidden="false" customHeight="true" outlineLevel="1" collapsed="false">
-      <c r="A47" s="98" t="s">
-        <v>47</v>
-      </c>
-      <c r="B47" s="98"/>
-      <c r="C47" s="98"/>
-      <c r="D47" s="98"/>
-      <c r="E47" s="98"/>
-      <c r="F47" s="98"/>
-      <c r="G47" s="98"/>
-      <c r="H47" s="98"/>
-      <c r="I47" s="98"/>
-      <c r="J47" s="98"/>
-      <c r="K47" s="98"/>
-      <c r="L47" s="98"/>
-      <c r="M47" s="98"/>
-      <c r="N47" s="98"/>
-      <c r="O47" s="99"/>
-      <c r="P47" s="99"/>
-      <c r="Q47" s="99"/>
-      <c r="R47" s="99"/>
-      <c r="S47" s="22"/>
-      <c r="T47" s="22"/>
-      <c r="U47" s="22"/>
-      <c r="V47" s="22"/>
-      <c r="W47" s="92"/>
-    </row>
-    <row r="48" s="1" customFormat="true" ht="17.1" hidden="false" customHeight="true" outlineLevel="1" collapsed="false">
-      <c r="A48" s="48"/>
-      <c r="B48" s="48"/>
-      <c r="C48" s="48"/>
-      <c r="D48" s="48"/>
-      <c r="E48" s="48"/>
-      <c r="F48" s="48"/>
-      <c r="G48" s="48"/>
-      <c r="H48" s="48"/>
-      <c r="I48" s="48"/>
-      <c r="J48" s="48"/>
-      <c r="K48" s="48"/>
-      <c r="L48" s="48"/>
-      <c r="M48" s="48"/>
-      <c r="N48" s="70"/>
-      <c r="O48" s="48"/>
-      <c r="P48" s="48"/>
-      <c r="Q48" s="48"/>
-      <c r="R48" s="70"/>
-    </row>
-    <row r="49" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="100"/>
-      <c r="B49" s="100"/>
-      <c r="C49" s="100"/>
-      <c r="D49" s="100"/>
-      <c r="E49" s="100"/>
-      <c r="F49" s="22"/>
-      <c r="G49" s="22"/>
-      <c r="H49" s="22"/>
-      <c r="I49" s="22"/>
-      <c r="J49" s="22"/>
-      <c r="K49" s="22"/>
-      <c r="L49" s="22"/>
-      <c r="M49" s="22"/>
-    </row>
-    <row r="50" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="101"/>
-      <c r="B50" s="100"/>
-      <c r="C50" s="100"/>
-      <c r="D50" s="100"/>
-      <c r="E50" s="100"/>
-      <c r="F50" s="22"/>
-      <c r="G50" s="22"/>
-      <c r="H50" s="22"/>
-      <c r="I50" s="22"/>
-      <c r="J50" s="22"/>
-      <c r="K50" s="22"/>
-      <c r="L50" s="22"/>
-      <c r="M50" s="22"/>
-    </row>
-    <row r="51" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A51" s="102" t="s">
-        <v>100</v>
-      </c>
-      <c r="B51" s="102"/>
-      <c r="C51" s="102"/>
-      <c r="D51" s="102"/>
-      <c r="E51" s="102"/>
-      <c r="F51" s="102"/>
-      <c r="G51" s="102"/>
+      <c r="B49" s="99"/>
+      <c r="C49" s="99"/>
+      <c r="D49" s="99"/>
+      <c r="E49" s="99"/>
+      <c r="F49" s="99"/>
+      <c r="G49" s="99"/>
+      <c r="H49" s="99"/>
+      <c r="I49" s="99"/>
+      <c r="J49" s="99"/>
+      <c r="K49" s="99"/>
+      <c r="L49" s="99"/>
+      <c r="M49" s="99"/>
+      <c r="N49" s="99"/>
+      <c r="O49" s="100"/>
+      <c r="P49" s="100"/>
+      <c r="Q49" s="100"/>
+      <c r="R49" s="100"/>
+      <c r="S49" s="22"/>
+      <c r="T49" s="22"/>
+      <c r="U49" s="22"/>
+      <c r="V49" s="22"/>
+      <c r="W49" s="93"/>
+    </row>
+    <row r="50" s="1" customFormat="true" ht="17.1" hidden="false" customHeight="true" outlineLevel="1" collapsed="false">
+      <c r="A50" s="49"/>
+      <c r="B50" s="49"/>
+      <c r="C50" s="49"/>
+      <c r="D50" s="49"/>
+      <c r="E50" s="49"/>
+      <c r="F50" s="49"/>
+      <c r="G50" s="49"/>
+      <c r="H50" s="49"/>
+      <c r="I50" s="49"/>
+      <c r="J50" s="49"/>
+      <c r="K50" s="49"/>
+      <c r="L50" s="49"/>
+      <c r="M50" s="49"/>
+      <c r="N50" s="71"/>
+      <c r="O50" s="49"/>
+      <c r="P50" s="49"/>
+      <c r="Q50" s="49"/>
+      <c r="R50" s="71"/>
+    </row>
+    <row r="51" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="101"/>
+      <c r="B51" s="101"/>
+      <c r="C51" s="101"/>
+      <c r="D51" s="101"/>
+      <c r="E51" s="101"/>
+      <c r="F51" s="22"/>
+      <c r="G51" s="22"/>
       <c r="H51" s="22"/>
       <c r="I51" s="22"/>
       <c r="J51" s="22"/>
@@ -2590,16 +2826,12 @@
       <c r="L51" s="22"/>
       <c r="M51" s="22"/>
     </row>
-    <row r="52" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A52" s="103" t="s">
-        <v>101</v>
-      </c>
-      <c r="B52" s="103"/>
-      <c r="C52" s="103"/>
-      <c r="D52" s="14" t="s">
-        <v>102</v>
-      </c>
-      <c r="E52" s="14"/>
+    <row r="52" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="102"/>
+      <c r="B52" s="101"/>
+      <c r="C52" s="101"/>
+      <c r="D52" s="101"/>
+      <c r="E52" s="101"/>
       <c r="F52" s="22"/>
       <c r="G52" s="22"/>
       <c r="H52" s="22"/>
@@ -2609,8 +2841,44 @@
       <c r="L52" s="22"/>
       <c r="M52" s="22"/>
     </row>
+    <row r="53" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A53" s="103" t="s">
+        <v>111</v>
+      </c>
+      <c r="B53" s="103"/>
+      <c r="C53" s="103"/>
+      <c r="D53" s="103"/>
+      <c r="E53" s="103"/>
+      <c r="F53" s="103"/>
+      <c r="G53" s="103"/>
+      <c r="H53" s="22"/>
+      <c r="I53" s="22"/>
+      <c r="J53" s="22"/>
+      <c r="K53" s="22"/>
+      <c r="L53" s="22"/>
+      <c r="M53" s="22"/>
+    </row>
+    <row r="54" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A54" s="104" t="s">
+        <v>112</v>
+      </c>
+      <c r="B54" s="104"/>
+      <c r="C54" s="104"/>
+      <c r="D54" s="14" t="s">
+        <v>113</v>
+      </c>
+      <c r="E54" s="14"/>
+      <c r="F54" s="22"/>
+      <c r="G54" s="22"/>
+      <c r="H54" s="22"/>
+      <c r="I54" s="22"/>
+      <c r="J54" s="22"/>
+      <c r="K54" s="22"/>
+      <c r="L54" s="22"/>
+      <c r="M54" s="22"/>
+    </row>
   </sheetData>
-  <mergeCells count="90">
+  <mergeCells count="94">
     <mergeCell ref="A6:E6"/>
     <mergeCell ref="F6:W6"/>
     <mergeCell ref="A7:E7"/>
@@ -2635,72 +2903,76 @@
     <mergeCell ref="U25:V25"/>
     <mergeCell ref="A26:C26"/>
     <mergeCell ref="U26:V26"/>
-    <mergeCell ref="A29:D29"/>
-    <mergeCell ref="E29:H29"/>
-    <mergeCell ref="I29:L29"/>
-    <mergeCell ref="A30:B30"/>
-    <mergeCell ref="C30:D30"/>
-    <mergeCell ref="E30:F30"/>
-    <mergeCell ref="G30:H30"/>
-    <mergeCell ref="I30:J30"/>
-    <mergeCell ref="K30:L30"/>
-    <mergeCell ref="A31:B31"/>
-    <mergeCell ref="C31:D31"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="G31:H31"/>
-    <mergeCell ref="I31:J31"/>
-    <mergeCell ref="K31:L31"/>
-    <mergeCell ref="B34:F34"/>
-    <mergeCell ref="I34:L34"/>
-    <mergeCell ref="M34:P34"/>
-    <mergeCell ref="Q34:R34"/>
-    <mergeCell ref="B35:F35"/>
-    <mergeCell ref="I35:L35"/>
-    <mergeCell ref="M35:P35"/>
-    <mergeCell ref="Q35:R35"/>
-    <mergeCell ref="A38:C38"/>
-    <mergeCell ref="K38:M38"/>
-    <mergeCell ref="N38:O38"/>
-    <mergeCell ref="A39:C39"/>
-    <mergeCell ref="K39:M39"/>
-    <mergeCell ref="N39:O39"/>
-    <mergeCell ref="A42:C42"/>
-    <mergeCell ref="D42:E42"/>
-    <mergeCell ref="F42:G42"/>
-    <mergeCell ref="H42:I42"/>
-    <mergeCell ref="J42:K42"/>
-    <mergeCell ref="L42:M42"/>
-    <mergeCell ref="N42:O42"/>
-    <mergeCell ref="A43:C43"/>
-    <mergeCell ref="D43:E43"/>
-    <mergeCell ref="F43:G43"/>
-    <mergeCell ref="H43:I43"/>
-    <mergeCell ref="J43:K43"/>
-    <mergeCell ref="L43:M43"/>
-    <mergeCell ref="N43:O43"/>
+    <mergeCell ref="A27:C27"/>
+    <mergeCell ref="U27:V27"/>
+    <mergeCell ref="A28:C28"/>
+    <mergeCell ref="U28:V28"/>
+    <mergeCell ref="A31:D31"/>
+    <mergeCell ref="E31:H31"/>
+    <mergeCell ref="I31:L31"/>
+    <mergeCell ref="A32:B32"/>
+    <mergeCell ref="C32:D32"/>
+    <mergeCell ref="E32:F32"/>
+    <mergeCell ref="G32:H32"/>
+    <mergeCell ref="I32:J32"/>
+    <mergeCell ref="K32:L32"/>
+    <mergeCell ref="A33:B33"/>
+    <mergeCell ref="C33:D33"/>
+    <mergeCell ref="E33:F33"/>
+    <mergeCell ref="G33:H33"/>
+    <mergeCell ref="I33:J33"/>
+    <mergeCell ref="K33:L33"/>
+    <mergeCell ref="B36:F36"/>
+    <mergeCell ref="I36:L36"/>
+    <mergeCell ref="M36:P36"/>
+    <mergeCell ref="Q36:R36"/>
+    <mergeCell ref="B37:F37"/>
+    <mergeCell ref="I37:L37"/>
+    <mergeCell ref="M37:P37"/>
+    <mergeCell ref="Q37:R37"/>
+    <mergeCell ref="A40:C40"/>
+    <mergeCell ref="K40:M40"/>
+    <mergeCell ref="N40:O40"/>
+    <mergeCell ref="A41:C41"/>
+    <mergeCell ref="K41:M41"/>
+    <mergeCell ref="N41:O41"/>
+    <mergeCell ref="A44:C44"/>
+    <mergeCell ref="D44:E44"/>
+    <mergeCell ref="F44:G44"/>
+    <mergeCell ref="H44:I44"/>
     <mergeCell ref="J44:K44"/>
+    <mergeCell ref="L44:M44"/>
     <mergeCell ref="N44:O44"/>
-    <mergeCell ref="A46:B46"/>
-    <mergeCell ref="C46:D46"/>
-    <mergeCell ref="E46:F46"/>
-    <mergeCell ref="G46:H46"/>
-    <mergeCell ref="I46:J46"/>
-    <mergeCell ref="K46:L46"/>
-    <mergeCell ref="M46:N46"/>
-    <mergeCell ref="O46:P46"/>
-    <mergeCell ref="Q46:R46"/>
-    <mergeCell ref="A47:B47"/>
-    <mergeCell ref="C47:D47"/>
-    <mergeCell ref="E47:F47"/>
-    <mergeCell ref="G47:H47"/>
-    <mergeCell ref="I47:J47"/>
-    <mergeCell ref="K47:L47"/>
-    <mergeCell ref="M47:N47"/>
-    <mergeCell ref="O47:P47"/>
-    <mergeCell ref="Q47:R47"/>
-    <mergeCell ref="A51:G51"/>
-    <mergeCell ref="A52:C52"/>
-    <mergeCell ref="D52:E52"/>
+    <mergeCell ref="A45:C45"/>
+    <mergeCell ref="D45:E45"/>
+    <mergeCell ref="F45:G45"/>
+    <mergeCell ref="H45:I45"/>
+    <mergeCell ref="J45:K45"/>
+    <mergeCell ref="L45:M45"/>
+    <mergeCell ref="N45:O45"/>
+    <mergeCell ref="J46:K46"/>
+    <mergeCell ref="N46:O46"/>
+    <mergeCell ref="A48:B48"/>
+    <mergeCell ref="C48:D48"/>
+    <mergeCell ref="E48:F48"/>
+    <mergeCell ref="G48:H48"/>
+    <mergeCell ref="I48:J48"/>
+    <mergeCell ref="K48:L48"/>
+    <mergeCell ref="M48:N48"/>
+    <mergeCell ref="O48:P48"/>
+    <mergeCell ref="Q48:R48"/>
+    <mergeCell ref="A49:B49"/>
+    <mergeCell ref="C49:D49"/>
+    <mergeCell ref="E49:F49"/>
+    <mergeCell ref="G49:H49"/>
+    <mergeCell ref="I49:J49"/>
+    <mergeCell ref="K49:L49"/>
+    <mergeCell ref="M49:N49"/>
+    <mergeCell ref="O49:P49"/>
+    <mergeCell ref="Q49:R49"/>
+    <mergeCell ref="A53:G53"/>
+    <mergeCell ref="A54:C54"/>
+    <mergeCell ref="D54:E54"/>
   </mergeCells>
   <conditionalFormatting sqref="A13:AMJ21">
     <cfRule type="expression" priority="2" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
@@ -2710,117 +2982,117 @@
       <formula>$A13="Входящий остаток"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D26:F26">
+  <conditionalFormatting sqref="K41:K43">
     <cfRule type="expression" priority="4" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
+      <formula>MOD(ROUND($K43,2),1)&lt;&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J29:J35">
+    <cfRule type="expression" priority="5" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
+      <formula>MOD(ROUND($J35,2),1)&lt;&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J31:J35">
+    <cfRule type="expression" priority="6" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="4">
+      <formula>MOD(ROUND($J35,2),1)&lt;&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J31:J35">
+    <cfRule type="expression" priority="7" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="5">
+      <formula>MOD(ROUND($J35,2),1)&lt;&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D29:F30">
+    <cfRule type="expression" priority="8" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="6">
+      <formula>MOD(ROUND($F30,2),1)&lt;&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G29:G30">
+    <cfRule type="expression" priority="9" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7">
+      <formula>MOD(ROUND($G30,2),1)&lt;&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H29:H30">
+    <cfRule type="expression" priority="10" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="8">
+      <formula>MOD(ROUND($H30,2),1)&lt;&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I29:I30">
+    <cfRule type="expression" priority="11" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="9">
+      <formula>MOD(ROUND($I30,2),1)&lt;&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J29:J30">
+    <cfRule type="expression" priority="12" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="10">
+      <formula>MOD(ROUND($J30,2),1)&lt;&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K29:K30">
+    <cfRule type="expression" priority="13" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="11">
+      <formula>MOD(ROUND($K30,2),1)&lt;&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J30:J35">
+    <cfRule type="expression" priority="14" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="12">
+      <formula>MOD(ROUND($J35,2),1)&lt;&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J32:J35">
+    <cfRule type="expression" priority="15" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="13">
+      <formula>MOD(ROUND($J35,2),1)&lt;&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J32:J35">
+    <cfRule type="expression" priority="16" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="14">
+      <formula>MOD(ROUND($J35,2),1)&lt;&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F29:W35">
+    <cfRule type="expression" priority="17" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="15">
+      <formula>$F35="Оборот / Итого"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F30:X35">
+    <cfRule type="expression" priority="18" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="16">
+      <formula>$F35="Оборот / Итого"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K42:K43">
+    <cfRule type="expression" priority="19" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="17">
+      <formula>MOD(ROUND($K43,2),1)&lt;&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D26:F28">
+    <cfRule type="expression" priority="20" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="18">
       <formula>MOD(ROUND($F26,2),1)&lt;&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G26">
-    <cfRule type="expression" priority="5" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
+  <conditionalFormatting sqref="G26:G28">
+    <cfRule type="expression" priority="21" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="19">
       <formula>MOD(ROUND($G26,2),1)&lt;&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I26">
-    <cfRule type="expression" priority="6" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="4">
+  <conditionalFormatting sqref="I26:I28">
+    <cfRule type="expression" priority="22" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="20">
       <formula>MOD(ROUND($I26,2),1)&lt;&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J26">
-    <cfRule type="expression" priority="7" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="5">
+  <conditionalFormatting sqref="J26:J28">
+    <cfRule type="expression" priority="23" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="21">
       <formula>MOD(ROUND($J26,2),1)&lt;&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K26">
-    <cfRule type="expression" priority="8" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="6">
+  <conditionalFormatting sqref="K26:K28">
+    <cfRule type="expression" priority="24" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="22">
       <formula>MOD(ROUND($K26,2),1)&lt;&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L26">
-    <cfRule type="expression" priority="9" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7">
+  <conditionalFormatting sqref="L26:L28">
+    <cfRule type="expression" priority="25" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="23">
       <formula>MOD(ROUND($L26,2),1)&lt;&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K39:K41">
-    <cfRule type="expression" priority="10" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="8">
-      <formula>MOD(ROUND($K41,2),1)&lt;&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J27:J33">
-    <cfRule type="expression" priority="11" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="9">
-      <formula>MOD(ROUND($J33,2),1)&lt;&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J29:J33">
-    <cfRule type="expression" priority="12" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="10">
-      <formula>MOD(ROUND($J33,2),1)&lt;&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J29:J33">
-    <cfRule type="expression" priority="13" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="11">
-      <formula>MOD(ROUND($J33,2),1)&lt;&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D27:F28">
-    <cfRule type="expression" priority="14" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="12">
-      <formula>MOD(ROUND($F28,2),1)&lt;&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G27:G28">
-    <cfRule type="expression" priority="15" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="13">
-      <formula>MOD(ROUND($G28,2),1)&lt;&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H27:H28">
-    <cfRule type="expression" priority="16" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="14">
-      <formula>MOD(ROUND($H28,2),1)&lt;&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I27:I28">
-    <cfRule type="expression" priority="17" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="15">
-      <formula>MOD(ROUND($I28,2),1)&lt;&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J27:J28">
-    <cfRule type="expression" priority="18" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="16">
-      <formula>MOD(ROUND($J28,2),1)&lt;&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K27:K28">
-    <cfRule type="expression" priority="19" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="17">
-      <formula>MOD(ROUND($K28,2),1)&lt;&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J28:J33">
-    <cfRule type="expression" priority="20" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="18">
-      <formula>MOD(ROUND($J33,2),1)&lt;&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J30:J33">
-    <cfRule type="expression" priority="21" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="19">
-      <formula>MOD(ROUND($J33,2),1)&lt;&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J30:J33">
-    <cfRule type="expression" priority="22" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="20">
-      <formula>MOD(ROUND($J33,2),1)&lt;&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F27:W33">
-    <cfRule type="expression" priority="23" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="21">
-      <formula>$F33="Оборот / Итого"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F28:X33">
-    <cfRule type="expression" priority="24" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="22">
-      <formula>$F33="Оборот / Итого"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K40:K41">
-    <cfRule type="expression" priority="25" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="23">
-      <formula>MOD(ROUND($K41,2),1)&lt;&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H26">
+  <conditionalFormatting sqref="H26:H28">
     <cfRule type="expression" priority="26" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="24">
       <formula>MOD(ROUND($H26,2),1)&lt;&gt;0</formula>
     </cfRule>
@@ -2843,7 +3115,7 @@
   </sheetPr>
   <dimension ref="A1:V32"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="U27" activeCellId="0" sqref="U27"/>
     </sheetView>
   </sheetViews>
@@ -2880,136 +3152,136 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="104" t="s">
-        <v>103</v>
-      </c>
-      <c r="V1" s="105" t="s">
-        <v>104</v>
+      <c r="A1" s="105" t="s">
+        <v>114</v>
+      </c>
+      <c r="V1" s="106" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="V2" s="105" t="s">
-        <v>105</v>
+      <c r="V2" s="106" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="V3" s="105" t="s">
-        <v>106</v>
+      <c r="V3" s="106" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="V4" s="105" t="s">
-        <v>107</v>
+      <c r="V4" s="106" t="s">
+        <v>118</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="V5" s="105" t="s">
-        <v>108</v>
+      <c r="V5" s="106" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="V6" s="105" t="s">
-        <v>109</v>
+      <c r="V6" s="106" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="V7" s="105" t="s">
-        <v>110</v>
+      <c r="V7" s="106" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="V8" s="105" t="s">
-        <v>111</v>
+      <c r="V8" s="106" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="V9" s="105" t="s">
-        <v>112</v>
+      <c r="V9" s="106" t="s">
+        <v>123</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="V10" s="105" t="s">
-        <v>113</v>
+      <c r="V10" s="106" t="s">
+        <v>124</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="V11" s="105" t="s">
-        <v>114</v>
+      <c r="V11" s="106" t="s">
+        <v>125</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="V12" s="105" t="s">
-        <v>115</v>
+      <c r="V12" s="106" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="V13" s="105" t="s">
-        <v>116</v>
+      <c r="V13" s="106" t="s">
+        <v>127</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="V14" s="105" t="s">
-        <v>117</v>
+      <c r="V14" s="106" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="V15" s="105" t="s">
-        <v>118</v>
+      <c r="V15" s="106" t="s">
+        <v>129</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="V16" s="105" t="s">
-        <v>119</v>
+      <c r="V16" s="106" t="s">
+        <v>130</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="V17" s="105" t="s">
-        <v>120</v>
+      <c r="V17" s="106" t="s">
+        <v>131</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="V18" s="105" t="s">
-        <v>121</v>
+      <c r="V18" s="106" t="s">
+        <v>132</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="105"/>
+      <c r="A20" s="106"/>
     </row>
     <row r="21" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="105"/>
+      <c r="A21" s="106"/>
     </row>
     <row r="22" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="105"/>
+      <c r="A22" s="106"/>
     </row>
     <row r="23" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="105"/>
+      <c r="A23" s="106"/>
     </row>
     <row r="24" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="105"/>
+      <c r="A24" s="106"/>
     </row>
     <row r="25" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="105"/>
+      <c r="A25" s="106"/>
     </row>
     <row r="26" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="105"/>
+      <c r="A26" s="106"/>
     </row>
     <row r="27" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="105"/>
+      <c r="A27" s="106"/>
     </row>
     <row r="28" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="105"/>
+      <c r="A28" s="106"/>
     </row>
     <row r="29" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="105"/>
+      <c r="A29" s="106"/>
     </row>
     <row r="30" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="105"/>
+      <c r="A30" s="106"/>
     </row>
     <row r="31" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="105"/>
+      <c r="A31" s="106"/>
     </row>
     <row r="32" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="105"/>
+      <c r="A32" s="106"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
Class UralsibCapital was replaced with StatementUKFU (based on StatementXLS) in order to load statements via intermediate JSON validation. Test set was updated.
</commit_message>
<xml_diff>
--- a/tests/test_data/kit.xlsx
+++ b/tests/test_data/kit.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="170">
   <si>
     <t xml:space="preserve">КИТ Финанс (АО)</t>
   </si>
@@ -231,15 +231,155 @@
     <t xml:space="preserve">xxx</t>
   </si>
   <si>
+    <t xml:space="preserve">Заключенные сделки с ценными бумагами</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Номер
+сделки</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Номер
+заявки</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Дата сделки</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Время сделки</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Место
+совершения
+сделки</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Наименование
+ЦБ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Тип операции</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Количество</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Цена сделки </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> НКД</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Сумма сделки</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Валюта
+заключения
+сделки</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Сумма оплаты</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Валюта
+оплаты
+сделки</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Дата поставки
+(план.)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Дата оплаты
+(план.)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Комиссия
+брокера</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Валюта
+комиссии
+брокера</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Дата
+списания
+комиссии
+брокера</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Комиссия
+ТС</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Валюта
+комиссии
+ТС</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Дата
+списания
+комиссии
+ТС</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Примечание</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Контрагент</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ставка РЕПО</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Дата обратной сделки РЕПО</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3312348787</t>
+  </si>
+  <si>
+    <t xml:space="preserve">21596123101</t>
+  </si>
+  <si>
+    <t xml:space="preserve">15:00:20</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ММВБT+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Покупка</t>
+  </si>
+  <si>
+    <t xml:space="preserve">15:38:08</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ТинькоффБ7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10:28:43</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Продажа</t>
+  </si>
+  <si>
+    <t xml:space="preserve">14:59:57</t>
+  </si>
+  <si>
+    <t xml:space="preserve">POLYMETAL INTL PLC, Polymetal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">JE00B6T5S470</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Оборот / Итого</t>
+  </si>
+  <si>
     <t xml:space="preserve">Движение денежных средств по неторговым операциям</t>
   </si>
   <si>
     <t xml:space="preserve">Дата</t>
   </si>
   <si>
-    <t xml:space="preserve">Тип операции</t>
-  </si>
-  <si>
     <t xml:space="preserve">Сумма</t>
   </si>
   <si>
@@ -247,9 +387,6 @@
   </si>
   <si>
     <t xml:space="preserve">Основание</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Примечание</t>
   </si>
   <si>
     <t xml:space="preserve">Секция</t>
@@ -311,10 +448,6 @@
   </si>
   <si>
     <t xml:space="preserve">Ставки риска для ценных бумаг, принимаемых в обеспечение</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Наименование
-ЦБ</t>
   </si>
   <si>
     <t xml:space="preserve">Количество ЦБ с
@@ -457,7 +590,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="14">
+  <numFmts count="15">
     <numFmt numFmtId="164" formatCode="#,##0.0##########"/>
     <numFmt numFmtId="165" formatCode="General"/>
     <numFmt numFmtId="166" formatCode="@"/>
@@ -469,9 +602,10 @@
     <numFmt numFmtId="172" formatCode="#,##0"/>
     <numFmt numFmtId="173" formatCode="#,##0.00_ ;\-#,##0.00\ "/>
     <numFmt numFmtId="174" formatCode="m/d/yyyy"/>
-    <numFmt numFmtId="175" formatCode="#,##0.00#######;\-#,##0.00#######;0"/>
-    <numFmt numFmtId="176" formatCode="#,##0.0000"/>
-    <numFmt numFmtId="177" formatCode="0000"/>
+    <numFmt numFmtId="175" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
+    <numFmt numFmtId="176" formatCode="#,##0.00#######;\-#,##0.00#######;0"/>
+    <numFmt numFmtId="177" formatCode="#,##0.0000"/>
+    <numFmt numFmtId="178" formatCode="0000"/>
   </numFmts>
   <fonts count="15">
     <font>
@@ -596,7 +730,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="17">
+  <borders count="19">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -723,6 +857,24 @@
       <diagonal/>
     </border>
     <border diagonalUp="false" diagonalDown="false">
+      <left/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="FFA6A6A6"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="thin"/>
+      <right style="hair"/>
+      <top style="thin">
+        <color rgb="FFA6A6A6"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
       <left style="thin"/>
       <right/>
       <top style="thin"/>
@@ -770,7 +922,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="107">
+  <cellXfs count="118">
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1015,7 +1167,71 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="true"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="5" fillId="3" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="167" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="174" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="175" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="173" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="11" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="174" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="16" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="5" fillId="3" borderId="17" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1027,15 +1243,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="174" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="175" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="176" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1047,18 +1255,10 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="165" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="165" fontId="12" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1103,11 +1303,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="175" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="176" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1143,7 +1339,7 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="176" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="177" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1159,7 +1355,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="176" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="177" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1167,7 +1363,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="169" fontId="5" fillId="0" borderId="16" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="169" fontId="5" fillId="0" borderId="18" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1195,7 +1391,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1209,7 +1405,7 @@
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
     <cellStyle name="Обычный 2" xfId="20"/>
   </cellStyles>
-  <dxfs count="25">
+  <dxfs count="31">
     <dxf>
       <font>
         <b val="1"/>
@@ -1346,6 +1542,68 @@
       </font>
       <numFmt numFmtId="164" formatCode="#,##0.0##########"/>
     </dxf>
+    <dxf>
+      <font>
+        <name val="Calibri"/>
+        <charset val="204"/>
+        <family val="2"/>
+        <color rgb="FF000000"/>
+        <sz val="11"/>
+      </font>
+      <numFmt numFmtId="164" formatCode="#,##0.0##########"/>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="Calibri"/>
+        <charset val="204"/>
+        <family val="2"/>
+        <color rgb="FF000000"/>
+        <sz val="11"/>
+      </font>
+      <numFmt numFmtId="164" formatCode="#,##0.0##########"/>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="Calibri"/>
+        <charset val="204"/>
+        <family val="2"/>
+        <color rgb="FF000000"/>
+        <sz val="11"/>
+      </font>
+      <numFmt numFmtId="164" formatCode="#,##0.0##########"/>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="Calibri"/>
+        <charset val="204"/>
+        <family val="2"/>
+        <color rgb="FF000000"/>
+        <sz val="11"/>
+      </font>
+      <numFmt numFmtId="164" formatCode="#,##0.0##########"/>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="Calibri"/>
+        <charset val="204"/>
+        <family val="2"/>
+        <b val="1"/>
+        <i val="0"/>
+        <color rgb="FF000000"/>
+        <sz val="11"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="Calibri"/>
+        <charset val="204"/>
+        <family val="2"/>
+        <b val="1"/>
+        <i val="0"/>
+        <color rgb="FF000000"/>
+        <sz val="11"/>
+      </font>
+    </dxf>
   </dxfs>
   <colors>
     <indexedColors>
@@ -1421,9 +1679,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>203040</xdr:colOff>
+      <xdr:colOff>202320</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>20160</xdr:rowOff>
+      <xdr:rowOff>19440</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1437,7 +1695,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="2741760" cy="690480"/>
+          <a:ext cx="2741040" cy="689760"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1457,10 +1715,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="true"/>
   </sheetPr>
-  <dimension ref="A1:AC54"/>
+  <dimension ref="A1:AD63"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E29" activeCellId="0" sqref="E29"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="M19" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="V41" activeCellId="0" sqref="V41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="1" outlineLevelCol="0"/>
@@ -2379,7 +2637,7 @@
       <c r="V34" s="28"/>
       <c r="W34" s="59"/>
     </row>
-    <row r="35" s="16" customFormat="true" ht="17.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="35" s="16" customFormat="true" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A35" s="29" t="s">
         <v>67</v>
       </c>
@@ -2396,489 +2654,1004 @@
       <c r="L35" s="29"/>
       <c r="M35" s="29"/>
     </row>
-    <row r="36" s="64" customFormat="true" ht="15.3" hidden="false" customHeight="true" outlineLevel="1" collapsed="false">
+    <row r="36" s="61" customFormat="true" ht="56.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A36" s="30" t="s">
         <v>68</v>
       </c>
-      <c r="B36" s="61" t="s">
+      <c r="B36" s="30" t="s">
         <v>69</v>
       </c>
-      <c r="C36" s="61"/>
-      <c r="D36" s="61"/>
-      <c r="E36" s="61"/>
-      <c r="F36" s="61"/>
-      <c r="G36" s="30" t="s">
+      <c r="C36" s="30" t="s">
         <v>70</v>
       </c>
+      <c r="D36" s="30" t="s">
+        <v>71</v>
+      </c>
+      <c r="E36" s="30" t="s">
+        <v>72</v>
+      </c>
+      <c r="F36" s="30" t="s">
+        <v>73</v>
+      </c>
+      <c r="G36" s="30"/>
       <c r="H36" s="30" t="s">
-        <v>71</v>
+        <v>27</v>
       </c>
       <c r="I36" s="30" t="s">
-        <v>72</v>
-      </c>
-      <c r="J36" s="30"/>
-      <c r="K36" s="30"/>
-      <c r="L36" s="30"/>
-      <c r="M36" s="62" t="s">
+        <v>74</v>
+      </c>
+      <c r="J36" s="30" t="s">
+        <v>75</v>
+      </c>
+      <c r="K36" s="30" t="s">
+        <v>76</v>
+      </c>
+      <c r="L36" s="30" t="s">
+        <v>77</v>
+      </c>
+      <c r="M36" s="30" t="s">
+        <v>78</v>
+      </c>
+      <c r="N36" s="33" t="s">
+        <v>79</v>
+      </c>
+      <c r="O36" s="33" t="s">
+        <v>80</v>
+      </c>
+      <c r="P36" s="33" t="s">
+        <v>81</v>
+      </c>
+      <c r="Q36" s="33" t="s">
+        <v>82</v>
+      </c>
+      <c r="R36" s="33" t="s">
+        <v>83</v>
+      </c>
+      <c r="S36" s="33" t="s">
+        <v>84</v>
+      </c>
+      <c r="T36" s="31" t="s">
+        <v>85</v>
+      </c>
+      <c r="U36" s="33" t="s">
+        <v>86</v>
+      </c>
+      <c r="V36" s="33" t="s">
+        <v>87</v>
+      </c>
+      <c r="W36" s="33" t="s">
+        <v>88</v>
+      </c>
+      <c r="X36" s="33" t="s">
+        <v>89</v>
+      </c>
+      <c r="Y36" s="33" t="s">
+        <v>90</v>
+      </c>
+      <c r="Z36" s="33" t="s">
+        <v>91</v>
+      </c>
+      <c r="AA36" s="33" t="s">
+        <v>92</v>
+      </c>
+      <c r="AB36" s="33" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="15.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A37" s="62" t="s">
+        <v>94</v>
+      </c>
+      <c r="B37" s="63" t="s">
+        <v>95</v>
+      </c>
+      <c r="C37" s="64" t="n">
+        <v>44268</v>
+      </c>
+      <c r="D37" s="65" t="s">
+        <v>96</v>
+      </c>
+      <c r="E37" s="66" t="s">
+        <v>97</v>
+      </c>
+      <c r="F37" s="67" t="s">
+        <v>52</v>
+      </c>
+      <c r="G37" s="67"/>
+      <c r="H37" s="62" t="s">
+        <v>53</v>
+      </c>
+      <c r="I37" s="36" t="s">
+        <v>98</v>
+      </c>
+      <c r="J37" s="37" t="n">
+        <v>10</v>
+      </c>
+      <c r="K37" s="66" t="n">
+        <v>987.65</v>
+      </c>
+      <c r="L37" s="66" t="n">
+        <v>0</v>
+      </c>
+      <c r="M37" s="68" t="n">
+        <v>-9876.5</v>
+      </c>
+      <c r="N37" s="62" t="s">
+        <v>50</v>
+      </c>
+      <c r="O37" s="68" t="n">
+        <v>-9876.5</v>
+      </c>
+      <c r="P37" s="62" t="s">
+        <v>50</v>
+      </c>
+      <c r="Q37" s="64" t="n">
+        <v>44270</v>
+      </c>
+      <c r="R37" s="64" t="n">
+        <v>44270</v>
+      </c>
+      <c r="S37" s="66" t="n">
+        <v>-5.67</v>
+      </c>
+      <c r="T37" s="69" t="s">
+        <v>50</v>
+      </c>
+      <c r="U37" s="64" t="n">
+        <v>44130</v>
+      </c>
+      <c r="V37" s="66" t="n">
+        <v>-1.23</v>
+      </c>
+      <c r="W37" s="66" t="s">
+        <v>50</v>
+      </c>
+      <c r="X37" s="64" t="n">
+        <v>44130</v>
+      </c>
+      <c r="Y37" s="70"/>
+      <c r="Z37" s="71"/>
+      <c r="AA37" s="71"/>
+      <c r="AB37" s="72"/>
+    </row>
+    <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A38" s="62" t="n">
+        <v>3720000652</v>
+      </c>
+      <c r="B38" s="63" t="n">
+        <v>23180041234</v>
+      </c>
+      <c r="C38" s="64" t="n">
+        <v>44271</v>
+      </c>
+      <c r="D38" s="65" t="s">
+        <v>99</v>
+      </c>
+      <c r="E38" s="66" t="s">
+        <v>97</v>
+      </c>
+      <c r="F38" s="67" t="s">
+        <v>100</v>
+      </c>
+      <c r="G38" s="67"/>
+      <c r="H38" s="62" t="s">
+        <v>57</v>
+      </c>
+      <c r="I38" s="36" t="s">
+        <v>98</v>
+      </c>
+      <c r="J38" s="37" t="n">
+        <v>1</v>
+      </c>
+      <c r="K38" s="66" t="n">
+        <v>100.57</v>
+      </c>
+      <c r="L38" s="66" t="n">
+        <v>16.83</v>
+      </c>
+      <c r="M38" s="68" t="n">
+        <v>-1005.7</v>
+      </c>
+      <c r="N38" s="62" t="s">
+        <v>50</v>
+      </c>
+      <c r="O38" s="68" t="n">
+        <v>-1005.7</v>
+      </c>
+      <c r="P38" s="62" t="s">
+        <v>50</v>
+      </c>
+      <c r="Q38" s="64" t="n">
+        <v>44272</v>
+      </c>
+      <c r="R38" s="64" t="n">
+        <v>44272</v>
+      </c>
+      <c r="S38" s="66" t="n">
+        <v>-0.4</v>
+      </c>
+      <c r="T38" s="69" t="s">
+        <v>50</v>
+      </c>
+      <c r="U38" s="64" t="n">
+        <v>44271</v>
+      </c>
+      <c r="V38" s="66" t="n">
+        <v>-0.1</v>
+      </c>
+      <c r="W38" s="66" t="s">
+        <v>50</v>
+      </c>
+      <c r="X38" s="64" t="n">
+        <v>44271</v>
+      </c>
+      <c r="Y38" s="70"/>
+      <c r="Z38" s="71"/>
+      <c r="AA38" s="71"/>
+      <c r="AB38" s="72"/>
+    </row>
+    <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A39" s="62" t="n">
+        <v>3725000743</v>
+      </c>
+      <c r="B39" s="63" t="n">
+        <v>23191928765</v>
+      </c>
+      <c r="C39" s="64" t="n">
+        <v>44272</v>
+      </c>
+      <c r="D39" s="65" t="s">
+        <v>101</v>
+      </c>
+      <c r="E39" s="66" t="s">
+        <v>97</v>
+      </c>
+      <c r="F39" s="67" t="s">
+        <v>100</v>
+      </c>
+      <c r="G39" s="67"/>
+      <c r="H39" s="62" t="s">
+        <v>57</v>
+      </c>
+      <c r="I39" s="36" t="s">
+        <v>102</v>
+      </c>
+      <c r="J39" s="37" t="n">
+        <v>1</v>
+      </c>
+      <c r="K39" s="66" t="n">
+        <v>100.41</v>
+      </c>
+      <c r="L39" s="66" t="n">
+        <v>17.03</v>
+      </c>
+      <c r="M39" s="68" t="n">
+        <v>1004.1</v>
+      </c>
+      <c r="N39" s="62" t="s">
+        <v>50</v>
+      </c>
+      <c r="O39" s="68" t="n">
+        <v>1004.1</v>
+      </c>
+      <c r="P39" s="62" t="s">
+        <v>50</v>
+      </c>
+      <c r="Q39" s="64" t="n">
+        <v>44273</v>
+      </c>
+      <c r="R39" s="64" t="n">
+        <v>44273</v>
+      </c>
+      <c r="S39" s="66" t="n">
+        <v>-0.4</v>
+      </c>
+      <c r="T39" s="69" t="s">
+        <v>50</v>
+      </c>
+      <c r="U39" s="64" t="n">
+        <v>44272</v>
+      </c>
+      <c r="V39" s="66" t="n">
+        <v>-0.1</v>
+      </c>
+      <c r="W39" s="66" t="s">
+        <v>50</v>
+      </c>
+      <c r="X39" s="64" t="n">
+        <v>44272</v>
+      </c>
+      <c r="Y39" s="70"/>
+      <c r="Z39" s="71"/>
+      <c r="AA39" s="71"/>
+      <c r="AB39" s="72"/>
+    </row>
+    <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A40" s="62" t="n">
+        <v>3720123978</v>
+      </c>
+      <c r="B40" s="63" t="n">
+        <v>23179999690</v>
+      </c>
+      <c r="C40" s="64" t="n">
+        <v>44281</v>
+      </c>
+      <c r="D40" s="65" t="s">
+        <v>103</v>
+      </c>
+      <c r="E40" s="66" t="s">
+        <v>97</v>
+      </c>
+      <c r="F40" s="73" t="s">
+        <v>104</v>
+      </c>
+      <c r="G40" s="73"/>
+      <c r="H40" s="62" t="s">
+        <v>105</v>
+      </c>
+      <c r="I40" s="36" t="s">
+        <v>98</v>
+      </c>
+      <c r="J40" s="37" t="n">
+        <v>10</v>
+      </c>
+      <c r="K40" s="66" t="n">
+        <v>1532.1</v>
+      </c>
+      <c r="L40" s="66" t="n">
+        <v>0</v>
+      </c>
+      <c r="M40" s="68" t="n">
+        <v>15321</v>
+      </c>
+      <c r="N40" s="62" t="s">
+        <v>50</v>
+      </c>
+      <c r="O40" s="68" t="n">
+        <v>-15321</v>
+      </c>
+      <c r="P40" s="62" t="s">
+        <v>50</v>
+      </c>
+      <c r="Q40" s="64" t="n">
+        <v>44283</v>
+      </c>
+      <c r="R40" s="64" t="n">
+        <v>44283</v>
+      </c>
+      <c r="S40" s="66" t="n">
+        <v>-7.11</v>
+      </c>
+      <c r="T40" s="69" t="s">
+        <v>50</v>
+      </c>
+      <c r="U40" s="64" t="n">
+        <v>44281</v>
+      </c>
+      <c r="V40" s="66" t="n">
+        <v>-1.55</v>
+      </c>
+      <c r="W40" s="66" t="s">
+        <v>50</v>
+      </c>
+      <c r="X40" s="64" t="n">
+        <v>44281</v>
+      </c>
+      <c r="Y40" s="70"/>
+      <c r="Z40" s="71"/>
+      <c r="AA40" s="71"/>
+      <c r="AB40" s="72"/>
+    </row>
+    <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="62"/>
+      <c r="B41" s="63"/>
+      <c r="C41" s="64"/>
+      <c r="D41" s="65"/>
+      <c r="E41" s="66"/>
+      <c r="F41" s="74"/>
+      <c r="G41" s="74"/>
+      <c r="H41" s="62"/>
+      <c r="I41" s="36"/>
+      <c r="J41" s="37"/>
+      <c r="K41" s="66"/>
+      <c r="L41" s="66"/>
+      <c r="M41" s="68"/>
+      <c r="N41" s="62"/>
+      <c r="O41" s="68"/>
+      <c r="P41" s="62"/>
+      <c r="Q41" s="64"/>
+      <c r="R41" s="64"/>
+      <c r="S41" s="66"/>
+      <c r="T41" s="69"/>
+      <c r="U41" s="64"/>
+      <c r="V41" s="66"/>
+      <c r="W41" s="66"/>
+      <c r="X41" s="64"/>
+      <c r="Y41" s="70"/>
+      <c r="Z41" s="71"/>
+      <c r="AA41" s="71"/>
+      <c r="AB41" s="72"/>
+    </row>
+    <row r="42" customFormat="false" ht="15.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A42" s="62"/>
+      <c r="B42" s="63"/>
+      <c r="C42" s="64"/>
+      <c r="D42" s="65"/>
+      <c r="E42" s="66"/>
+      <c r="F42" s="67" t="s">
+        <v>106</v>
+      </c>
+      <c r="G42" s="67"/>
+      <c r="H42" s="62"/>
+      <c r="I42" s="36"/>
+      <c r="J42" s="37"/>
+      <c r="K42" s="66"/>
+      <c r="L42" s="66"/>
+      <c r="M42" s="68" t="n">
+        <v>9878.1</v>
+      </c>
+      <c r="N42" s="62" t="s">
+        <v>50</v>
+      </c>
+      <c r="O42" s="68" t="n">
+        <v>9878.1</v>
+      </c>
+      <c r="P42" s="62" t="s">
+        <v>50</v>
+      </c>
+      <c r="Q42" s="64"/>
+      <c r="R42" s="64"/>
+      <c r="S42" s="66" t="n">
+        <v>6.47</v>
+      </c>
+      <c r="T42" s="69" t="s">
+        <v>50</v>
+      </c>
+      <c r="U42" s="64"/>
+      <c r="V42" s="66" t="n">
+        <v>1.43</v>
+      </c>
+      <c r="W42" s="66" t="s">
+        <v>50</v>
+      </c>
+      <c r="X42" s="64"/>
+      <c r="Y42" s="70"/>
+      <c r="Z42" s="71"/>
+      <c r="AA42" s="71"/>
+      <c r="AB42" s="72"/>
+    </row>
+    <row r="43" s="1" customFormat="true" ht="17.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A43" s="75"/>
+      <c r="B43" s="75"/>
+      <c r="C43" s="75"/>
+      <c r="D43" s="75"/>
+      <c r="E43" s="75"/>
+      <c r="F43" s="75"/>
+      <c r="G43" s="75"/>
+      <c r="H43" s="75"/>
+      <c r="I43" s="48"/>
+      <c r="J43" s="48"/>
+      <c r="K43" s="75"/>
+      <c r="L43" s="75"/>
+      <c r="M43" s="75"/>
+      <c r="N43" s="75"/>
+      <c r="O43" s="48"/>
+      <c r="P43" s="75"/>
+      <c r="Q43" s="48"/>
+      <c r="R43" s="48"/>
+      <c r="S43" s="48"/>
+      <c r="T43" s="75"/>
+      <c r="U43" s="76"/>
+      <c r="V43" s="48"/>
+      <c r="W43" s="75"/>
+      <c r="X43" s="75"/>
+      <c r="Y43" s="75"/>
+      <c r="Z43" s="48"/>
+      <c r="AA43" s="48"/>
+      <c r="AB43" s="75"/>
+      <c r="AC43" s="51"/>
+      <c r="AD43" s="51"/>
+    </row>
+    <row r="44" s="16" customFormat="true" ht="17.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A44" s="29" t="s">
+        <v>107</v>
+      </c>
+      <c r="B44" s="29"/>
+      <c r="C44" s="29"/>
+      <c r="D44" s="29"/>
+      <c r="E44" s="29"/>
+      <c r="F44" s="29"/>
+      <c r="G44" s="29"/>
+      <c r="H44" s="29"/>
+      <c r="I44" s="29"/>
+      <c r="J44" s="29"/>
+      <c r="K44" s="29"/>
+      <c r="L44" s="29"/>
+      <c r="M44" s="29"/>
+    </row>
+    <row r="45" s="61" customFormat="true" ht="15.3" hidden="false" customHeight="true" outlineLevel="1" collapsed="false">
+      <c r="A45" s="30" t="s">
+        <v>108</v>
+      </c>
+      <c r="B45" s="77" t="s">
+        <v>74</v>
+      </c>
+      <c r="C45" s="77"/>
+      <c r="D45" s="77"/>
+      <c r="E45" s="77"/>
+      <c r="F45" s="77"/>
+      <c r="G45" s="30" t="s">
+        <v>109</v>
+      </c>
+      <c r="H45" s="30" t="s">
+        <v>110</v>
+      </c>
+      <c r="I45" s="30" t="s">
+        <v>111</v>
+      </c>
+      <c r="J45" s="30"/>
+      <c r="K45" s="30"/>
+      <c r="L45" s="30"/>
+      <c r="M45" s="78" t="s">
+        <v>90</v>
+      </c>
+      <c r="N45" s="78"/>
+      <c r="O45" s="78"/>
+      <c r="P45" s="78"/>
+      <c r="Q45" s="79" t="s">
+        <v>112</v>
+      </c>
+      <c r="R45" s="79"/>
+    </row>
+    <row r="46" s="16" customFormat="true" ht="29.7" hidden="false" customHeight="true" outlineLevel="1" collapsed="false">
+      <c r="A46" s="64" t="n">
+        <v>44223</v>
+      </c>
+      <c r="B46" s="36" t="s">
+        <v>113</v>
+      </c>
+      <c r="C46" s="36"/>
+      <c r="D46" s="36"/>
+      <c r="E46" s="36"/>
+      <c r="F46" s="36"/>
+      <c r="G46" s="80" t="n">
+        <v>-808</v>
+      </c>
+      <c r="H46" s="81" t="s">
+        <v>50</v>
+      </c>
+      <c r="I46" s="82" t="s">
+        <v>114</v>
+      </c>
+      <c r="J46" s="82"/>
+      <c r="K46" s="82"/>
+      <c r="L46" s="82"/>
+      <c r="M46" s="73" t="s">
+        <v>115</v>
+      </c>
+      <c r="N46" s="73"/>
+      <c r="O46" s="73"/>
+      <c r="P46" s="73"/>
+      <c r="Q46" s="81" t="s">
+        <v>116</v>
+      </c>
+      <c r="R46" s="81"/>
+    </row>
+    <row r="47" s="1" customFormat="true" ht="17.1" hidden="false" customHeight="true" outlineLevel="1" collapsed="false">
+      <c r="A47" s="48"/>
+      <c r="B47" s="48"/>
+      <c r="C47" s="48"/>
+      <c r="D47" s="48"/>
+      <c r="E47" s="48"/>
+      <c r="F47" s="48"/>
+      <c r="G47" s="48"/>
+      <c r="H47" s="83"/>
+      <c r="I47" s="75"/>
+      <c r="J47" s="75"/>
+      <c r="K47" s="48"/>
+      <c r="L47" s="48"/>
+      <c r="M47" s="48"/>
+      <c r="N47" s="48"/>
+      <c r="O47" s="84"/>
+      <c r="P47" s="75"/>
+      <c r="Q47" s="75"/>
+      <c r="R47" s="75"/>
+    </row>
+    <row r="48" s="16" customFormat="true" ht="17.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A48" s="29" t="s">
+        <v>117</v>
+      </c>
+      <c r="B48" s="29"/>
+      <c r="C48" s="29"/>
+      <c r="D48" s="29"/>
+      <c r="E48" s="85"/>
+      <c r="F48" s="85"/>
+      <c r="G48" s="85"/>
+      <c r="H48" s="55"/>
+      <c r="I48" s="86"/>
+      <c r="J48" s="87"/>
+      <c r="K48" s="27"/>
+      <c r="L48" s="27"/>
+      <c r="M48" s="27"/>
+      <c r="N48" s="27"/>
+      <c r="O48" s="27"/>
+      <c r="P48" s="27"/>
+    </row>
+    <row r="49" s="91" customFormat="true" ht="56.7" hidden="false" customHeight="true" outlineLevel="1" collapsed="false">
+      <c r="A49" s="78" t="s">
+        <v>118</v>
+      </c>
+      <c r="B49" s="78"/>
+      <c r="C49" s="78"/>
+      <c r="D49" s="88" t="s">
+        <v>119</v>
+      </c>
+      <c r="E49" s="88" t="s">
+        <v>120</v>
+      </c>
+      <c r="F49" s="88" t="s">
+        <v>121</v>
+      </c>
+      <c r="G49" s="88" t="s">
+        <v>122</v>
+      </c>
+      <c r="H49" s="89" t="s">
+        <v>123</v>
+      </c>
+      <c r="I49" s="89" t="s">
+        <v>124</v>
+      </c>
+      <c r="J49" s="89" t="s">
+        <v>125</v>
+      </c>
+      <c r="K49" s="78" t="s">
+        <v>126</v>
+      </c>
+      <c r="L49" s="78"/>
+      <c r="M49" s="78"/>
+      <c r="N49" s="79" t="s">
+        <v>112</v>
+      </c>
+      <c r="O49" s="79"/>
+      <c r="P49" s="90"/>
+      <c r="Q49" s="90" t="s">
+        <v>127</v>
+      </c>
+      <c r="R49" s="90"/>
+      <c r="S49" s="90"/>
+    </row>
+    <row r="50" s="91" customFormat="true" ht="29.7" hidden="false" customHeight="true" outlineLevel="1" collapsed="false">
+      <c r="A50" s="92" t="s">
+        <v>128</v>
+      </c>
+      <c r="B50" s="92"/>
+      <c r="C50" s="92"/>
+      <c r="D50" s="93" t="n">
+        <v>44210</v>
+      </c>
+      <c r="E50" s="94" t="n">
+        <v>2600</v>
+      </c>
+      <c r="F50" s="67" t="n">
+        <v>2.391</v>
+      </c>
+      <c r="G50" s="95" t="n">
+        <v>6216.6</v>
+      </c>
+      <c r="H50" s="96" t="n">
+        <v>6216.6</v>
+      </c>
+      <c r="I50" s="97" t="s">
+        <v>50</v>
+      </c>
+      <c r="J50" s="98" t="n">
+        <v>44223</v>
+      </c>
+      <c r="K50" s="92" t="s">
+        <v>129</v>
+      </c>
+      <c r="L50" s="92"/>
+      <c r="M50" s="92"/>
+      <c r="N50" s="81" t="s">
+        <v>116</v>
+      </c>
+      <c r="O50" s="81"/>
+      <c r="P50" s="90"/>
+      <c r="Q50" s="90"/>
+      <c r="R50" s="90"/>
+      <c r="S50" s="90"/>
+    </row>
+    <row r="51" s="103" customFormat="true" ht="13.2" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
+      <c r="A51" s="99"/>
+      <c r="B51" s="99"/>
+      <c r="C51" s="99"/>
+      <c r="D51" s="100"/>
+      <c r="E51" s="99"/>
+      <c r="F51" s="100"/>
+      <c r="G51" s="100"/>
+      <c r="H51" s="100"/>
+      <c r="I51" s="101"/>
+      <c r="J51" s="100"/>
+      <c r="K51" s="99"/>
+      <c r="L51" s="99"/>
+      <c r="M51" s="99"/>
+      <c r="N51" s="102"/>
+      <c r="O51" s="102"/>
+      <c r="P51" s="90"/>
+      <c r="Q51" s="90"/>
+      <c r="R51" s="90"/>
+    </row>
+    <row r="52" s="15" customFormat="true" ht="17.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A52" s="29" t="s">
+        <v>130</v>
+      </c>
+      <c r="B52" s="29"/>
+      <c r="C52" s="29"/>
+      <c r="D52" s="29"/>
+      <c r="E52" s="29"/>
+      <c r="F52" s="29"/>
+      <c r="G52" s="29"/>
+      <c r="H52" s="29"/>
+      <c r="I52" s="29"/>
+      <c r="J52" s="29"/>
+      <c r="K52" s="29"/>
+      <c r="L52" s="29"/>
+      <c r="M52" s="29"/>
+      <c r="N52" s="22"/>
+      <c r="O52" s="22"/>
+      <c r="P52" s="104"/>
+    </row>
+    <row r="53" s="15" customFormat="true" ht="43.2" hidden="false" customHeight="true" outlineLevel="1" collapsed="false">
+      <c r="A53" s="88" t="s">
         <v>73</v>
       </c>
-      <c r="N36" s="62"/>
-      <c r="O36" s="62"/>
-      <c r="P36" s="62"/>
-      <c r="Q36" s="63" t="s">
-        <v>74</v>
-      </c>
-      <c r="R36" s="63"/>
-    </row>
-    <row r="37" s="16" customFormat="true" ht="29.7" hidden="false" customHeight="true" outlineLevel="1" collapsed="false">
-      <c r="A37" s="65" t="n">
-        <v>44223</v>
-      </c>
-      <c r="B37" s="36" t="s">
-        <v>75</v>
-      </c>
-      <c r="C37" s="36"/>
-      <c r="D37" s="36"/>
-      <c r="E37" s="36"/>
-      <c r="F37" s="36"/>
-      <c r="G37" s="66" t="n">
-        <v>-808</v>
-      </c>
-      <c r="H37" s="67" t="s">
-        <v>50</v>
-      </c>
-      <c r="I37" s="68" t="s">
-        <v>76</v>
-      </c>
-      <c r="J37" s="68"/>
-      <c r="K37" s="68"/>
-      <c r="L37" s="68"/>
-      <c r="M37" s="69" t="s">
-        <v>77</v>
-      </c>
-      <c r="N37" s="69"/>
-      <c r="O37" s="69"/>
-      <c r="P37" s="69"/>
-      <c r="Q37" s="67" t="s">
-        <v>78</v>
-      </c>
-      <c r="R37" s="67"/>
-    </row>
-    <row r="38" s="1" customFormat="true" ht="17.1" hidden="false" customHeight="true" outlineLevel="1" collapsed="false">
-      <c r="A38" s="48"/>
-      <c r="B38" s="48"/>
-      <c r="C38" s="48"/>
-      <c r="D38" s="48"/>
-      <c r="E38" s="48"/>
-      <c r="F38" s="48"/>
-      <c r="G38" s="48"/>
-      <c r="H38" s="70"/>
-      <c r="I38" s="71"/>
-      <c r="J38" s="71"/>
-      <c r="K38" s="48"/>
-      <c r="L38" s="48"/>
-      <c r="M38" s="48"/>
-      <c r="N38" s="48"/>
-      <c r="O38" s="72"/>
-      <c r="P38" s="71"/>
-      <c r="Q38" s="71"/>
-      <c r="R38" s="71"/>
-    </row>
-    <row r="39" s="16" customFormat="true" ht="17.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A39" s="29" t="s">
-        <v>79</v>
-      </c>
-      <c r="B39" s="29"/>
-      <c r="C39" s="29"/>
-      <c r="D39" s="29"/>
-      <c r="E39" s="73"/>
-      <c r="F39" s="73"/>
-      <c r="G39" s="73"/>
-      <c r="H39" s="55"/>
-      <c r="I39" s="74"/>
-      <c r="J39" s="75"/>
-      <c r="K39" s="27"/>
-      <c r="L39" s="27"/>
-      <c r="M39" s="27"/>
-      <c r="N39" s="27"/>
-      <c r="O39" s="27"/>
-      <c r="P39" s="27"/>
-    </row>
-    <row r="40" s="79" customFormat="true" ht="56.7" hidden="false" customHeight="true" outlineLevel="1" collapsed="false">
-      <c r="A40" s="62" t="s">
-        <v>80</v>
-      </c>
-      <c r="B40" s="62"/>
-      <c r="C40" s="62"/>
-      <c r="D40" s="76" t="s">
-        <v>81</v>
-      </c>
-      <c r="E40" s="76" t="s">
-        <v>82</v>
-      </c>
-      <c r="F40" s="76" t="s">
-        <v>83</v>
-      </c>
-      <c r="G40" s="76" t="s">
-        <v>84</v>
-      </c>
-      <c r="H40" s="77" t="s">
-        <v>85</v>
-      </c>
-      <c r="I40" s="77" t="s">
-        <v>86</v>
-      </c>
-      <c r="J40" s="77" t="s">
-        <v>87</v>
-      </c>
-      <c r="K40" s="62" t="s">
-        <v>88</v>
-      </c>
-      <c r="L40" s="62"/>
-      <c r="M40" s="62"/>
-      <c r="N40" s="63" t="s">
-        <v>74</v>
-      </c>
-      <c r="O40" s="63"/>
-      <c r="P40" s="78"/>
-      <c r="Q40" s="78" t="s">
-        <v>89</v>
-      </c>
-      <c r="R40" s="78"/>
-      <c r="S40" s="78"/>
-    </row>
-    <row r="41" s="79" customFormat="true" ht="29.7" hidden="false" customHeight="true" outlineLevel="1" collapsed="false">
-      <c r="A41" s="80" t="s">
-        <v>90</v>
-      </c>
-      <c r="B41" s="80"/>
-      <c r="C41" s="80"/>
-      <c r="D41" s="81" t="n">
-        <v>44210</v>
-      </c>
-      <c r="E41" s="82" t="n">
-        <v>2600</v>
-      </c>
-      <c r="F41" s="83" t="n">
-        <v>2.391</v>
-      </c>
-      <c r="G41" s="84" t="n">
-        <v>6216.6</v>
-      </c>
-      <c r="H41" s="85" t="n">
-        <v>6216.6</v>
-      </c>
-      <c r="I41" s="86" t="s">
-        <v>50</v>
-      </c>
-      <c r="J41" s="87" t="n">
-        <v>44223</v>
-      </c>
-      <c r="K41" s="80" t="s">
-        <v>91</v>
-      </c>
-      <c r="L41" s="80"/>
-      <c r="M41" s="80"/>
-      <c r="N41" s="67" t="s">
-        <v>78</v>
-      </c>
-      <c r="O41" s="67"/>
-      <c r="P41" s="78"/>
-      <c r="Q41" s="78"/>
-      <c r="R41" s="78"/>
-      <c r="S41" s="78"/>
-    </row>
-    <row r="42" s="92" customFormat="true" ht="13.2" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
-      <c r="A42" s="88"/>
-      <c r="B42" s="88"/>
-      <c r="C42" s="88"/>
-      <c r="D42" s="89"/>
-      <c r="E42" s="88"/>
-      <c r="F42" s="89"/>
-      <c r="G42" s="89"/>
-      <c r="H42" s="89"/>
-      <c r="I42" s="90"/>
-      <c r="J42" s="89"/>
-      <c r="K42" s="88"/>
-      <c r="L42" s="88"/>
-      <c r="M42" s="88"/>
-      <c r="N42" s="91"/>
-      <c r="O42" s="91"/>
-      <c r="P42" s="78"/>
-      <c r="Q42" s="78"/>
-      <c r="R42" s="78"/>
-    </row>
-    <row r="43" s="15" customFormat="true" ht="17.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A43" s="29" t="s">
-        <v>92</v>
-      </c>
-      <c r="B43" s="29"/>
-      <c r="C43" s="29"/>
-      <c r="D43" s="29"/>
-      <c r="E43" s="29"/>
-      <c r="F43" s="29"/>
-      <c r="G43" s="29"/>
-      <c r="H43" s="29"/>
-      <c r="I43" s="29"/>
-      <c r="J43" s="29"/>
-      <c r="K43" s="29"/>
-      <c r="L43" s="29"/>
-      <c r="M43" s="29"/>
-      <c r="N43" s="22"/>
-      <c r="O43" s="22"/>
-      <c r="P43" s="93"/>
-    </row>
-    <row r="44" s="15" customFormat="true" ht="43.2" hidden="false" customHeight="true" outlineLevel="1" collapsed="false">
-      <c r="A44" s="76" t="s">
-        <v>93</v>
-      </c>
-      <c r="B44" s="76"/>
-      <c r="C44" s="76"/>
-      <c r="D44" s="76" t="s">
-        <v>94</v>
-      </c>
-      <c r="E44" s="76"/>
-      <c r="F44" s="76" t="s">
-        <v>95</v>
-      </c>
-      <c r="G44" s="76"/>
-      <c r="H44" s="76" t="s">
-        <v>96</v>
-      </c>
-      <c r="I44" s="76"/>
-      <c r="J44" s="76" t="s">
-        <v>97</v>
-      </c>
-      <c r="K44" s="76"/>
-      <c r="L44" s="76" t="s">
-        <v>98</v>
-      </c>
-      <c r="M44" s="76"/>
-      <c r="N44" s="76" t="s">
-        <v>99</v>
-      </c>
-      <c r="O44" s="76"/>
-      <c r="P44" s="22"/>
-      <c r="Q44" s="22"/>
-      <c r="R44" s="93"/>
-    </row>
-    <row r="45" s="15" customFormat="true" ht="17.1" hidden="false" customHeight="true" outlineLevel="1" collapsed="false">
-      <c r="A45" s="86" t="s">
-        <v>100</v>
-      </c>
-      <c r="B45" s="86"/>
-      <c r="C45" s="86"/>
-      <c r="D45" s="86"/>
-      <c r="E45" s="86"/>
-      <c r="F45" s="86"/>
-      <c r="G45" s="86"/>
-      <c r="H45" s="94"/>
-      <c r="I45" s="94"/>
-      <c r="J45" s="86"/>
-      <c r="K45" s="86"/>
-      <c r="L45" s="86"/>
-      <c r="M45" s="86"/>
-      <c r="N45" s="86"/>
-      <c r="O45" s="86"/>
-      <c r="P45" s="22"/>
-      <c r="Q45" s="22"/>
-      <c r="R45" s="93"/>
-    </row>
-    <row r="46" s="51" customFormat="true" ht="17.1" hidden="false" customHeight="true" outlineLevel="1" collapsed="false">
-      <c r="A46" s="95"/>
-      <c r="B46" s="95"/>
-      <c r="C46" s="95"/>
-      <c r="D46" s="95"/>
-      <c r="E46" s="95"/>
-      <c r="F46" s="95"/>
-      <c r="G46" s="95"/>
-      <c r="H46" s="95"/>
-      <c r="I46" s="95"/>
-      <c r="J46" s="95"/>
-      <c r="K46" s="95"/>
-      <c r="L46" s="95"/>
-      <c r="M46" s="71"/>
-      <c r="N46" s="95"/>
-      <c r="O46" s="95"/>
-    </row>
-    <row r="47" s="15" customFormat="true" ht="17.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A47" s="29" t="s">
-        <v>101</v>
-      </c>
-      <c r="B47" s="29"/>
-      <c r="C47" s="29"/>
-      <c r="D47" s="29"/>
-      <c r="E47" s="29"/>
-      <c r="F47" s="29"/>
-      <c r="G47" s="29"/>
-      <c r="H47" s="29"/>
-      <c r="I47" s="29"/>
-      <c r="J47" s="29"/>
-      <c r="K47" s="29"/>
-      <c r="L47" s="29"/>
-      <c r="M47" s="29"/>
-      <c r="N47" s="22"/>
-      <c r="O47" s="22"/>
-      <c r="P47" s="93"/>
-    </row>
-    <row r="48" s="98" customFormat="true" ht="56.7" hidden="false" customHeight="true" outlineLevel="1" collapsed="false">
-      <c r="A48" s="33" t="s">
-        <v>102</v>
-      </c>
-      <c r="B48" s="33"/>
-      <c r="C48" s="33" t="s">
-        <v>103</v>
-      </c>
-      <c r="D48" s="33"/>
-      <c r="E48" s="30" t="s">
-        <v>104</v>
-      </c>
-      <c r="F48" s="30"/>
-      <c r="G48" s="30" t="s">
-        <v>105</v>
-      </c>
-      <c r="H48" s="30"/>
-      <c r="I48" s="30" t="s">
-        <v>106</v>
-      </c>
-      <c r="J48" s="30"/>
-      <c r="K48" s="30" t="s">
-        <v>107</v>
-      </c>
-      <c r="L48" s="30"/>
-      <c r="M48" s="30" t="s">
-        <v>108</v>
-      </c>
-      <c r="N48" s="30"/>
-      <c r="O48" s="30" t="s">
-        <v>109</v>
-      </c>
-      <c r="P48" s="30"/>
-      <c r="Q48" s="30" t="s">
-        <v>110</v>
-      </c>
-      <c r="R48" s="30"/>
-      <c r="S48" s="96"/>
-      <c r="T48" s="96"/>
-      <c r="U48" s="96"/>
-      <c r="V48" s="96"/>
-      <c r="W48" s="97"/>
-    </row>
-    <row r="49" s="15" customFormat="true" ht="17.1" hidden="false" customHeight="true" outlineLevel="1" collapsed="false">
-      <c r="A49" s="99" t="s">
+      <c r="B53" s="88"/>
+      <c r="C53" s="88"/>
+      <c r="D53" s="88" t="s">
+        <v>131</v>
+      </c>
+      <c r="E53" s="88"/>
+      <c r="F53" s="88" t="s">
+        <v>132</v>
+      </c>
+      <c r="G53" s="88"/>
+      <c r="H53" s="88" t="s">
+        <v>133</v>
+      </c>
+      <c r="I53" s="88"/>
+      <c r="J53" s="88" t="s">
+        <v>134</v>
+      </c>
+      <c r="K53" s="88"/>
+      <c r="L53" s="88" t="s">
+        <v>135</v>
+      </c>
+      <c r="M53" s="88"/>
+      <c r="N53" s="88" t="s">
+        <v>136</v>
+      </c>
+      <c r="O53" s="88"/>
+      <c r="P53" s="22"/>
+      <c r="Q53" s="22"/>
+      <c r="R53" s="104"/>
+    </row>
+    <row r="54" s="15" customFormat="true" ht="17.1" hidden="false" customHeight="true" outlineLevel="1" collapsed="false">
+      <c r="A54" s="97" t="s">
+        <v>137</v>
+      </c>
+      <c r="B54" s="97"/>
+      <c r="C54" s="97"/>
+      <c r="D54" s="97"/>
+      <c r="E54" s="97"/>
+      <c r="F54" s="97"/>
+      <c r="G54" s="97"/>
+      <c r="H54" s="105"/>
+      <c r="I54" s="105"/>
+      <c r="J54" s="97"/>
+      <c r="K54" s="97"/>
+      <c r="L54" s="97"/>
+      <c r="M54" s="97"/>
+      <c r="N54" s="97"/>
+      <c r="O54" s="97"/>
+      <c r="P54" s="22"/>
+      <c r="Q54" s="22"/>
+      <c r="R54" s="104"/>
+    </row>
+    <row r="55" s="51" customFormat="true" ht="17.1" hidden="false" customHeight="true" outlineLevel="1" collapsed="false">
+      <c r="A55" s="106"/>
+      <c r="B55" s="106"/>
+      <c r="C55" s="106"/>
+      <c r="D55" s="106"/>
+      <c r="E55" s="106"/>
+      <c r="F55" s="106"/>
+      <c r="G55" s="106"/>
+      <c r="H55" s="106"/>
+      <c r="I55" s="106"/>
+      <c r="J55" s="106"/>
+      <c r="K55" s="106"/>
+      <c r="L55" s="106"/>
+      <c r="M55" s="75"/>
+      <c r="N55" s="106"/>
+      <c r="O55" s="106"/>
+    </row>
+    <row r="56" s="15" customFormat="true" ht="17.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A56" s="29" t="s">
+        <v>138</v>
+      </c>
+      <c r="B56" s="29"/>
+      <c r="C56" s="29"/>
+      <c r="D56" s="29"/>
+      <c r="E56" s="29"/>
+      <c r="F56" s="29"/>
+      <c r="G56" s="29"/>
+      <c r="H56" s="29"/>
+      <c r="I56" s="29"/>
+      <c r="J56" s="29"/>
+      <c r="K56" s="29"/>
+      <c r="L56" s="29"/>
+      <c r="M56" s="29"/>
+      <c r="N56" s="22"/>
+      <c r="O56" s="22"/>
+      <c r="P56" s="104"/>
+    </row>
+    <row r="57" s="109" customFormat="true" ht="56.7" hidden="false" customHeight="true" outlineLevel="1" collapsed="false">
+      <c r="A57" s="33" t="s">
+        <v>139</v>
+      </c>
+      <c r="B57" s="33"/>
+      <c r="C57" s="33" t="s">
+        <v>140</v>
+      </c>
+      <c r="D57" s="33"/>
+      <c r="E57" s="30" t="s">
+        <v>141</v>
+      </c>
+      <c r="F57" s="30"/>
+      <c r="G57" s="30" t="s">
+        <v>142</v>
+      </c>
+      <c r="H57" s="30"/>
+      <c r="I57" s="30" t="s">
+        <v>143</v>
+      </c>
+      <c r="J57" s="30"/>
+      <c r="K57" s="30" t="s">
+        <v>144</v>
+      </c>
+      <c r="L57" s="30"/>
+      <c r="M57" s="30" t="s">
+        <v>145</v>
+      </c>
+      <c r="N57" s="30"/>
+      <c r="O57" s="30" t="s">
+        <v>146</v>
+      </c>
+      <c r="P57" s="30"/>
+      <c r="Q57" s="30" t="s">
+        <v>147</v>
+      </c>
+      <c r="R57" s="30"/>
+      <c r="S57" s="107"/>
+      <c r="T57" s="107"/>
+      <c r="U57" s="107"/>
+      <c r="V57" s="107"/>
+      <c r="W57" s="108"/>
+    </row>
+    <row r="58" s="15" customFormat="true" ht="17.1" hidden="false" customHeight="true" outlineLevel="1" collapsed="false">
+      <c r="A58" s="110" t="s">
         <v>66</v>
       </c>
-      <c r="B49" s="99"/>
-      <c r="C49" s="99"/>
-      <c r="D49" s="99"/>
-      <c r="E49" s="99"/>
-      <c r="F49" s="99"/>
-      <c r="G49" s="99"/>
-      <c r="H49" s="99"/>
-      <c r="I49" s="99"/>
-      <c r="J49" s="99"/>
-      <c r="K49" s="99"/>
-      <c r="L49" s="99"/>
-      <c r="M49" s="99"/>
-      <c r="N49" s="99"/>
-      <c r="O49" s="100"/>
-      <c r="P49" s="100"/>
-      <c r="Q49" s="100"/>
-      <c r="R49" s="100"/>
-      <c r="S49" s="22"/>
-      <c r="T49" s="22"/>
-      <c r="U49" s="22"/>
-      <c r="V49" s="22"/>
-      <c r="W49" s="93"/>
-    </row>
-    <row r="50" s="1" customFormat="true" ht="17.1" hidden="false" customHeight="true" outlineLevel="1" collapsed="false">
-      <c r="A50" s="49"/>
-      <c r="B50" s="49"/>
-      <c r="C50" s="49"/>
-      <c r="D50" s="49"/>
-      <c r="E50" s="49"/>
-      <c r="F50" s="49"/>
-      <c r="G50" s="49"/>
-      <c r="H50" s="49"/>
-      <c r="I50" s="49"/>
-      <c r="J50" s="49"/>
-      <c r="K50" s="49"/>
-      <c r="L50" s="49"/>
-      <c r="M50" s="49"/>
-      <c r="N50" s="71"/>
-      <c r="O50" s="49"/>
-      <c r="P50" s="49"/>
-      <c r="Q50" s="49"/>
-      <c r="R50" s="71"/>
-    </row>
-    <row r="51" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="101"/>
-      <c r="B51" s="101"/>
-      <c r="C51" s="101"/>
-      <c r="D51" s="101"/>
-      <c r="E51" s="101"/>
-      <c r="F51" s="22"/>
-      <c r="G51" s="22"/>
-      <c r="H51" s="22"/>
-      <c r="I51" s="22"/>
-      <c r="J51" s="22"/>
-      <c r="K51" s="22"/>
-      <c r="L51" s="22"/>
-      <c r="M51" s="22"/>
-    </row>
-    <row r="52" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="102"/>
-      <c r="B52" s="101"/>
-      <c r="C52" s="101"/>
-      <c r="D52" s="101"/>
-      <c r="E52" s="101"/>
-      <c r="F52" s="22"/>
-      <c r="G52" s="22"/>
-      <c r="H52" s="22"/>
-      <c r="I52" s="22"/>
-      <c r="J52" s="22"/>
-      <c r="K52" s="22"/>
-      <c r="L52" s="22"/>
-      <c r="M52" s="22"/>
-    </row>
-    <row r="53" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A53" s="103" t="s">
-        <v>111</v>
-      </c>
-      <c r="B53" s="103"/>
-      <c r="C53" s="103"/>
-      <c r="D53" s="103"/>
-      <c r="E53" s="103"/>
-      <c r="F53" s="103"/>
-      <c r="G53" s="103"/>
-      <c r="H53" s="22"/>
-      <c r="I53" s="22"/>
-      <c r="J53" s="22"/>
-      <c r="K53" s="22"/>
-      <c r="L53" s="22"/>
-      <c r="M53" s="22"/>
-    </row>
-    <row r="54" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A54" s="104" t="s">
-        <v>112</v>
-      </c>
-      <c r="B54" s="104"/>
-      <c r="C54" s="104"/>
-      <c r="D54" s="14" t="s">
-        <v>113</v>
-      </c>
-      <c r="E54" s="14"/>
-      <c r="F54" s="22"/>
-      <c r="G54" s="22"/>
-      <c r="H54" s="22"/>
-      <c r="I54" s="22"/>
-      <c r="J54" s="22"/>
-      <c r="K54" s="22"/>
-      <c r="L54" s="22"/>
-      <c r="M54" s="22"/>
+      <c r="B58" s="110"/>
+      <c r="C58" s="110"/>
+      <c r="D58" s="110"/>
+      <c r="E58" s="110"/>
+      <c r="F58" s="110"/>
+      <c r="G58" s="110"/>
+      <c r="H58" s="110"/>
+      <c r="I58" s="110"/>
+      <c r="J58" s="110"/>
+      <c r="K58" s="110"/>
+      <c r="L58" s="110"/>
+      <c r="M58" s="110"/>
+      <c r="N58" s="110"/>
+      <c r="O58" s="111"/>
+      <c r="P58" s="111"/>
+      <c r="Q58" s="111"/>
+      <c r="R58" s="111"/>
+      <c r="S58" s="22"/>
+      <c r="T58" s="22"/>
+      <c r="U58" s="22"/>
+      <c r="V58" s="22"/>
+      <c r="W58" s="104"/>
+    </row>
+    <row r="59" s="1" customFormat="true" ht="17.1" hidden="false" customHeight="true" outlineLevel="1" collapsed="false">
+      <c r="A59" s="49"/>
+      <c r="B59" s="49"/>
+      <c r="C59" s="49"/>
+      <c r="D59" s="49"/>
+      <c r="E59" s="49"/>
+      <c r="F59" s="49"/>
+      <c r="G59" s="49"/>
+      <c r="H59" s="49"/>
+      <c r="I59" s="49"/>
+      <c r="J59" s="49"/>
+      <c r="K59" s="49"/>
+      <c r="L59" s="49"/>
+      <c r="M59" s="49"/>
+      <c r="N59" s="75"/>
+      <c r="O59" s="49"/>
+      <c r="P59" s="49"/>
+      <c r="Q59" s="49"/>
+      <c r="R59" s="75"/>
+    </row>
+    <row r="60" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A60" s="112"/>
+      <c r="B60" s="112"/>
+      <c r="C60" s="112"/>
+      <c r="D60" s="112"/>
+      <c r="E60" s="112"/>
+      <c r="F60" s="22"/>
+      <c r="G60" s="22"/>
+      <c r="H60" s="22"/>
+      <c r="I60" s="22"/>
+      <c r="J60" s="22"/>
+      <c r="K60" s="22"/>
+      <c r="L60" s="22"/>
+      <c r="M60" s="22"/>
+    </row>
+    <row r="61" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A61" s="113"/>
+      <c r="B61" s="112"/>
+      <c r="C61" s="112"/>
+      <c r="D61" s="112"/>
+      <c r="E61" s="112"/>
+      <c r="F61" s="22"/>
+      <c r="G61" s="22"/>
+      <c r="H61" s="22"/>
+      <c r="I61" s="22"/>
+      <c r="J61" s="22"/>
+      <c r="K61" s="22"/>
+      <c r="L61" s="22"/>
+      <c r="M61" s="22"/>
+    </row>
+    <row r="62" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A62" s="114" t="s">
+        <v>148</v>
+      </c>
+      <c r="B62" s="114"/>
+      <c r="C62" s="114"/>
+      <c r="D62" s="114"/>
+      <c r="E62" s="114"/>
+      <c r="F62" s="114"/>
+      <c r="G62" s="114"/>
+      <c r="H62" s="22"/>
+      <c r="I62" s="22"/>
+      <c r="J62" s="22"/>
+      <c r="K62" s="22"/>
+      <c r="L62" s="22"/>
+      <c r="M62" s="22"/>
+    </row>
+    <row r="63" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A63" s="115" t="s">
+        <v>149</v>
+      </c>
+      <c r="B63" s="115"/>
+      <c r="C63" s="115"/>
+      <c r="D63" s="14" t="s">
+        <v>150</v>
+      </c>
+      <c r="E63" s="14"/>
+      <c r="F63" s="22"/>
+      <c r="G63" s="22"/>
+      <c r="H63" s="22"/>
+      <c r="I63" s="22"/>
+      <c r="J63" s="22"/>
+      <c r="K63" s="22"/>
+      <c r="L63" s="22"/>
+      <c r="M63" s="22"/>
     </row>
   </sheetData>
-  <mergeCells count="94">
+  <mergeCells count="101">
     <mergeCell ref="A6:E6"/>
     <mergeCell ref="F6:W6"/>
     <mergeCell ref="A7:E7"/>
@@ -2922,57 +3695,64 @@
     <mergeCell ref="G33:H33"/>
     <mergeCell ref="I33:J33"/>
     <mergeCell ref="K33:L33"/>
-    <mergeCell ref="B36:F36"/>
-    <mergeCell ref="I36:L36"/>
-    <mergeCell ref="M36:P36"/>
-    <mergeCell ref="Q36:R36"/>
-    <mergeCell ref="B37:F37"/>
-    <mergeCell ref="I37:L37"/>
-    <mergeCell ref="M37:P37"/>
-    <mergeCell ref="Q37:R37"/>
-    <mergeCell ref="A40:C40"/>
-    <mergeCell ref="K40:M40"/>
-    <mergeCell ref="N40:O40"/>
-    <mergeCell ref="A41:C41"/>
-    <mergeCell ref="K41:M41"/>
-    <mergeCell ref="N41:O41"/>
-    <mergeCell ref="A44:C44"/>
-    <mergeCell ref="D44:E44"/>
-    <mergeCell ref="F44:G44"/>
-    <mergeCell ref="H44:I44"/>
-    <mergeCell ref="J44:K44"/>
-    <mergeCell ref="L44:M44"/>
-    <mergeCell ref="N44:O44"/>
-    <mergeCell ref="A45:C45"/>
-    <mergeCell ref="D45:E45"/>
-    <mergeCell ref="F45:G45"/>
-    <mergeCell ref="H45:I45"/>
-    <mergeCell ref="J45:K45"/>
-    <mergeCell ref="L45:M45"/>
-    <mergeCell ref="N45:O45"/>
-    <mergeCell ref="J46:K46"/>
-    <mergeCell ref="N46:O46"/>
-    <mergeCell ref="A48:B48"/>
-    <mergeCell ref="C48:D48"/>
-    <mergeCell ref="E48:F48"/>
-    <mergeCell ref="G48:H48"/>
-    <mergeCell ref="I48:J48"/>
-    <mergeCell ref="K48:L48"/>
-    <mergeCell ref="M48:N48"/>
-    <mergeCell ref="O48:P48"/>
-    <mergeCell ref="Q48:R48"/>
-    <mergeCell ref="A49:B49"/>
-    <mergeCell ref="C49:D49"/>
-    <mergeCell ref="E49:F49"/>
-    <mergeCell ref="G49:H49"/>
-    <mergeCell ref="I49:J49"/>
-    <mergeCell ref="K49:L49"/>
-    <mergeCell ref="M49:N49"/>
-    <mergeCell ref="O49:P49"/>
-    <mergeCell ref="Q49:R49"/>
-    <mergeCell ref="A53:G53"/>
+    <mergeCell ref="F36:G36"/>
+    <mergeCell ref="F37:G37"/>
+    <mergeCell ref="F38:G38"/>
+    <mergeCell ref="F39:G39"/>
+    <mergeCell ref="F40:G40"/>
+    <mergeCell ref="F41:G41"/>
+    <mergeCell ref="F42:G42"/>
+    <mergeCell ref="B45:F45"/>
+    <mergeCell ref="I45:L45"/>
+    <mergeCell ref="M45:P45"/>
+    <mergeCell ref="Q45:R45"/>
+    <mergeCell ref="B46:F46"/>
+    <mergeCell ref="I46:L46"/>
+    <mergeCell ref="M46:P46"/>
+    <mergeCell ref="Q46:R46"/>
+    <mergeCell ref="A49:C49"/>
+    <mergeCell ref="K49:M49"/>
+    <mergeCell ref="N49:O49"/>
+    <mergeCell ref="A50:C50"/>
+    <mergeCell ref="K50:M50"/>
+    <mergeCell ref="N50:O50"/>
+    <mergeCell ref="A53:C53"/>
+    <mergeCell ref="D53:E53"/>
+    <mergeCell ref="F53:G53"/>
+    <mergeCell ref="H53:I53"/>
+    <mergeCell ref="J53:K53"/>
+    <mergeCell ref="L53:M53"/>
+    <mergeCell ref="N53:O53"/>
     <mergeCell ref="A54:C54"/>
     <mergeCell ref="D54:E54"/>
+    <mergeCell ref="F54:G54"/>
+    <mergeCell ref="H54:I54"/>
+    <mergeCell ref="J54:K54"/>
+    <mergeCell ref="L54:M54"/>
+    <mergeCell ref="N54:O54"/>
+    <mergeCell ref="J55:K55"/>
+    <mergeCell ref="N55:O55"/>
+    <mergeCell ref="A57:B57"/>
+    <mergeCell ref="C57:D57"/>
+    <mergeCell ref="E57:F57"/>
+    <mergeCell ref="G57:H57"/>
+    <mergeCell ref="I57:J57"/>
+    <mergeCell ref="K57:L57"/>
+    <mergeCell ref="M57:N57"/>
+    <mergeCell ref="O57:P57"/>
+    <mergeCell ref="Q57:R57"/>
+    <mergeCell ref="A58:B58"/>
+    <mergeCell ref="C58:D58"/>
+    <mergeCell ref="E58:F58"/>
+    <mergeCell ref="G58:H58"/>
+    <mergeCell ref="I58:J58"/>
+    <mergeCell ref="K58:L58"/>
+    <mergeCell ref="M58:N58"/>
+    <mergeCell ref="O58:P58"/>
+    <mergeCell ref="Q58:R58"/>
+    <mergeCell ref="A62:G62"/>
+    <mergeCell ref="A63:C63"/>
+    <mergeCell ref="D63:E63"/>
   </mergeCells>
   <conditionalFormatting sqref="A13:AMJ21">
     <cfRule type="expression" priority="2" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
@@ -2982,22 +3762,22 @@
       <formula>$A13="Входящий остаток"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K41:K43">
+  <conditionalFormatting sqref="K50:K52">
     <cfRule type="expression" priority="4" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
-      <formula>MOD(ROUND($K43,2),1)&lt;&gt;0</formula>
+      <formula>MOD(ROUND($K52,2),1)&lt;&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J29:J35">
+  <conditionalFormatting sqref="J44 J29:J33">
     <cfRule type="expression" priority="5" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
       <formula>MOD(ROUND($J35,2),1)&lt;&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J31:J35">
+  <conditionalFormatting sqref="J44 J31:J33">
     <cfRule type="expression" priority="6" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="4">
       <formula>MOD(ROUND($J35,2),1)&lt;&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J31:J35">
+  <conditionalFormatting sqref="J44 J31:J33">
     <cfRule type="expression" priority="7" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="5">
       <formula>MOD(ROUND($J35,2),1)&lt;&gt;0</formula>
     </cfRule>
@@ -3032,34 +3812,34 @@
       <formula>MOD(ROUND($K30,2),1)&lt;&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J30:J35">
+  <conditionalFormatting sqref="J44 J30:J33">
     <cfRule type="expression" priority="14" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="12">
       <formula>MOD(ROUND($J35,2),1)&lt;&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J32:J35">
+  <conditionalFormatting sqref="J44 J32:J33">
     <cfRule type="expression" priority="15" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="13">
       <formula>MOD(ROUND($J35,2),1)&lt;&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J32:J35">
+  <conditionalFormatting sqref="J44 J32:J33">
     <cfRule type="expression" priority="16" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="14">
       <formula>MOD(ROUND($J35,2),1)&lt;&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F29:W35">
+  <conditionalFormatting sqref="F44:W44 F29:W33">
     <cfRule type="expression" priority="17" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="15">
       <formula>$F35="Оборот / Итого"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F30:X35">
+  <conditionalFormatting sqref="F44:X44 F30:X33">
     <cfRule type="expression" priority="18" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="16">
       <formula>$F35="Оборот / Итого"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K42:K43">
+  <conditionalFormatting sqref="K51:K52">
     <cfRule type="expression" priority="19" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="17">
-      <formula>MOD(ROUND($K43,2),1)&lt;&gt;0</formula>
+      <formula>MOD(ROUND($K52,2),1)&lt;&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D26:F28">
@@ -3095,6 +3875,36 @@
   <conditionalFormatting sqref="H26:H28">
     <cfRule type="expression" priority="26" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="24">
       <formula>MOD(ROUND($H26,2),1)&lt;&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J37:J42">
+    <cfRule type="expression" priority="27" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="25">
+      <formula>MOD(ROUND($J37,2),1)&lt;&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J42:J43">
+    <cfRule type="expression" priority="28" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="26">
+      <formula>MOD(ROUND($J44,2),1)&lt;&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J42:J43">
+    <cfRule type="expression" priority="29" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="27">
+      <formula>MOD(ROUND($J44,2),1)&lt;&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J43">
+    <cfRule type="expression" priority="30" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="28">
+      <formula>MOD(ROUND($J44,2),1)&lt;&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="X38:X40 F37:W42">
+    <cfRule type="expression" priority="31" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="29">
+      <formula>$F37="Оборот / Итого"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F42:X43">
+    <cfRule type="expression" priority="32" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="30">
+      <formula>$F44="Оборот / Итого"</formula>
     </cfRule>
   </conditionalFormatting>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -3152,136 +3962,136 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="105" t="s">
-        <v>114</v>
-      </c>
-      <c r="V1" s="106" t="s">
-        <v>115</v>
+      <c r="A1" s="116" t="s">
+        <v>151</v>
+      </c>
+      <c r="V1" s="117" t="s">
+        <v>152</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="V2" s="106" t="s">
-        <v>116</v>
+      <c r="V2" s="117" t="s">
+        <v>153</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="V3" s="106" t="s">
-        <v>117</v>
+      <c r="V3" s="117" t="s">
+        <v>154</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="V4" s="106" t="s">
-        <v>118</v>
+      <c r="V4" s="117" t="s">
+        <v>155</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="V5" s="106" t="s">
-        <v>119</v>
+      <c r="V5" s="117" t="s">
+        <v>156</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="V6" s="106" t="s">
-        <v>120</v>
+      <c r="V6" s="117" t="s">
+        <v>157</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="V7" s="106" t="s">
-        <v>121</v>
+      <c r="V7" s="117" t="s">
+        <v>158</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="V8" s="106" t="s">
-        <v>122</v>
+      <c r="V8" s="117" t="s">
+        <v>159</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="V9" s="106" t="s">
-        <v>123</v>
+      <c r="V9" s="117" t="s">
+        <v>160</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="V10" s="106" t="s">
-        <v>124</v>
+      <c r="V10" s="117" t="s">
+        <v>161</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="V11" s="106" t="s">
-        <v>125</v>
+      <c r="V11" s="117" t="s">
+        <v>162</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="V12" s="106" t="s">
-        <v>126</v>
+      <c r="V12" s="117" t="s">
+        <v>163</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="V13" s="106" t="s">
-        <v>127</v>
+      <c r="V13" s="117" t="s">
+        <v>164</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="V14" s="106" t="s">
-        <v>128</v>
+      <c r="V14" s="117" t="s">
+        <v>165</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="V15" s="106" t="s">
-        <v>129</v>
+      <c r="V15" s="117" t="s">
+        <v>166</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="V16" s="106" t="s">
-        <v>130</v>
+      <c r="V16" s="117" t="s">
+        <v>167</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="V17" s="106" t="s">
-        <v>131</v>
+      <c r="V17" s="117" t="s">
+        <v>168</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="V18" s="106" t="s">
-        <v>132</v>
+      <c r="V18" s="117" t="s">
+        <v>169</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="106"/>
+      <c r="A20" s="117"/>
     </row>
     <row r="21" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="106"/>
+      <c r="A21" s="117"/>
     </row>
     <row r="22" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="106"/>
+      <c r="A22" s="117"/>
     </row>
     <row r="23" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="106"/>
+      <c r="A23" s="117"/>
     </row>
     <row r="24" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="106"/>
+      <c r="A24" s="117"/>
     </row>
     <row r="25" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="106"/>
+      <c r="A25" s="117"/>
     </row>
     <row r="26" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="106"/>
+      <c r="A26" s="117"/>
     </row>
     <row r="27" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="106"/>
+      <c r="A27" s="117"/>
     </row>
     <row r="28" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="106"/>
+      <c r="A28" s="117"/>
     </row>
     <row r="29" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="106"/>
+      <c r="A29" s="117"/>
     </row>
     <row r="30" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="106"/>
+      <c r="A30" s="117"/>
     </row>
     <row r="31" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="106"/>
+      <c r="A31" s="117"/>
     </row>
     <row r="32" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="106"/>
+      <c r="A32" s="117"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
Class KITFinance was replaced with StatementKIT (based on StatementXLS) in order to load statements via intermediate JSON validation. Test set was updated.
</commit_message>
<xml_diff>
--- a/tests/test_data/kit.xlsx
+++ b/tests/test_data/kit.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="181">
   <si>
     <t xml:space="preserve">КИТ Финанс (АО)</t>
   </si>
@@ -402,6 +402,39 @@
   </si>
   <si>
     <t xml:space="preserve">Основной рынок</t>
+  </si>
+  <si>
+    <t xml:space="preserve">% по займу ЦБ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">договор займа от 16.04.2021</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Проценты по договору займа ЦБ ДЗ/16042021-1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Внесение д/с в торг</t>
+  </si>
+  <si>
+    <t xml:space="preserve">зачисление - неторговое поручение от 15.03.2021</t>
+  </si>
+  <si>
+    <t xml:space="preserve">НП/в/А/150321/74123</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Комиссия НРД</t>
+  </si>
+  <si>
+    <t xml:space="preserve">счет от 28.05.2021</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Счет НКО АО НРД за хранение ЦБ №H000/02923468 от 28.05.2021 г.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ком бр аб плата спот</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Абонентская плата за обслуживание счета 11249</t>
   </si>
   <si>
     <t xml:space="preserve">Дивиденды, купоны и частичные погашения</t>
@@ -922,7 +955,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="118">
+  <cellXfs count="124">
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1253,6 +1286,30 @@
     </xf>
     <xf numFmtId="165" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="174" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -1405,7 +1462,7 @@
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
     <cellStyle name="Обычный 2" xfId="20"/>
   </cellStyles>
-  <dxfs count="31">
+  <dxfs count="32">
     <dxf>
       <font>
         <b val="1"/>
@@ -1604,6 +1661,16 @@
         <sz val="11"/>
       </font>
     </dxf>
+    <dxf>
+      <font>
+        <name val="Calibri"/>
+        <charset val="204"/>
+        <family val="2"/>
+        <color rgb="FF000000"/>
+        <sz val="11"/>
+      </font>
+      <numFmt numFmtId="164" formatCode="#,##0.0##########"/>
+    </dxf>
   </dxfs>
   <colors>
     <indexedColors>
@@ -1679,9 +1746,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>202320</xdr:colOff>
+      <xdr:colOff>201960</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>19440</xdr:rowOff>
+      <xdr:rowOff>19080</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1695,7 +1762,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="2741040" cy="689760"/>
+          <a:ext cx="2740680" cy="689400"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1715,10 +1782,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="true"/>
   </sheetPr>
-  <dimension ref="A1:AD63"/>
+  <dimension ref="A1:AD1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="M19" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="V41" activeCellId="0" sqref="V41"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A22" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="M49" activeCellId="0" sqref="M49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="1" outlineLevelCol="0"/>
@@ -3237,246 +3304,287 @@
       </c>
       <c r="R46" s="81"/>
     </row>
-    <row r="47" s="1" customFormat="true" ht="17.1" hidden="false" customHeight="true" outlineLevel="1" collapsed="false">
-      <c r="A47" s="48"/>
-      <c r="B47" s="48"/>
-      <c r="C47" s="48"/>
-      <c r="D47" s="48"/>
-      <c r="E47" s="48"/>
-      <c r="F47" s="48"/>
-      <c r="G47" s="48"/>
-      <c r="H47" s="83"/>
-      <c r="I47" s="75"/>
-      <c r="J47" s="75"/>
-      <c r="K47" s="48"/>
-      <c r="L47" s="48"/>
-      <c r="M47" s="48"/>
-      <c r="N47" s="48"/>
-      <c r="O47" s="84"/>
-      <c r="P47" s="75"/>
-      <c r="Q47" s="75"/>
-      <c r="R47" s="75"/>
-    </row>
-    <row r="48" s="16" customFormat="true" ht="17.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A48" s="29" t="s">
+    <row r="47" s="16" customFormat="true" ht="12.8" hidden="false" customHeight="true" outlineLevel="1" collapsed="false">
+      <c r="A47" s="64" t="n">
+        <v>44303</v>
+      </c>
+      <c r="B47" s="36" t="s">
         <v>117</v>
       </c>
-      <c r="B48" s="29"/>
-      <c r="C48" s="29"/>
-      <c r="D48" s="29"/>
-      <c r="E48" s="85"/>
-      <c r="F48" s="85"/>
-      <c r="G48" s="85"/>
-      <c r="H48" s="55"/>
-      <c r="I48" s="86"/>
-      <c r="J48" s="87"/>
-      <c r="K48" s="27"/>
-      <c r="L48" s="27"/>
-      <c r="M48" s="27"/>
-      <c r="N48" s="27"/>
-      <c r="O48" s="27"/>
-      <c r="P48" s="27"/>
-    </row>
-    <row r="49" s="91" customFormat="true" ht="56.7" hidden="false" customHeight="true" outlineLevel="1" collapsed="false">
-      <c r="A49" s="78" t="s">
+      <c r="C47" s="36"/>
+      <c r="D47" s="36"/>
+      <c r="E47" s="36"/>
+      <c r="F47" s="36"/>
+      <c r="G47" s="80" t="n">
+        <v>43.21</v>
+      </c>
+      <c r="H47" s="81" t="s">
+        <v>50</v>
+      </c>
+      <c r="I47" s="82" t="s">
         <v>118</v>
       </c>
-      <c r="B49" s="78"/>
-      <c r="C49" s="78"/>
-      <c r="D49" s="88" t="s">
+      <c r="J47" s="82"/>
+      <c r="K47" s="82"/>
+      <c r="L47" s="82"/>
+      <c r="M47" s="73" t="s">
         <v>119</v>
       </c>
-      <c r="E49" s="88" t="s">
+      <c r="N47" s="73"/>
+      <c r="O47" s="73"/>
+      <c r="P47" s="73"/>
+      <c r="Q47" s="81" t="s">
+        <v>116</v>
+      </c>
+      <c r="R47" s="81"/>
+    </row>
+    <row r="48" s="88" customFormat="true" ht="15.3" hidden="false" customHeight="true" outlineLevel="1" collapsed="false">
+      <c r="A48" s="83" t="n">
+        <v>44270</v>
+      </c>
+      <c r="B48" s="84" t="s">
         <v>120</v>
       </c>
-      <c r="F49" s="88" t="s">
+      <c r="C48" s="84"/>
+      <c r="D48" s="84"/>
+      <c r="E48" s="84"/>
+      <c r="F48" s="84"/>
+      <c r="G48" s="80" t="n">
+        <v>123</v>
+      </c>
+      <c r="H48" s="85" t="s">
+        <v>50</v>
+      </c>
+      <c r="I48" s="86" t="s">
         <v>121</v>
       </c>
-      <c r="G49" s="88" t="s">
+      <c r="J48" s="86"/>
+      <c r="K48" s="86"/>
+      <c r="L48" s="86"/>
+      <c r="M48" s="87" t="s">
         <v>122</v>
       </c>
-      <c r="H49" s="89" t="s">
+      <c r="N48" s="87"/>
+      <c r="O48" s="87"/>
+      <c r="P48" s="87"/>
+      <c r="Q48" s="85" t="s">
+        <v>116</v>
+      </c>
+      <c r="R48" s="85"/>
+    </row>
+    <row r="49" s="88" customFormat="true" ht="12.8" hidden="false" customHeight="true" outlineLevel="1" collapsed="false">
+      <c r="A49" s="83" t="n">
+        <v>44346</v>
+      </c>
+      <c r="B49" s="84" t="s">
         <v>123</v>
       </c>
-      <c r="I49" s="89" t="s">
+      <c r="C49" s="84"/>
+      <c r="D49" s="84"/>
+      <c r="E49" s="84"/>
+      <c r="F49" s="84"/>
+      <c r="G49" s="80" t="n">
+        <v>-17.6</v>
+      </c>
+      <c r="H49" s="85" t="s">
+        <v>50</v>
+      </c>
+      <c r="I49" s="86" t="s">
         <v>124</v>
       </c>
-      <c r="J49" s="89" t="s">
+      <c r="J49" s="86"/>
+      <c r="K49" s="86"/>
+      <c r="L49" s="86"/>
+      <c r="M49" s="87" t="s">
         <v>125</v>
       </c>
-      <c r="K49" s="78" t="s">
+      <c r="N49" s="87"/>
+      <c r="O49" s="87"/>
+      <c r="P49" s="87"/>
+      <c r="Q49" s="85" t="s">
+        <v>116</v>
+      </c>
+      <c r="R49" s="85"/>
+    </row>
+    <row r="50" s="88" customFormat="true" ht="15.3" hidden="false" customHeight="true" outlineLevel="1" collapsed="false">
+      <c r="A50" s="83" t="n">
+        <v>44286</v>
+      </c>
+      <c r="B50" s="84" t="s">
         <v>126</v>
       </c>
-      <c r="L49" s="78"/>
-      <c r="M49" s="78"/>
-      <c r="N49" s="79" t="s">
-        <v>112</v>
-      </c>
-      <c r="O49" s="79"/>
-      <c r="P49" s="90"/>
-      <c r="Q49" s="90" t="s">
+      <c r="C50" s="84"/>
+      <c r="D50" s="84"/>
+      <c r="E50" s="84"/>
+      <c r="F50" s="84"/>
+      <c r="G50" s="80" t="n">
+        <v>-200</v>
+      </c>
+      <c r="H50" s="85" t="s">
+        <v>50</v>
+      </c>
+      <c r="I50" s="86"/>
+      <c r="J50" s="86"/>
+      <c r="K50" s="86"/>
+      <c r="L50" s="86"/>
+      <c r="M50" s="87" t="s">
         <v>127</v>
       </c>
-      <c r="R49" s="90"/>
-      <c r="S49" s="90"/>
-    </row>
-    <row r="50" s="91" customFormat="true" ht="29.7" hidden="false" customHeight="true" outlineLevel="1" collapsed="false">
-      <c r="A50" s="92" t="s">
+      <c r="N50" s="87"/>
+      <c r="O50" s="87"/>
+      <c r="P50" s="87"/>
+      <c r="Q50" s="85" t="s">
+        <v>116</v>
+      </c>
+      <c r="R50" s="85"/>
+    </row>
+    <row r="51" s="1" customFormat="true" ht="17.1" hidden="false" customHeight="true" outlineLevel="1" collapsed="false">
+      <c r="A51" s="48"/>
+      <c r="B51" s="48"/>
+      <c r="C51" s="48"/>
+      <c r="D51" s="48"/>
+      <c r="E51" s="48"/>
+      <c r="F51" s="48"/>
+      <c r="G51" s="48"/>
+      <c r="H51" s="89"/>
+      <c r="I51" s="75"/>
+      <c r="J51" s="75"/>
+      <c r="K51" s="48"/>
+      <c r="L51" s="48"/>
+      <c r="M51" s="48"/>
+      <c r="N51" s="48"/>
+      <c r="O51" s="90"/>
+      <c r="P51" s="75"/>
+      <c r="Q51" s="75"/>
+      <c r="R51" s="75"/>
+    </row>
+    <row r="52" s="16" customFormat="true" ht="17.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A52" s="29" t="s">
         <v>128</v>
-      </c>
-      <c r="B50" s="92"/>
-      <c r="C50" s="92"/>
-      <c r="D50" s="93" t="n">
-        <v>44210</v>
-      </c>
-      <c r="E50" s="94" t="n">
-        <v>2600</v>
-      </c>
-      <c r="F50" s="67" t="n">
-        <v>2.391</v>
-      </c>
-      <c r="G50" s="95" t="n">
-        <v>6216.6</v>
-      </c>
-      <c r="H50" s="96" t="n">
-        <v>6216.6</v>
-      </c>
-      <c r="I50" s="97" t="s">
-        <v>50</v>
-      </c>
-      <c r="J50" s="98" t="n">
-        <v>44223</v>
-      </c>
-      <c r="K50" s="92" t="s">
-        <v>129</v>
-      </c>
-      <c r="L50" s="92"/>
-      <c r="M50" s="92"/>
-      <c r="N50" s="81" t="s">
-        <v>116</v>
-      </c>
-      <c r="O50" s="81"/>
-      <c r="P50" s="90"/>
-      <c r="Q50" s="90"/>
-      <c r="R50" s="90"/>
-      <c r="S50" s="90"/>
-    </row>
-    <row r="51" s="103" customFormat="true" ht="13.2" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
-      <c r="A51" s="99"/>
-      <c r="B51" s="99"/>
-      <c r="C51" s="99"/>
-      <c r="D51" s="100"/>
-      <c r="E51" s="99"/>
-      <c r="F51" s="100"/>
-      <c r="G51" s="100"/>
-      <c r="H51" s="100"/>
-      <c r="I51" s="101"/>
-      <c r="J51" s="100"/>
-      <c r="K51" s="99"/>
-      <c r="L51" s="99"/>
-      <c r="M51" s="99"/>
-      <c r="N51" s="102"/>
-      <c r="O51" s="102"/>
-      <c r="P51" s="90"/>
-      <c r="Q51" s="90"/>
-      <c r="R51" s="90"/>
-    </row>
-    <row r="52" s="15" customFormat="true" ht="17.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A52" s="29" t="s">
-        <v>130</v>
       </c>
       <c r="B52" s="29"/>
       <c r="C52" s="29"/>
       <c r="D52" s="29"/>
-      <c r="E52" s="29"/>
-      <c r="F52" s="29"/>
-      <c r="G52" s="29"/>
-      <c r="H52" s="29"/>
-      <c r="I52" s="29"/>
-      <c r="J52" s="29"/>
-      <c r="K52" s="29"/>
-      <c r="L52" s="29"/>
-      <c r="M52" s="29"/>
-      <c r="N52" s="22"/>
-      <c r="O52" s="22"/>
-      <c r="P52" s="104"/>
-    </row>
-    <row r="53" s="15" customFormat="true" ht="43.2" hidden="false" customHeight="true" outlineLevel="1" collapsed="false">
-      <c r="A53" s="88" t="s">
-        <v>73</v>
-      </c>
-      <c r="B53" s="88"/>
-      <c r="C53" s="88"/>
-      <c r="D53" s="88" t="s">
+      <c r="E52" s="91"/>
+      <c r="F52" s="91"/>
+      <c r="G52" s="91"/>
+      <c r="H52" s="55"/>
+      <c r="I52" s="92"/>
+      <c r="J52" s="93"/>
+      <c r="K52" s="27"/>
+      <c r="L52" s="27"/>
+      <c r="M52" s="27"/>
+      <c r="N52" s="27"/>
+      <c r="O52" s="27"/>
+      <c r="P52" s="27"/>
+    </row>
+    <row r="53" s="97" customFormat="true" ht="56.7" hidden="false" customHeight="true" outlineLevel="1" collapsed="false">
+      <c r="A53" s="78" t="s">
+        <v>129</v>
+      </c>
+      <c r="B53" s="78"/>
+      <c r="C53" s="78"/>
+      <c r="D53" s="94" t="s">
+        <v>130</v>
+      </c>
+      <c r="E53" s="94" t="s">
         <v>131</v>
       </c>
-      <c r="E53" s="88"/>
-      <c r="F53" s="88" t="s">
+      <c r="F53" s="94" t="s">
         <v>132</v>
       </c>
-      <c r="G53" s="88"/>
-      <c r="H53" s="88" t="s">
+      <c r="G53" s="94" t="s">
         <v>133</v>
       </c>
-      <c r="I53" s="88"/>
-      <c r="J53" s="88" t="s">
+      <c r="H53" s="95" t="s">
         <v>134</v>
       </c>
-      <c r="K53" s="88"/>
-      <c r="L53" s="88" t="s">
+      <c r="I53" s="95" t="s">
         <v>135</v>
       </c>
-      <c r="M53" s="88"/>
-      <c r="N53" s="88" t="s">
+      <c r="J53" s="95" t="s">
         <v>136</v>
       </c>
-      <c r="O53" s="88"/>
-      <c r="P53" s="22"/>
-      <c r="Q53" s="22"/>
-      <c r="R53" s="104"/>
-    </row>
-    <row r="54" s="15" customFormat="true" ht="17.1" hidden="false" customHeight="true" outlineLevel="1" collapsed="false">
-      <c r="A54" s="97" t="s">
+      <c r="K53" s="78" t="s">
         <v>137</v>
       </c>
-      <c r="B54" s="97"/>
-      <c r="C54" s="97"/>
-      <c r="D54" s="97"/>
-      <c r="E54" s="97"/>
-      <c r="F54" s="97"/>
-      <c r="G54" s="97"/>
-      <c r="H54" s="105"/>
-      <c r="I54" s="105"/>
-      <c r="J54" s="97"/>
-      <c r="K54" s="97"/>
-      <c r="L54" s="97"/>
-      <c r="M54" s="97"/>
-      <c r="N54" s="97"/>
-      <c r="O54" s="97"/>
-      <c r="P54" s="22"/>
-      <c r="Q54" s="22"/>
-      <c r="R54" s="104"/>
-    </row>
-    <row r="55" s="51" customFormat="true" ht="17.1" hidden="false" customHeight="true" outlineLevel="1" collapsed="false">
-      <c r="A55" s="106"/>
-      <c r="B55" s="106"/>
-      <c r="C55" s="106"/>
+      <c r="L53" s="78"/>
+      <c r="M53" s="78"/>
+      <c r="N53" s="79" t="s">
+        <v>112</v>
+      </c>
+      <c r="O53" s="79"/>
+      <c r="P53" s="96"/>
+      <c r="Q53" s="96" t="s">
+        <v>138</v>
+      </c>
+      <c r="R53" s="96"/>
+      <c r="S53" s="96"/>
+    </row>
+    <row r="54" s="97" customFormat="true" ht="29.7" hidden="false" customHeight="true" outlineLevel="1" collapsed="false">
+      <c r="A54" s="98" t="s">
+        <v>139</v>
+      </c>
+      <c r="B54" s="98"/>
+      <c r="C54" s="98"/>
+      <c r="D54" s="99" t="n">
+        <v>44210</v>
+      </c>
+      <c r="E54" s="100" t="n">
+        <v>2600</v>
+      </c>
+      <c r="F54" s="67" t="n">
+        <v>2.391</v>
+      </c>
+      <c r="G54" s="101" t="n">
+        <v>6216.6</v>
+      </c>
+      <c r="H54" s="102" t="n">
+        <v>6216.6</v>
+      </c>
+      <c r="I54" s="103" t="s">
+        <v>50</v>
+      </c>
+      <c r="J54" s="104" t="n">
+        <v>44223</v>
+      </c>
+      <c r="K54" s="98" t="s">
+        <v>140</v>
+      </c>
+      <c r="L54" s="98"/>
+      <c r="M54" s="98"/>
+      <c r="N54" s="81" t="s">
+        <v>116</v>
+      </c>
+      <c r="O54" s="81"/>
+      <c r="P54" s="96"/>
+      <c r="Q54" s="96"/>
+      <c r="R54" s="96"/>
+      <c r="S54" s="96"/>
+    </row>
+    <row r="55" s="109" customFormat="true" ht="13.2" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
+      <c r="A55" s="105"/>
+      <c r="B55" s="105"/>
+      <c r="C55" s="105"/>
       <c r="D55" s="106"/>
-      <c r="E55" s="106"/>
+      <c r="E55" s="105"/>
       <c r="F55" s="106"/>
       <c r="G55" s="106"/>
       <c r="H55" s="106"/>
-      <c r="I55" s="106"/>
+      <c r="I55" s="107"/>
       <c r="J55" s="106"/>
-      <c r="K55" s="106"/>
-      <c r="L55" s="106"/>
-      <c r="M55" s="75"/>
-      <c r="N55" s="106"/>
-      <c r="O55" s="106"/>
+      <c r="K55" s="105"/>
+      <c r="L55" s="105"/>
+      <c r="M55" s="105"/>
+      <c r="N55" s="108"/>
+      <c r="O55" s="108"/>
+      <c r="P55" s="96"/>
+      <c r="Q55" s="96"/>
+      <c r="R55" s="96"/>
     </row>
     <row r="56" s="15" customFormat="true" ht="17.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A56" s="29" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="B56" s="29"/>
       <c r="C56" s="29"/>
@@ -3492,166 +3600,264 @@
       <c r="M56" s="29"/>
       <c r="N56" s="22"/>
       <c r="O56" s="22"/>
-      <c r="P56" s="104"/>
-    </row>
-    <row r="57" s="109" customFormat="true" ht="56.7" hidden="false" customHeight="true" outlineLevel="1" collapsed="false">
-      <c r="A57" s="33" t="s">
-        <v>139</v>
-      </c>
-      <c r="B57" s="33"/>
-      <c r="C57" s="33" t="s">
-        <v>140</v>
-      </c>
-      <c r="D57" s="33"/>
-      <c r="E57" s="30" t="s">
-        <v>141</v>
-      </c>
-      <c r="F57" s="30"/>
-      <c r="G57" s="30" t="s">
+      <c r="P56" s="110"/>
+    </row>
+    <row r="57" s="15" customFormat="true" ht="43.2" hidden="false" customHeight="true" outlineLevel="1" collapsed="false">
+      <c r="A57" s="94" t="s">
+        <v>73</v>
+      </c>
+      <c r="B57" s="94"/>
+      <c r="C57" s="94"/>
+      <c r="D57" s="94" t="s">
         <v>142</v>
       </c>
-      <c r="H57" s="30"/>
-      <c r="I57" s="30" t="s">
+      <c r="E57" s="94"/>
+      <c r="F57" s="94" t="s">
         <v>143</v>
       </c>
-      <c r="J57" s="30"/>
-      <c r="K57" s="30" t="s">
+      <c r="G57" s="94"/>
+      <c r="H57" s="94" t="s">
         <v>144</v>
       </c>
-      <c r="L57" s="30"/>
-      <c r="M57" s="30" t="s">
+      <c r="I57" s="94"/>
+      <c r="J57" s="94" t="s">
         <v>145</v>
       </c>
-      <c r="N57" s="30"/>
-      <c r="O57" s="30" t="s">
+      <c r="K57" s="94"/>
+      <c r="L57" s="94" t="s">
         <v>146</v>
       </c>
-      <c r="P57" s="30"/>
-      <c r="Q57" s="30" t="s">
+      <c r="M57" s="94"/>
+      <c r="N57" s="94" t="s">
         <v>147</v>
       </c>
-      <c r="R57" s="30"/>
-      <c r="S57" s="107"/>
-      <c r="T57" s="107"/>
-      <c r="U57" s="107"/>
-      <c r="V57" s="107"/>
-      <c r="W57" s="108"/>
+      <c r="O57" s="94"/>
+      <c r="P57" s="22"/>
+      <c r="Q57" s="22"/>
+      <c r="R57" s="110"/>
     </row>
     <row r="58" s="15" customFormat="true" ht="17.1" hidden="false" customHeight="true" outlineLevel="1" collapsed="false">
-      <c r="A58" s="110" t="s">
+      <c r="A58" s="103" t="s">
+        <v>148</v>
+      </c>
+      <c r="B58" s="103"/>
+      <c r="C58" s="103"/>
+      <c r="D58" s="103"/>
+      <c r="E58" s="103"/>
+      <c r="F58" s="103"/>
+      <c r="G58" s="103"/>
+      <c r="H58" s="111"/>
+      <c r="I58" s="111"/>
+      <c r="J58" s="103"/>
+      <c r="K58" s="103"/>
+      <c r="L58" s="103"/>
+      <c r="M58" s="103"/>
+      <c r="N58" s="103"/>
+      <c r="O58" s="103"/>
+      <c r="P58" s="22"/>
+      <c r="Q58" s="22"/>
+      <c r="R58" s="110"/>
+    </row>
+    <row r="59" s="51" customFormat="true" ht="17.1" hidden="false" customHeight="true" outlineLevel="1" collapsed="false">
+      <c r="A59" s="112"/>
+      <c r="B59" s="112"/>
+      <c r="C59" s="112"/>
+      <c r="D59" s="112"/>
+      <c r="E59" s="112"/>
+      <c r="F59" s="112"/>
+      <c r="G59" s="112"/>
+      <c r="H59" s="112"/>
+      <c r="I59" s="112"/>
+      <c r="J59" s="112"/>
+      <c r="K59" s="112"/>
+      <c r="L59" s="112"/>
+      <c r="M59" s="75"/>
+      <c r="N59" s="112"/>
+      <c r="O59" s="112"/>
+    </row>
+    <row r="60" s="15" customFormat="true" ht="17.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A60" s="29" t="s">
+        <v>149</v>
+      </c>
+      <c r="B60" s="29"/>
+      <c r="C60" s="29"/>
+      <c r="D60" s="29"/>
+      <c r="E60" s="29"/>
+      <c r="F60" s="29"/>
+      <c r="G60" s="29"/>
+      <c r="H60" s="29"/>
+      <c r="I60" s="29"/>
+      <c r="J60" s="29"/>
+      <c r="K60" s="29"/>
+      <c r="L60" s="29"/>
+      <c r="M60" s="29"/>
+      <c r="N60" s="22"/>
+      <c r="O60" s="22"/>
+      <c r="P60" s="110"/>
+    </row>
+    <row r="61" s="115" customFormat="true" ht="56.7" hidden="false" customHeight="true" outlineLevel="1" collapsed="false">
+      <c r="A61" s="33" t="s">
+        <v>150</v>
+      </c>
+      <c r="B61" s="33"/>
+      <c r="C61" s="33" t="s">
+        <v>151</v>
+      </c>
+      <c r="D61" s="33"/>
+      <c r="E61" s="30" t="s">
+        <v>152</v>
+      </c>
+      <c r="F61" s="30"/>
+      <c r="G61" s="30" t="s">
+        <v>153</v>
+      </c>
+      <c r="H61" s="30"/>
+      <c r="I61" s="30" t="s">
+        <v>154</v>
+      </c>
+      <c r="J61" s="30"/>
+      <c r="K61" s="30" t="s">
+        <v>155</v>
+      </c>
+      <c r="L61" s="30"/>
+      <c r="M61" s="30" t="s">
+        <v>156</v>
+      </c>
+      <c r="N61" s="30"/>
+      <c r="O61" s="30" t="s">
+        <v>157</v>
+      </c>
+      <c r="P61" s="30"/>
+      <c r="Q61" s="30" t="s">
+        <v>158</v>
+      </c>
+      <c r="R61" s="30"/>
+      <c r="S61" s="113"/>
+      <c r="T61" s="113"/>
+      <c r="U61" s="113"/>
+      <c r="V61" s="113"/>
+      <c r="W61" s="114"/>
+    </row>
+    <row r="62" s="15" customFormat="true" ht="17.1" hidden="false" customHeight="true" outlineLevel="1" collapsed="false">
+      <c r="A62" s="116" t="s">
         <v>66</v>
       </c>
-      <c r="B58" s="110"/>
-      <c r="C58" s="110"/>
-      <c r="D58" s="110"/>
-      <c r="E58" s="110"/>
-      <c r="F58" s="110"/>
-      <c r="G58" s="110"/>
-      <c r="H58" s="110"/>
-      <c r="I58" s="110"/>
-      <c r="J58" s="110"/>
-      <c r="K58" s="110"/>
-      <c r="L58" s="110"/>
-      <c r="M58" s="110"/>
-      <c r="N58" s="110"/>
-      <c r="O58" s="111"/>
-      <c r="P58" s="111"/>
-      <c r="Q58" s="111"/>
-      <c r="R58" s="111"/>
-      <c r="S58" s="22"/>
-      <c r="T58" s="22"/>
-      <c r="U58" s="22"/>
-      <c r="V58" s="22"/>
-      <c r="W58" s="104"/>
-    </row>
-    <row r="59" s="1" customFormat="true" ht="17.1" hidden="false" customHeight="true" outlineLevel="1" collapsed="false">
-      <c r="A59" s="49"/>
-      <c r="B59" s="49"/>
-      <c r="C59" s="49"/>
-      <c r="D59" s="49"/>
-      <c r="E59" s="49"/>
-      <c r="F59" s="49"/>
-      <c r="G59" s="49"/>
-      <c r="H59" s="49"/>
-      <c r="I59" s="49"/>
-      <c r="J59" s="49"/>
-      <c r="K59" s="49"/>
-      <c r="L59" s="49"/>
-      <c r="M59" s="49"/>
-      <c r="N59" s="75"/>
-      <c r="O59" s="49"/>
-      <c r="P59" s="49"/>
-      <c r="Q59" s="49"/>
-      <c r="R59" s="75"/>
-    </row>
-    <row r="60" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A60" s="112"/>
-      <c r="B60" s="112"/>
-      <c r="C60" s="112"/>
-      <c r="D60" s="112"/>
-      <c r="E60" s="112"/>
-      <c r="F60" s="22"/>
-      <c r="G60" s="22"/>
-      <c r="H60" s="22"/>
-      <c r="I60" s="22"/>
-      <c r="J60" s="22"/>
-      <c r="K60" s="22"/>
-      <c r="L60" s="22"/>
-      <c r="M60" s="22"/>
-    </row>
-    <row r="61" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A61" s="113"/>
-      <c r="B61" s="112"/>
-      <c r="C61" s="112"/>
-      <c r="D61" s="112"/>
-      <c r="E61" s="112"/>
-      <c r="F61" s="22"/>
-      <c r="G61" s="22"/>
-      <c r="H61" s="22"/>
-      <c r="I61" s="22"/>
-      <c r="J61" s="22"/>
-      <c r="K61" s="22"/>
-      <c r="L61" s="22"/>
-      <c r="M61" s="22"/>
-    </row>
-    <row r="62" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A62" s="114" t="s">
-        <v>148</v>
-      </c>
-      <c r="B62" s="114"/>
-      <c r="C62" s="114"/>
-      <c r="D62" s="114"/>
-      <c r="E62" s="114"/>
-      <c r="F62" s="114"/>
-      <c r="G62" s="114"/>
-      <c r="H62" s="22"/>
-      <c r="I62" s="22"/>
-      <c r="J62" s="22"/>
-      <c r="K62" s="22"/>
-      <c r="L62" s="22"/>
-      <c r="M62" s="22"/>
-    </row>
-    <row r="63" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A63" s="115" t="s">
-        <v>149</v>
-      </c>
-      <c r="B63" s="115"/>
-      <c r="C63" s="115"/>
-      <c r="D63" s="14" t="s">
-        <v>150</v>
-      </c>
-      <c r="E63" s="14"/>
-      <c r="F63" s="22"/>
-      <c r="G63" s="22"/>
-      <c r="H63" s="22"/>
-      <c r="I63" s="22"/>
-      <c r="J63" s="22"/>
-      <c r="K63" s="22"/>
-      <c r="L63" s="22"/>
-      <c r="M63" s="22"/>
-    </row>
+      <c r="B62" s="116"/>
+      <c r="C62" s="116"/>
+      <c r="D62" s="116"/>
+      <c r="E62" s="116"/>
+      <c r="F62" s="116"/>
+      <c r="G62" s="116"/>
+      <c r="H62" s="116"/>
+      <c r="I62" s="116"/>
+      <c r="J62" s="116"/>
+      <c r="K62" s="116"/>
+      <c r="L62" s="116"/>
+      <c r="M62" s="116"/>
+      <c r="N62" s="116"/>
+      <c r="O62" s="117"/>
+      <c r="P62" s="117"/>
+      <c r="Q62" s="117"/>
+      <c r="R62" s="117"/>
+      <c r="S62" s="22"/>
+      <c r="T62" s="22"/>
+      <c r="U62" s="22"/>
+      <c r="V62" s="22"/>
+      <c r="W62" s="110"/>
+    </row>
+    <row r="63" s="1" customFormat="true" ht="17.1" hidden="false" customHeight="true" outlineLevel="1" collapsed="false">
+      <c r="A63" s="49"/>
+      <c r="B63" s="49"/>
+      <c r="C63" s="49"/>
+      <c r="D63" s="49"/>
+      <c r="E63" s="49"/>
+      <c r="F63" s="49"/>
+      <c r="G63" s="49"/>
+      <c r="H63" s="49"/>
+      <c r="I63" s="49"/>
+      <c r="J63" s="49"/>
+      <c r="K63" s="49"/>
+      <c r="L63" s="49"/>
+      <c r="M63" s="49"/>
+      <c r="N63" s="75"/>
+      <c r="O63" s="49"/>
+      <c r="P63" s="49"/>
+      <c r="Q63" s="49"/>
+      <c r="R63" s="75"/>
+    </row>
+    <row r="64" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A64" s="118"/>
+      <c r="B64" s="118"/>
+      <c r="C64" s="118"/>
+      <c r="D64" s="118"/>
+      <c r="E64" s="118"/>
+      <c r="F64" s="22"/>
+      <c r="G64" s="22"/>
+      <c r="H64" s="22"/>
+      <c r="I64" s="22"/>
+      <c r="J64" s="22"/>
+      <c r="K64" s="22"/>
+      <c r="L64" s="22"/>
+      <c r="M64" s="22"/>
+    </row>
+    <row r="65" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A65" s="119"/>
+      <c r="B65" s="118"/>
+      <c r="C65" s="118"/>
+      <c r="D65" s="118"/>
+      <c r="E65" s="118"/>
+      <c r="F65" s="22"/>
+      <c r="G65" s="22"/>
+      <c r="H65" s="22"/>
+      <c r="I65" s="22"/>
+      <c r="J65" s="22"/>
+      <c r="K65" s="22"/>
+      <c r="L65" s="22"/>
+      <c r="M65" s="22"/>
+    </row>
+    <row r="66" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A66" s="120" t="s">
+        <v>159</v>
+      </c>
+      <c r="B66" s="120"/>
+      <c r="C66" s="120"/>
+      <c r="D66" s="120"/>
+      <c r="E66" s="120"/>
+      <c r="F66" s="120"/>
+      <c r="G66" s="120"/>
+      <c r="H66" s="22"/>
+      <c r="I66" s="22"/>
+      <c r="J66" s="22"/>
+      <c r="K66" s="22"/>
+      <c r="L66" s="22"/>
+      <c r="M66" s="22"/>
+    </row>
+    <row r="67" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A67" s="121" t="s">
+        <v>160</v>
+      </c>
+      <c r="B67" s="121"/>
+      <c r="C67" s="121"/>
+      <c r="D67" s="14" t="s">
+        <v>161</v>
+      </c>
+      <c r="E67" s="14"/>
+      <c r="F67" s="22"/>
+      <c r="G67" s="22"/>
+      <c r="H67" s="22"/>
+      <c r="I67" s="22"/>
+      <c r="J67" s="22"/>
+      <c r="K67" s="22"/>
+      <c r="L67" s="22"/>
+      <c r="M67" s="22"/>
+    </row>
+    <row r="1048572" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
-  <mergeCells count="101">
+  <mergeCells count="117">
     <mergeCell ref="A6:E6"/>
     <mergeCell ref="F6:W6"/>
     <mergeCell ref="A7:E7"/>
@@ -3710,49 +3916,65 @@
     <mergeCell ref="I46:L46"/>
     <mergeCell ref="M46:P46"/>
     <mergeCell ref="Q46:R46"/>
-    <mergeCell ref="A49:C49"/>
-    <mergeCell ref="K49:M49"/>
-    <mergeCell ref="N49:O49"/>
-    <mergeCell ref="A50:C50"/>
-    <mergeCell ref="K50:M50"/>
-    <mergeCell ref="N50:O50"/>
+    <mergeCell ref="B47:F47"/>
+    <mergeCell ref="I47:L47"/>
+    <mergeCell ref="M47:P47"/>
+    <mergeCell ref="Q47:R47"/>
+    <mergeCell ref="B48:F48"/>
+    <mergeCell ref="I48:L48"/>
+    <mergeCell ref="M48:P48"/>
+    <mergeCell ref="Q48:R48"/>
+    <mergeCell ref="B49:F49"/>
+    <mergeCell ref="I49:L49"/>
+    <mergeCell ref="M49:P49"/>
+    <mergeCell ref="Q49:R49"/>
+    <mergeCell ref="B50:F50"/>
+    <mergeCell ref="I50:L50"/>
+    <mergeCell ref="M50:P50"/>
+    <mergeCell ref="Q50:R50"/>
     <mergeCell ref="A53:C53"/>
-    <mergeCell ref="D53:E53"/>
-    <mergeCell ref="F53:G53"/>
-    <mergeCell ref="H53:I53"/>
-    <mergeCell ref="J53:K53"/>
-    <mergeCell ref="L53:M53"/>
+    <mergeCell ref="K53:M53"/>
     <mergeCell ref="N53:O53"/>
     <mergeCell ref="A54:C54"/>
-    <mergeCell ref="D54:E54"/>
-    <mergeCell ref="F54:G54"/>
-    <mergeCell ref="H54:I54"/>
-    <mergeCell ref="J54:K54"/>
-    <mergeCell ref="L54:M54"/>
+    <mergeCell ref="K54:M54"/>
     <mergeCell ref="N54:O54"/>
-    <mergeCell ref="J55:K55"/>
-    <mergeCell ref="N55:O55"/>
-    <mergeCell ref="A57:B57"/>
-    <mergeCell ref="C57:D57"/>
-    <mergeCell ref="E57:F57"/>
-    <mergeCell ref="G57:H57"/>
-    <mergeCell ref="I57:J57"/>
-    <mergeCell ref="K57:L57"/>
-    <mergeCell ref="M57:N57"/>
-    <mergeCell ref="O57:P57"/>
-    <mergeCell ref="Q57:R57"/>
-    <mergeCell ref="A58:B58"/>
-    <mergeCell ref="C58:D58"/>
-    <mergeCell ref="E58:F58"/>
-    <mergeCell ref="G58:H58"/>
-    <mergeCell ref="I58:J58"/>
-    <mergeCell ref="K58:L58"/>
-    <mergeCell ref="M58:N58"/>
-    <mergeCell ref="O58:P58"/>
-    <mergeCell ref="Q58:R58"/>
-    <mergeCell ref="A62:G62"/>
-    <mergeCell ref="A63:C63"/>
-    <mergeCell ref="D63:E63"/>
+    <mergeCell ref="A57:C57"/>
+    <mergeCell ref="D57:E57"/>
+    <mergeCell ref="F57:G57"/>
+    <mergeCell ref="H57:I57"/>
+    <mergeCell ref="J57:K57"/>
+    <mergeCell ref="L57:M57"/>
+    <mergeCell ref="N57:O57"/>
+    <mergeCell ref="A58:C58"/>
+    <mergeCell ref="D58:E58"/>
+    <mergeCell ref="F58:G58"/>
+    <mergeCell ref="H58:I58"/>
+    <mergeCell ref="J58:K58"/>
+    <mergeCell ref="L58:M58"/>
+    <mergeCell ref="N58:O58"/>
+    <mergeCell ref="J59:K59"/>
+    <mergeCell ref="N59:O59"/>
+    <mergeCell ref="A61:B61"/>
+    <mergeCell ref="C61:D61"/>
+    <mergeCell ref="E61:F61"/>
+    <mergeCell ref="G61:H61"/>
+    <mergeCell ref="I61:J61"/>
+    <mergeCell ref="K61:L61"/>
+    <mergeCell ref="M61:N61"/>
+    <mergeCell ref="O61:P61"/>
+    <mergeCell ref="Q61:R61"/>
+    <mergeCell ref="A62:B62"/>
+    <mergeCell ref="C62:D62"/>
+    <mergeCell ref="E62:F62"/>
+    <mergeCell ref="G62:H62"/>
+    <mergeCell ref="I62:J62"/>
+    <mergeCell ref="K62:L62"/>
+    <mergeCell ref="M62:N62"/>
+    <mergeCell ref="O62:P62"/>
+    <mergeCell ref="Q62:R62"/>
+    <mergeCell ref="A66:G66"/>
+    <mergeCell ref="A67:C67"/>
+    <mergeCell ref="D67:E67"/>
   </mergeCells>
   <conditionalFormatting sqref="A13:AMJ21">
     <cfRule type="expression" priority="2" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
@@ -3762,9 +3984,9 @@
       <formula>$A13="Входящий остаток"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K50:K52">
+  <conditionalFormatting sqref="K54:K56">
     <cfRule type="expression" priority="4" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
-      <formula>MOD(ROUND($K52,2),1)&lt;&gt;0</formula>
+      <formula>MOD(ROUND($K56,2),1)&lt;&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J44 J29:J33">
@@ -3837,9 +4059,9 @@
       <formula>$F35="Оборот / Итого"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K51:K52">
+  <conditionalFormatting sqref="K55:K56">
     <cfRule type="expression" priority="19" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="17">
-      <formula>MOD(ROUND($K52,2),1)&lt;&gt;0</formula>
+      <formula>MOD(ROUND($K56,2),1)&lt;&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D26:F28">
@@ -3907,6 +4129,31 @@
       <formula>$F44="Оборот / Итого"</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="K47">
+    <cfRule type="expression" priority="33" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="8">
+      <formula>MOD(ROUND($K56,2),1)&lt;&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K48">
+    <cfRule type="expression" priority="34" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="31">
+      <formula>MOD(ROUND($K53,2),1)&lt;&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K48">
+    <cfRule type="expression" priority="35" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="26">
+      <formula>MOD(ROUND($K52,2),1)&lt;&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K49:K50">
+    <cfRule type="expression" priority="36" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="31">
+      <formula>MOD(ROUND($K53,2),1)&lt;&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K49:K50">
+    <cfRule type="expression" priority="37" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="26">
+      <formula>MOD(ROUND($K52,2),1)&lt;&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.511805555555555"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1000" pageOrder="downThenOver" orientation="landscape" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -3962,136 +4209,136 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="116" t="s">
-        <v>151</v>
-      </c>
-      <c r="V1" s="117" t="s">
-        <v>152</v>
+      <c r="A1" s="122" t="s">
+        <v>162</v>
+      </c>
+      <c r="V1" s="123" t="s">
+        <v>163</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="V2" s="117" t="s">
-        <v>153</v>
+      <c r="V2" s="123" t="s">
+        <v>164</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="V3" s="117" t="s">
-        <v>154</v>
+      <c r="V3" s="123" t="s">
+        <v>165</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="V4" s="117" t="s">
-        <v>155</v>
+      <c r="V4" s="123" t="s">
+        <v>166</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="V5" s="117" t="s">
-        <v>156</v>
+      <c r="V5" s="123" t="s">
+        <v>167</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="V6" s="117" t="s">
-        <v>157</v>
+      <c r="V6" s="123" t="s">
+        <v>168</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="V7" s="117" t="s">
-        <v>158</v>
+      <c r="V7" s="123" t="s">
+        <v>169</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="V8" s="117" t="s">
-        <v>159</v>
+      <c r="V8" s="123" t="s">
+        <v>170</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="V9" s="117" t="s">
-        <v>160</v>
+      <c r="V9" s="123" t="s">
+        <v>171</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="V10" s="117" t="s">
-        <v>161</v>
+      <c r="V10" s="123" t="s">
+        <v>172</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="V11" s="117" t="s">
-        <v>162</v>
+      <c r="V11" s="123" t="s">
+        <v>173</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="V12" s="117" t="s">
-        <v>163</v>
+      <c r="V12" s="123" t="s">
+        <v>174</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="V13" s="117" t="s">
-        <v>164</v>
+      <c r="V13" s="123" t="s">
+        <v>175</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="V14" s="117" t="s">
-        <v>165</v>
+      <c r="V14" s="123" t="s">
+        <v>176</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="V15" s="117" t="s">
-        <v>166</v>
+      <c r="V15" s="123" t="s">
+        <v>177</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="V16" s="117" t="s">
-        <v>167</v>
+      <c r="V16" s="123" t="s">
+        <v>178</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="V17" s="117" t="s">
-        <v>168</v>
+      <c r="V17" s="123" t="s">
+        <v>179</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="V18" s="117" t="s">
-        <v>169</v>
+      <c r="V18" s="123" t="s">
+        <v>180</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="117"/>
+      <c r="A20" s="123"/>
     </row>
     <row r="21" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="117"/>
+      <c r="A21" s="123"/>
     </row>
     <row r="22" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="117"/>
+      <c r="A22" s="123"/>
     </row>
     <row r="23" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="117"/>
+      <c r="A23" s="123"/>
     </row>
     <row r="24" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="117"/>
+      <c r="A24" s="123"/>
     </row>
     <row r="25" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="117"/>
+      <c r="A25" s="123"/>
     </row>
     <row r="26" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="117"/>
+      <c r="A26" s="123"/>
     </row>
     <row r="27" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="117"/>
+      <c r="A27" s="123"/>
     </row>
     <row r="28" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="117"/>
+      <c r="A28" s="123"/>
     </row>
     <row r="29" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="117"/>
+      <c r="A29" s="123"/>
     </row>
     <row r="30" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="117"/>
+      <c r="A30" s="123"/>
     </row>
     <row r="31" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="117"/>
+      <c r="A31" s="123"/>
     </row>
     <row r="32" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="117"/>
+      <c r="A32" s="123"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
KIT broker statement import improvements
</commit_message>
<xml_diff>
--- a/tests/test_data/kit.xlsx
+++ b/tests/test_data/kit.xlsx
@@ -955,7 +955,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="124">
+  <cellXfs count="118">
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1286,30 +1286,6 @@
     </xf>
     <xf numFmtId="165" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="174" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -1746,9 +1722,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>201960</xdr:colOff>
+      <xdr:colOff>201600</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>19080</xdr:rowOff>
+      <xdr:rowOff>18720</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1762,7 +1738,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="2740680" cy="689400"/>
+          <a:ext cx="2740320" cy="689040"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1784,8 +1760,8 @@
   </sheetPr>
   <dimension ref="A1:AD1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A22" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="M49" activeCellId="0" sqref="M49"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J40" activeCellId="0" sqref="J40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="1" outlineLevelCol="0"/>
@@ -2984,7 +2960,7 @@
         <v>102</v>
       </c>
       <c r="J39" s="37" t="n">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="K39" s="66" t="n">
         <v>100.41</v>
@@ -3338,105 +3314,105 @@
       </c>
       <c r="R47" s="81"/>
     </row>
-    <row r="48" s="88" customFormat="true" ht="15.3" hidden="false" customHeight="true" outlineLevel="1" collapsed="false">
-      <c r="A48" s="83" t="n">
+    <row r="48" s="16" customFormat="true" ht="15.3" hidden="false" customHeight="true" outlineLevel="1" collapsed="false">
+      <c r="A48" s="64" t="n">
         <v>44270</v>
       </c>
-      <c r="B48" s="84" t="s">
+      <c r="B48" s="36" t="s">
         <v>120</v>
       </c>
-      <c r="C48" s="84"/>
-      <c r="D48" s="84"/>
-      <c r="E48" s="84"/>
-      <c r="F48" s="84"/>
+      <c r="C48" s="36"/>
+      <c r="D48" s="36"/>
+      <c r="E48" s="36"/>
+      <c r="F48" s="36"/>
       <c r="G48" s="80" t="n">
         <v>123</v>
       </c>
-      <c r="H48" s="85" t="s">
+      <c r="H48" s="81" t="s">
         <v>50</v>
       </c>
-      <c r="I48" s="86" t="s">
+      <c r="I48" s="82" t="s">
         <v>121</v>
       </c>
-      <c r="J48" s="86"/>
-      <c r="K48" s="86"/>
-      <c r="L48" s="86"/>
-      <c r="M48" s="87" t="s">
+      <c r="J48" s="82"/>
+      <c r="K48" s="82"/>
+      <c r="L48" s="82"/>
+      <c r="M48" s="73" t="s">
         <v>122</v>
       </c>
-      <c r="N48" s="87"/>
-      <c r="O48" s="87"/>
-      <c r="P48" s="87"/>
-      <c r="Q48" s="85" t="s">
+      <c r="N48" s="73"/>
+      <c r="O48" s="73"/>
+      <c r="P48" s="73"/>
+      <c r="Q48" s="81" t="s">
         <v>116</v>
       </c>
-      <c r="R48" s="85"/>
-    </row>
-    <row r="49" s="88" customFormat="true" ht="12.8" hidden="false" customHeight="true" outlineLevel="1" collapsed="false">
-      <c r="A49" s="83" t="n">
+      <c r="R48" s="81"/>
+    </row>
+    <row r="49" s="16" customFormat="true" ht="12.8" hidden="false" customHeight="true" outlineLevel="1" collapsed="false">
+      <c r="A49" s="64" t="n">
         <v>44346</v>
       </c>
-      <c r="B49" s="84" t="s">
+      <c r="B49" s="36" t="s">
         <v>123</v>
       </c>
-      <c r="C49" s="84"/>
-      <c r="D49" s="84"/>
-      <c r="E49" s="84"/>
-      <c r="F49" s="84"/>
+      <c r="C49" s="36"/>
+      <c r="D49" s="36"/>
+      <c r="E49" s="36"/>
+      <c r="F49" s="36"/>
       <c r="G49" s="80" t="n">
         <v>-17.6</v>
       </c>
-      <c r="H49" s="85" t="s">
+      <c r="H49" s="81" t="s">
         <v>50</v>
       </c>
-      <c r="I49" s="86" t="s">
+      <c r="I49" s="82" t="s">
         <v>124</v>
       </c>
-      <c r="J49" s="86"/>
-      <c r="K49" s="86"/>
-      <c r="L49" s="86"/>
-      <c r="M49" s="87" t="s">
+      <c r="J49" s="82"/>
+      <c r="K49" s="82"/>
+      <c r="L49" s="82"/>
+      <c r="M49" s="73" t="s">
         <v>125</v>
       </c>
-      <c r="N49" s="87"/>
-      <c r="O49" s="87"/>
-      <c r="P49" s="87"/>
-      <c r="Q49" s="85" t="s">
+      <c r="N49" s="73"/>
+      <c r="O49" s="73"/>
+      <c r="P49" s="73"/>
+      <c r="Q49" s="81" t="s">
         <v>116</v>
       </c>
-      <c r="R49" s="85"/>
-    </row>
-    <row r="50" s="88" customFormat="true" ht="15.3" hidden="false" customHeight="true" outlineLevel="1" collapsed="false">
-      <c r="A50" s="83" t="n">
+      <c r="R49" s="81"/>
+    </row>
+    <row r="50" s="16" customFormat="true" ht="15.3" hidden="false" customHeight="true" outlineLevel="1" collapsed="false">
+      <c r="A50" s="64" t="n">
         <v>44286</v>
       </c>
-      <c r="B50" s="84" t="s">
+      <c r="B50" s="36" t="s">
         <v>126</v>
       </c>
-      <c r="C50" s="84"/>
-      <c r="D50" s="84"/>
-      <c r="E50" s="84"/>
-      <c r="F50" s="84"/>
+      <c r="C50" s="36"/>
+      <c r="D50" s="36"/>
+      <c r="E50" s="36"/>
+      <c r="F50" s="36"/>
       <c r="G50" s="80" t="n">
         <v>-200</v>
       </c>
-      <c r="H50" s="85" t="s">
+      <c r="H50" s="81" t="s">
         <v>50</v>
       </c>
-      <c r="I50" s="86"/>
-      <c r="J50" s="86"/>
-      <c r="K50" s="86"/>
-      <c r="L50" s="86"/>
-      <c r="M50" s="87" t="s">
+      <c r="I50" s="82"/>
+      <c r="J50" s="82"/>
+      <c r="K50" s="82"/>
+      <c r="L50" s="82"/>
+      <c r="M50" s="73" t="s">
         <v>127</v>
       </c>
-      <c r="N50" s="87"/>
-      <c r="O50" s="87"/>
-      <c r="P50" s="87"/>
-      <c r="Q50" s="85" t="s">
+      <c r="N50" s="73"/>
+      <c r="O50" s="73"/>
+      <c r="P50" s="73"/>
+      <c r="Q50" s="81" t="s">
         <v>116</v>
       </c>
-      <c r="R50" s="85"/>
+      <c r="R50" s="81"/>
     </row>
     <row r="51" s="1" customFormat="true" ht="17.1" hidden="false" customHeight="true" outlineLevel="1" collapsed="false">
       <c r="A51" s="48"/>
@@ -3446,14 +3422,14 @@
       <c r="E51" s="48"/>
       <c r="F51" s="48"/>
       <c r="G51" s="48"/>
-      <c r="H51" s="89"/>
+      <c r="H51" s="83"/>
       <c r="I51" s="75"/>
       <c r="J51" s="75"/>
       <c r="K51" s="48"/>
       <c r="L51" s="48"/>
       <c r="M51" s="48"/>
       <c r="N51" s="48"/>
-      <c r="O51" s="90"/>
+      <c r="O51" s="84"/>
       <c r="P51" s="75"/>
       <c r="Q51" s="75"/>
       <c r="R51" s="75"/>
@@ -3465,12 +3441,12 @@
       <c r="B52" s="29"/>
       <c r="C52" s="29"/>
       <c r="D52" s="29"/>
-      <c r="E52" s="91"/>
-      <c r="F52" s="91"/>
-      <c r="G52" s="91"/>
+      <c r="E52" s="85"/>
+      <c r="F52" s="85"/>
+      <c r="G52" s="85"/>
       <c r="H52" s="55"/>
-      <c r="I52" s="92"/>
-      <c r="J52" s="93"/>
+      <c r="I52" s="86"/>
+      <c r="J52" s="87"/>
       <c r="K52" s="27"/>
       <c r="L52" s="27"/>
       <c r="M52" s="27"/>
@@ -3478,31 +3454,31 @@
       <c r="O52" s="27"/>
       <c r="P52" s="27"/>
     </row>
-    <row r="53" s="97" customFormat="true" ht="56.7" hidden="false" customHeight="true" outlineLevel="1" collapsed="false">
+    <row r="53" s="91" customFormat="true" ht="56.7" hidden="false" customHeight="true" outlineLevel="1" collapsed="false">
       <c r="A53" s="78" t="s">
         <v>129</v>
       </c>
       <c r="B53" s="78"/>
       <c r="C53" s="78"/>
-      <c r="D53" s="94" t="s">
+      <c r="D53" s="88" t="s">
         <v>130</v>
       </c>
-      <c r="E53" s="94" t="s">
+      <c r="E53" s="88" t="s">
         <v>131</v>
       </c>
-      <c r="F53" s="94" t="s">
+      <c r="F53" s="88" t="s">
         <v>132</v>
       </c>
-      <c r="G53" s="94" t="s">
+      <c r="G53" s="88" t="s">
         <v>133</v>
       </c>
-      <c r="H53" s="95" t="s">
+      <c r="H53" s="89" t="s">
         <v>134</v>
       </c>
-      <c r="I53" s="95" t="s">
+      <c r="I53" s="89" t="s">
         <v>135</v>
       </c>
-      <c r="J53" s="95" t="s">
+      <c r="J53" s="89" t="s">
         <v>136</v>
       </c>
       <c r="K53" s="78" t="s">
@@ -3514,73 +3490,73 @@
         <v>112</v>
       </c>
       <c r="O53" s="79"/>
-      <c r="P53" s="96"/>
-      <c r="Q53" s="96" t="s">
+      <c r="P53" s="90"/>
+      <c r="Q53" s="90" t="s">
         <v>138</v>
       </c>
-      <c r="R53" s="96"/>
-      <c r="S53" s="96"/>
-    </row>
-    <row r="54" s="97" customFormat="true" ht="29.7" hidden="false" customHeight="true" outlineLevel="1" collapsed="false">
-      <c r="A54" s="98" t="s">
+      <c r="R53" s="90"/>
+      <c r="S53" s="90"/>
+    </row>
+    <row r="54" s="91" customFormat="true" ht="29.7" hidden="false" customHeight="true" outlineLevel="1" collapsed="false">
+      <c r="A54" s="92" t="s">
         <v>139</v>
       </c>
-      <c r="B54" s="98"/>
-      <c r="C54" s="98"/>
-      <c r="D54" s="99" t="n">
+      <c r="B54" s="92"/>
+      <c r="C54" s="92"/>
+      <c r="D54" s="93" t="n">
         <v>44210</v>
       </c>
-      <c r="E54" s="100" t="n">
+      <c r="E54" s="94" t="n">
         <v>2600</v>
       </c>
       <c r="F54" s="67" t="n">
         <v>2.391</v>
       </c>
-      <c r="G54" s="101" t="n">
+      <c r="G54" s="95" t="n">
         <v>6216.6</v>
       </c>
-      <c r="H54" s="102" t="n">
+      <c r="H54" s="96" t="n">
         <v>6216.6</v>
       </c>
-      <c r="I54" s="103" t="s">
+      <c r="I54" s="97" t="s">
         <v>50</v>
       </c>
-      <c r="J54" s="104" t="n">
+      <c r="J54" s="98" t="n">
         <v>44223</v>
       </c>
-      <c r="K54" s="98" t="s">
+      <c r="K54" s="92" t="s">
         <v>140</v>
       </c>
-      <c r="L54" s="98"/>
-      <c r="M54" s="98"/>
+      <c r="L54" s="92"/>
+      <c r="M54" s="92"/>
       <c r="N54" s="81" t="s">
         <v>116</v>
       </c>
       <c r="O54" s="81"/>
-      <c r="P54" s="96"/>
-      <c r="Q54" s="96"/>
-      <c r="R54" s="96"/>
-      <c r="S54" s="96"/>
-    </row>
-    <row r="55" s="109" customFormat="true" ht="13.2" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
-      <c r="A55" s="105"/>
-      <c r="B55" s="105"/>
-      <c r="C55" s="105"/>
-      <c r="D55" s="106"/>
-      <c r="E55" s="105"/>
-      <c r="F55" s="106"/>
-      <c r="G55" s="106"/>
-      <c r="H55" s="106"/>
-      <c r="I55" s="107"/>
-      <c r="J55" s="106"/>
-      <c r="K55" s="105"/>
-      <c r="L55" s="105"/>
-      <c r="M55" s="105"/>
-      <c r="N55" s="108"/>
-      <c r="O55" s="108"/>
-      <c r="P55" s="96"/>
-      <c r="Q55" s="96"/>
-      <c r="R55" s="96"/>
+      <c r="P54" s="90"/>
+      <c r="Q54" s="90"/>
+      <c r="R54" s="90"/>
+      <c r="S54" s="90"/>
+    </row>
+    <row r="55" s="103" customFormat="true" ht="13.2" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
+      <c r="A55" s="99"/>
+      <c r="B55" s="99"/>
+      <c r="C55" s="99"/>
+      <c r="D55" s="100"/>
+      <c r="E55" s="99"/>
+      <c r="F55" s="100"/>
+      <c r="G55" s="100"/>
+      <c r="H55" s="100"/>
+      <c r="I55" s="101"/>
+      <c r="J55" s="100"/>
+      <c r="K55" s="99"/>
+      <c r="L55" s="99"/>
+      <c r="M55" s="99"/>
+      <c r="N55" s="102"/>
+      <c r="O55" s="102"/>
+      <c r="P55" s="90"/>
+      <c r="Q55" s="90"/>
+      <c r="R55" s="90"/>
     </row>
     <row r="56" s="15" customFormat="true" ht="17.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A56" s="29" t="s">
@@ -3600,80 +3576,80 @@
       <c r="M56" s="29"/>
       <c r="N56" s="22"/>
       <c r="O56" s="22"/>
-      <c r="P56" s="110"/>
+      <c r="P56" s="104"/>
     </row>
     <row r="57" s="15" customFormat="true" ht="43.2" hidden="false" customHeight="true" outlineLevel="1" collapsed="false">
-      <c r="A57" s="94" t="s">
+      <c r="A57" s="88" t="s">
         <v>73</v>
       </c>
-      <c r="B57" s="94"/>
-      <c r="C57" s="94"/>
-      <c r="D57" s="94" t="s">
+      <c r="B57" s="88"/>
+      <c r="C57" s="88"/>
+      <c r="D57" s="88" t="s">
         <v>142</v>
       </c>
-      <c r="E57" s="94"/>
-      <c r="F57" s="94" t="s">
+      <c r="E57" s="88"/>
+      <c r="F57" s="88" t="s">
         <v>143</v>
       </c>
-      <c r="G57" s="94"/>
-      <c r="H57" s="94" t="s">
+      <c r="G57" s="88"/>
+      <c r="H57" s="88" t="s">
         <v>144</v>
       </c>
-      <c r="I57" s="94"/>
-      <c r="J57" s="94" t="s">
+      <c r="I57" s="88"/>
+      <c r="J57" s="88" t="s">
         <v>145</v>
       </c>
-      <c r="K57" s="94"/>
-      <c r="L57" s="94" t="s">
+      <c r="K57" s="88"/>
+      <c r="L57" s="88" t="s">
         <v>146</v>
       </c>
-      <c r="M57" s="94"/>
-      <c r="N57" s="94" t="s">
+      <c r="M57" s="88"/>
+      <c r="N57" s="88" t="s">
         <v>147</v>
       </c>
-      <c r="O57" s="94"/>
+      <c r="O57" s="88"/>
       <c r="P57" s="22"/>
       <c r="Q57" s="22"/>
-      <c r="R57" s="110"/>
+      <c r="R57" s="104"/>
     </row>
     <row r="58" s="15" customFormat="true" ht="17.1" hidden="false" customHeight="true" outlineLevel="1" collapsed="false">
-      <c r="A58" s="103" t="s">
+      <c r="A58" s="97" t="s">
         <v>148</v>
       </c>
-      <c r="B58" s="103"/>
-      <c r="C58" s="103"/>
-      <c r="D58" s="103"/>
-      <c r="E58" s="103"/>
-      <c r="F58" s="103"/>
-      <c r="G58" s="103"/>
-      <c r="H58" s="111"/>
-      <c r="I58" s="111"/>
-      <c r="J58" s="103"/>
-      <c r="K58" s="103"/>
-      <c r="L58" s="103"/>
-      <c r="M58" s="103"/>
-      <c r="N58" s="103"/>
-      <c r="O58" s="103"/>
+      <c r="B58" s="97"/>
+      <c r="C58" s="97"/>
+      <c r="D58" s="97"/>
+      <c r="E58" s="97"/>
+      <c r="F58" s="97"/>
+      <c r="G58" s="97"/>
+      <c r="H58" s="105"/>
+      <c r="I58" s="105"/>
+      <c r="J58" s="97"/>
+      <c r="K58" s="97"/>
+      <c r="L58" s="97"/>
+      <c r="M58" s="97"/>
+      <c r="N58" s="97"/>
+      <c r="O58" s="97"/>
       <c r="P58" s="22"/>
       <c r="Q58" s="22"/>
-      <c r="R58" s="110"/>
+      <c r="R58" s="104"/>
     </row>
     <row r="59" s="51" customFormat="true" ht="17.1" hidden="false" customHeight="true" outlineLevel="1" collapsed="false">
-      <c r="A59" s="112"/>
-      <c r="B59" s="112"/>
-      <c r="C59" s="112"/>
-      <c r="D59" s="112"/>
-      <c r="E59" s="112"/>
-      <c r="F59" s="112"/>
-      <c r="G59" s="112"/>
-      <c r="H59" s="112"/>
-      <c r="I59" s="112"/>
-      <c r="J59" s="112"/>
-      <c r="K59" s="112"/>
-      <c r="L59" s="112"/>
+      <c r="A59" s="106"/>
+      <c r="B59" s="106"/>
+      <c r="C59" s="106"/>
+      <c r="D59" s="106"/>
+      <c r="E59" s="106"/>
+      <c r="F59" s="106"/>
+      <c r="G59" s="106"/>
+      <c r="H59" s="106"/>
+      <c r="I59" s="106"/>
+      <c r="J59" s="106"/>
+      <c r="K59" s="106"/>
+      <c r="L59" s="106"/>
       <c r="M59" s="75"/>
-      <c r="N59" s="112"/>
-      <c r="O59" s="112"/>
+      <c r="N59" s="106"/>
+      <c r="O59" s="106"/>
     </row>
     <row r="60" s="15" customFormat="true" ht="17.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A60" s="29" t="s">
@@ -3693,9 +3669,9 @@
       <c r="M60" s="29"/>
       <c r="N60" s="22"/>
       <c r="O60" s="22"/>
-      <c r="P60" s="110"/>
-    </row>
-    <row r="61" s="115" customFormat="true" ht="56.7" hidden="false" customHeight="true" outlineLevel="1" collapsed="false">
+      <c r="P60" s="104"/>
+    </row>
+    <row r="61" s="109" customFormat="true" ht="56.7" hidden="false" customHeight="true" outlineLevel="1" collapsed="false">
       <c r="A61" s="33" t="s">
         <v>150</v>
       </c>
@@ -3732,38 +3708,38 @@
         <v>158</v>
       </c>
       <c r="R61" s="30"/>
-      <c r="S61" s="113"/>
-      <c r="T61" s="113"/>
-      <c r="U61" s="113"/>
-      <c r="V61" s="113"/>
-      <c r="W61" s="114"/>
+      <c r="S61" s="107"/>
+      <c r="T61" s="107"/>
+      <c r="U61" s="107"/>
+      <c r="V61" s="107"/>
+      <c r="W61" s="108"/>
     </row>
     <row r="62" s="15" customFormat="true" ht="17.1" hidden="false" customHeight="true" outlineLevel="1" collapsed="false">
-      <c r="A62" s="116" t="s">
+      <c r="A62" s="110" t="s">
         <v>66</v>
       </c>
-      <c r="B62" s="116"/>
-      <c r="C62" s="116"/>
-      <c r="D62" s="116"/>
-      <c r="E62" s="116"/>
-      <c r="F62" s="116"/>
-      <c r="G62" s="116"/>
-      <c r="H62" s="116"/>
-      <c r="I62" s="116"/>
-      <c r="J62" s="116"/>
-      <c r="K62" s="116"/>
-      <c r="L62" s="116"/>
-      <c r="M62" s="116"/>
-      <c r="N62" s="116"/>
-      <c r="O62" s="117"/>
-      <c r="P62" s="117"/>
-      <c r="Q62" s="117"/>
-      <c r="R62" s="117"/>
+      <c r="B62" s="110"/>
+      <c r="C62" s="110"/>
+      <c r="D62" s="110"/>
+      <c r="E62" s="110"/>
+      <c r="F62" s="110"/>
+      <c r="G62" s="110"/>
+      <c r="H62" s="110"/>
+      <c r="I62" s="110"/>
+      <c r="J62" s="110"/>
+      <c r="K62" s="110"/>
+      <c r="L62" s="110"/>
+      <c r="M62" s="110"/>
+      <c r="N62" s="110"/>
+      <c r="O62" s="111"/>
+      <c r="P62" s="111"/>
+      <c r="Q62" s="111"/>
+      <c r="R62" s="111"/>
       <c r="S62" s="22"/>
       <c r="T62" s="22"/>
       <c r="U62" s="22"/>
       <c r="V62" s="22"/>
-      <c r="W62" s="110"/>
+      <c r="W62" s="104"/>
     </row>
     <row r="63" s="1" customFormat="true" ht="17.1" hidden="false" customHeight="true" outlineLevel="1" collapsed="false">
       <c r="A63" s="49"/>
@@ -3786,11 +3762,11 @@
       <c r="R63" s="75"/>
     </row>
     <row r="64" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A64" s="118"/>
-      <c r="B64" s="118"/>
-      <c r="C64" s="118"/>
-      <c r="D64" s="118"/>
-      <c r="E64" s="118"/>
+      <c r="A64" s="112"/>
+      <c r="B64" s="112"/>
+      <c r="C64" s="112"/>
+      <c r="D64" s="112"/>
+      <c r="E64" s="112"/>
       <c r="F64" s="22"/>
       <c r="G64" s="22"/>
       <c r="H64" s="22"/>
@@ -3801,11 +3777,11 @@
       <c r="M64" s="22"/>
     </row>
     <row r="65" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A65" s="119"/>
-      <c r="B65" s="118"/>
-      <c r="C65" s="118"/>
-      <c r="D65" s="118"/>
-      <c r="E65" s="118"/>
+      <c r="A65" s="113"/>
+      <c r="B65" s="112"/>
+      <c r="C65" s="112"/>
+      <c r="D65" s="112"/>
+      <c r="E65" s="112"/>
       <c r="F65" s="22"/>
       <c r="G65" s="22"/>
       <c r="H65" s="22"/>
@@ -3816,15 +3792,15 @@
       <c r="M65" s="22"/>
     </row>
     <row r="66" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A66" s="120" t="s">
+      <c r="A66" s="114" t="s">
         <v>159</v>
       </c>
-      <c r="B66" s="120"/>
-      <c r="C66" s="120"/>
-      <c r="D66" s="120"/>
-      <c r="E66" s="120"/>
-      <c r="F66" s="120"/>
-      <c r="G66" s="120"/>
+      <c r="B66" s="114"/>
+      <c r="C66" s="114"/>
+      <c r="D66" s="114"/>
+      <c r="E66" s="114"/>
+      <c r="F66" s="114"/>
+      <c r="G66" s="114"/>
       <c r="H66" s="22"/>
       <c r="I66" s="22"/>
       <c r="J66" s="22"/>
@@ -3833,11 +3809,11 @@
       <c r="M66" s="22"/>
     </row>
     <row r="67" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A67" s="121" t="s">
+      <c r="A67" s="115" t="s">
         <v>160</v>
       </c>
-      <c r="B67" s="121"/>
-      <c r="C67" s="121"/>
+      <c r="B67" s="115"/>
+      <c r="C67" s="115"/>
       <c r="D67" s="14" t="s">
         <v>161</v>
       </c>
@@ -4209,136 +4185,136 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="122" t="s">
+      <c r="A1" s="116" t="s">
         <v>162</v>
       </c>
-      <c r="V1" s="123" t="s">
+      <c r="V1" s="117" t="s">
         <v>163</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="V2" s="123" t="s">
+      <c r="V2" s="117" t="s">
         <v>164</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="V3" s="123" t="s">
+      <c r="V3" s="117" t="s">
         <v>165</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="V4" s="123" t="s">
+      <c r="V4" s="117" t="s">
         <v>166</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="V5" s="123" t="s">
+      <c r="V5" s="117" t="s">
         <v>167</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="V6" s="123" t="s">
+      <c r="V6" s="117" t="s">
         <v>168</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="V7" s="123" t="s">
+      <c r="V7" s="117" t="s">
         <v>169</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="V8" s="123" t="s">
+      <c r="V8" s="117" t="s">
         <v>170</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="V9" s="123" t="s">
+      <c r="V9" s="117" t="s">
         <v>171</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="V10" s="123" t="s">
+      <c r="V10" s="117" t="s">
         <v>172</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="V11" s="123" t="s">
+      <c r="V11" s="117" t="s">
         <v>173</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="V12" s="123" t="s">
+      <c r="V12" s="117" t="s">
         <v>174</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="V13" s="123" t="s">
+      <c r="V13" s="117" t="s">
         <v>175</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="V14" s="123" t="s">
+      <c r="V14" s="117" t="s">
         <v>176</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="V15" s="123" t="s">
+      <c r="V15" s="117" t="s">
         <v>177</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="V16" s="123" t="s">
+      <c r="V16" s="117" t="s">
         <v>178</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="V17" s="123" t="s">
+      <c r="V17" s="117" t="s">
         <v>179</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="V18" s="123" t="s">
+      <c r="V18" s="117" t="s">
         <v>180</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="123"/>
+      <c r="A20" s="117"/>
     </row>
     <row r="21" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="123"/>
+      <c r="A21" s="117"/>
     </row>
     <row r="22" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="123"/>
+      <c r="A22" s="117"/>
     </row>
     <row r="23" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="123"/>
+      <c r="A23" s="117"/>
     </row>
     <row r="24" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="123"/>
+      <c r="A24" s="117"/>
     </row>
     <row r="25" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="123"/>
+      <c r="A25" s="117"/>
     </row>
     <row r="26" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="123"/>
+      <c r="A26" s="117"/>
     </row>
     <row r="27" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="123"/>
+      <c r="A27" s="117"/>
     </row>
     <row r="28" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="123"/>
+      <c r="A28" s="117"/>
     </row>
     <row r="29" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="123"/>
+      <c r="A29" s="117"/>
     </row>
     <row r="30" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="123"/>
+      <c r="A30" s="117"/>
     </row>
     <row r="31" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="123"/>
+      <c r="A31" s="117"/>
     </row>
     <row r="32" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="123"/>
+      <c r="A32" s="117"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>